<commit_message>
Updated options descriptions file.
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24321"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plopez\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plopez\PycharmProjects\btap_batch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="11_53698E743833A7DBB6B553360D97D2D32F5A08B7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{130863AB-6931-40F0-A133-86CE8C6DD780}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="14730" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BTAPOptions" sheetId="1" r:id="rId1"/>
+    <sheet name="ReadME" sheetId="2" r:id="rId1"/>
+    <sheet name="BTAPOptions" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="287">
   <si>
     <t>Variable</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>:epw _file</t>
-  </si>
-  <si>
-    <t>Set the geographic location and climate database to use for the simulation. The available Canadian locations are available in the hyperlink prefixed by CAN with the epw extention</t>
   </si>
   <si>
     <t>CAN_QC_Montreal-Trudeau.Intl.AP.716270_CWEC2016.epw</t>
@@ -895,13 +892,19 @@
   </si>
   <si>
     <t>Will scale the outdoor air requirements for the entire building</t>
+  </si>
+  <si>
+    <t>BTAPOptions contains the token field allowed in the YAML analysis input files.  Please see the examples folder and the *.yml files for examples of applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set the geographic location and climate database to use for the simulation. The available Canadian locations are available in the hyperlink. BTAP supports only the CAN_* files but the american files may work as well. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1956,15 +1959,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" style="2" customWidth="1"/>
@@ -1976,7 +1999,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1999,7 +2022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="2" spans="1:7" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2012,7 +2035,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2026,7 +2049,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2040,7 +2063,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2054,7 +2077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2071,7 +2094,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>22</v>
@@ -2089,7 +2112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="8" spans="1:7" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -2102,7 +2125,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
@@ -2117,7 +2140,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2132,7 +2155,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
@@ -2147,7 +2170,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
@@ -2162,7 +2185,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2177,7 +2200,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
@@ -2192,7 +2215,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2207,7 +2230,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
@@ -2222,7 +2245,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
@@ -2237,7 +2260,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
@@ -2252,7 +2275,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>48</v>
       </c>
@@ -2267,7 +2290,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>50</v>
       </c>
@@ -2282,7 +2305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>52</v>
       </c>
@@ -2297,7 +2320,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>54</v>
       </c>
@@ -2312,7 +2335,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>56</v>
       </c>
@@ -2327,7 +2350,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>58</v>
       </c>
@@ -2342,7 +2365,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>60</v>
       </c>
@@ -2357,12 +2380,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" ht="63" customHeight="1">
+    <row r="26" spans="1:7" s="7" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>63</v>
+        <v>286</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -2370,117 +2393,117 @@
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="C28" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F33" s="20"/>
       <c r="G33" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="7" customFormat="1" ht="30">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
@@ -2488,63 +2511,63 @@
       <c r="F34" s="21"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" ht="30">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G35" s="3" t="s">
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="30">
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30">
-      <c r="C37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="7" customFormat="1">
-      <c r="A38" s="5" t="s">
+      <c r="B38" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
@@ -2552,68 +2575,68 @@
       <c r="F38" s="6"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="3" t="s">
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="30">
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="30">
-      <c r="A43" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="16"/>
@@ -2621,36 +2644,36 @@
       <c r="F43" s="16"/>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="F44" s="20"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="20"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="20"/>
+    </row>
+    <row r="46" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E45" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F45" s="20"/>
-    </row>
-    <row r="46" spans="1:7" s="7" customFormat="1">
-      <c r="A46" s="5" t="s">
+      <c r="B46" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
@@ -2658,41 +2681,41 @@
       <c r="F46" s="6"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E47" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="20" t="s">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E48" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" s="7" customFormat="1" ht="30">
-      <c r="A49" s="5" t="s">
+      <c r="B49" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="6"/>
@@ -2700,41 +2723,41 @@
       <c r="F49" s="6"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="20"/>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C51" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E50" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="20"/>
-    </row>
-    <row r="51" spans="1:7" ht="30">
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="E51" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="20" t="s">
+      <c r="G51" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G51" s="3" t="s">
+    </row>
+    <row r="52" spans="1:7" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" s="7" customFormat="1" ht="30">
-      <c r="A52" s="5" t="s">
+      <c r="B52" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>115</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="6"/>
@@ -2742,82 +2765,82 @@
       <c r="F52" s="6"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" ht="30">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E53" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="20" t="s">
+    </row>
+    <row r="54" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="C54" s="29" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="120">
-      <c r="C54" s="29" t="s">
+      <c r="D54" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="E54" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="E54" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" s="20" t="s">
+    </row>
+    <row r="55" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="C55" s="28" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="150">
-      <c r="C55" s="28" t="s">
+      <c r="D55" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="27" t="s">
+      <c r="E55" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="E55" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="20" t="s">
+    </row>
+    <row r="56" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="C56" s="31" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="120">
-      <c r="C56" s="31" t="s">
+      <c r="D56" s="30" t="s">
         <v>124</v>
-      </c>
-      <c r="D56" s="30" t="s">
-        <v>125</v>
       </c>
       <c r="E56" s="11" t="b">
         <v>0</v>
       </c>
       <c r="F56" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="C57" s="28" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="90">
-      <c r="C57" s="28" t="s">
+      <c r="D57" s="27" t="s">
         <v>127</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>128</v>
       </c>
       <c r="E57" s="11" t="b">
         <v>0</v>
       </c>
       <c r="F57" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="5" t="s">
+      <c r="B58" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
@@ -2825,52 +2848,52 @@
       <c r="F58" s="6"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="20"/>
+    </row>
+    <row r="60" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="C60" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E59" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="20"/>
-    </row>
-    <row r="60" spans="1:7" ht="75">
-      <c r="C60" s="7" t="s">
+      <c r="D60" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="E60" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E60" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="20" t="s">
+    </row>
+    <row r="61" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="C61" s="7" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="120">
-      <c r="C61" s="7" t="s">
+      <c r="D61" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="E61" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="E61" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="20" t="s">
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="30">
-      <c r="A62" s="6" t="s">
+      <c r="B62" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="6"/>
@@ -2878,85 +2901,85 @@
       <c r="F62" s="6"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:7" ht="30">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E63" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C64" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E63" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="30">
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="20"/>
+    </row>
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E64" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="20"/>
-    </row>
-    <row r="65" spans="1:7" ht="60">
-      <c r="C65" s="1" t="s">
+      <c r="D65" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="E65" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="20" t="s">
+    </row>
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="30">
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="20"/>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E66" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="20"/>
-    </row>
-    <row r="67" spans="1:7" ht="30">
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="20"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E67" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="20"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="E68" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="20"/>
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E68" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" s="20"/>
-    </row>
-    <row r="69" spans="1:7" ht="30">
-      <c r="A69" s="5" t="s">
+      <c r="B69" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>154</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="6"/>
@@ -2964,54 +2987,54 @@
       <c r="F69" s="6"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D70" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E70" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="E70" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="20" t="s">
+    </row>
+    <row r="71" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="60">
-      <c r="C71" s="1" t="s">
+      <c r="D71" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="E71" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="20" t="s">
+    </row>
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="45">
-      <c r="C72" s="1" t="s">
+      <c r="D72" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="E72" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="20" t="s">
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="5" t="s">
+      <c r="B73" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="6"/>
@@ -3019,40 +3042,40 @@
       <c r="F73" s="6"/>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="1:7" ht="75">
+    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C74" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D74" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E74" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E74" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="20" t="s">
+    </row>
+    <row r="75" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="120">
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="E75" s="11" t="b">
         <v>0</v>
       </c>
       <c r="F75" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="30">
-      <c r="A76" s="5" t="s">
+      <c r="B76" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>171</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
@@ -3060,89 +3083,89 @@
       <c r="F76" s="6"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="1:7" ht="75">
+    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C77" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D77" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E77" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E77" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="20" t="s">
+      <c r="G77" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>0.314</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E78" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F78" s="20"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>0.27800000000000002</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E79" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F79" s="20"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>0.247</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E80" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F80" s="20"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>0.21</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E81" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F81" s="20"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>0.183</v>
       </c>
       <c r="D82" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E82" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="20"/>
+    </row>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E82" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="20"/>
-    </row>
-    <row r="83" spans="1:7" ht="30">
-      <c r="A83" s="5" t="s">
+      <c r="B83" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>177</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="6"/>
@@ -3150,77 +3173,77 @@
       <c r="F83" s="6"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="1:7" ht="75">
+    <row r="84" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C84" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D84" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E84" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E84" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G84" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>0.22700000000000001</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E85" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F85" s="20"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>0.183</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E86" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F86" s="20"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>0.16200000000000001</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E87" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F87" s="20"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>0.14199999999999999</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E88" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F88" s="20"/>
     </row>
-    <row r="89" spans="1:7" ht="30">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="6"/>
@@ -3228,113 +3251,113 @@
       <c r="F89" s="6"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="1:7" ht="75">
+    <row r="90" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C90" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D90" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E90" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E90" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G90" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>0.22700000000000001</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E91" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F91" s="20"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <v>0.193</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E92" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F92" s="20"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <v>0.183</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E93" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F93" s="20"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <v>0.16200000000000001</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E94" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F94" s="20"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <v>0.14199999999999999</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E95" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F95" s="20"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <v>0.13800000000000001</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E96" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F96" s="20"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C97" s="1">
         <v>0.121</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E97" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F97" s="20"/>
     </row>
-    <row r="98" spans="1:7" ht="30">
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="6"/>
@@ -3342,77 +3365,77 @@
       <c r="F98" s="6"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="1:7" ht="75">
+    <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D99" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E99" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E99" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G99" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
         <v>0.56799999999999995</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E100" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F100" s="20"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
         <v>0.379</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E101" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F101" s="20"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C102" s="1">
         <v>0.28399999999999997</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E102" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F102" s="20"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C103" s="1">
         <v>0.21</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E103" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F103" s="20"/>
     </row>
-    <row r="104" spans="1:7" ht="30">
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="6"/>
@@ -3420,59 +3443,59 @@
       <c r="F104" s="6"/>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="1:7" ht="75">
+    <row r="105" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C105" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D105" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E105" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E105" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G105" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C106" s="1">
         <v>0.75800000000000001</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E106" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F106" s="20"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C107" s="1">
         <v>0.379</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E107" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F107" s="20"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E108" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F108" s="20"/>
     </row>
-    <row r="109" spans="1:7" ht="30">
+    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B109" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>186</v>
       </c>
       <c r="C109" s="5"/>
       <c r="D109" s="6"/>
@@ -3480,77 +3503,77 @@
       <c r="F109" s="6"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="1:7" ht="75">
+    <row r="110" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C110" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D110" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E110" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E110" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G110" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C111" s="1">
         <v>0.56799999999999995</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E111" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F111" s="20"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C112" s="4">
         <v>0.379</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E112" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F112" s="20"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C113" s="1">
         <v>0.28399999999999997</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E113" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F113" s="20"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C114" s="1">
         <v>0.21</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E114" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F114" s="20"/>
     </row>
-    <row r="115" spans="1:7" ht="30">
+    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B115" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="C115" s="5"/>
       <c r="D115" s="6"/>
@@ -3558,130 +3581,130 @@
       <c r="F115" s="6"/>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="1:7" ht="75">
+    <row r="116" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C116" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D116" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E116" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E116" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G116" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C117" s="1">
         <v>2.4</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E117" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F117" s="20"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C118" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E118" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F118" s="20"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C119" s="1">
         <v>1.6</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E119" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F119" s="20"/>
     </row>
-    <row r="120" spans="1:7" ht="30">
+    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B120" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="C120" s="5"/>
       <c r="D120" s="16"/>
       <c r="E120" s="18"/>
       <c r="F120" s="22"/>
     </row>
-    <row r="121" spans="1:7" ht="75">
+    <row r="121" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C121" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D121" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E121" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E121" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F121" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G121" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C122" s="1">
         <v>2.4</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E122" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F122" s="20"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C123" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E123" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F123" s="20"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C124" s="1">
         <v>1.6</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E124" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F124" s="20"/>
     </row>
-    <row r="125" spans="1:7" ht="30">
+    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B125" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="C125" s="5"/>
       <c r="D125" s="6"/>
@@ -3689,65 +3712,65 @@
       <c r="F125" s="6"/>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="1:7" ht="75">
+    <row r="126" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C126" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D126" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E126" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F126" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E126" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F126" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G126" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C127" s="1">
         <v>2.4</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E127" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F127" s="20"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C128" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E128" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F128" s="20"/>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C129" s="1">
         <v>1.6</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E129" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F129" s="20"/>
     </row>
-    <row r="130" spans="1:7" ht="30">
+    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B130" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="B130" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="C130" s="5"/>
       <c r="D130" s="16"/>
@@ -3755,65 +3778,65 @@
       <c r="F130" s="22"/>
       <c r="G130" s="17"/>
     </row>
-    <row r="131" spans="1:7" ht="75">
+    <row r="131" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C131" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D131" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E131" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F131" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E131" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F131" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G131" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C132" s="1">
         <v>2.4</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E132" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F132" s="20"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C133" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E133" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F133" s="20"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C134" s="1">
         <v>1.6</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E134" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F134" s="20"/>
     </row>
-    <row r="135" spans="1:7" ht="30">
+    <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B135" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="C135" s="5"/>
       <c r="D135" s="6"/>
@@ -3821,24 +3844,24 @@
       <c r="F135" s="22"/>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="1:7" ht="75">
+    <row r="136" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C136" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D136" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E136" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F136" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E136" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F136" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G136" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C137" s="1">
         <v>0.05</v>
       </c>
@@ -3847,24 +3870,24 @@
       </c>
       <c r="F137" s="20"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C138" s="1">
         <v>0.9</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E138" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F138" s="20"/>
     </row>
-    <row r="139" spans="1:7" ht="30">
+    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B139" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="B139" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="C139" s="5"/>
       <c r="D139" s="6"/>
@@ -3872,53 +3895,53 @@
       <c r="F139" s="23"/>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="1:7" ht="75">
+    <row r="140" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C140" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D140" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E140" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F140" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E140" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F140" s="20" t="s">
-        <v>173</v>
-      </c>
       <c r="G140" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C141" s="1">
         <v>0.05</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E141" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F141" s="20"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C142" s="1">
         <v>0.9</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E142" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F142" s="20"/>
     </row>
-    <row r="143" spans="1:7" ht="30">
+    <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B143" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="B143" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="C143" s="5"/>
       <c r="D143" s="6"/>
@@ -3926,21 +3949,21 @@
       <c r="F143" s="23"/>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="1:7" ht="75">
+    <row r="144" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C144" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E144" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F144" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G144" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C145" s="1">
         <v>0.05</v>
       </c>
@@ -3949,7 +3972,7 @@
       </c>
       <c r="F145" s="20"/>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C146" s="1">
         <v>0.9</v>
       </c>
@@ -3958,12 +3981,12 @@
       </c>
       <c r="F146" s="20"/>
     </row>
-    <row r="147" spans="1:7" ht="45">
+    <row r="147" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B147" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="B147" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="C147" s="5"/>
       <c r="D147" s="6"/>
@@ -3971,84 +3994,84 @@
       <c r="F147" s="23"/>
       <c r="G147" s="5"/>
     </row>
-    <row r="148" spans="1:7" ht="165">
+    <row r="148" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="C148" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D148" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E148" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F148" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="E148" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F148" s="26" t="s">
+      <c r="G148" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G148" s="1" t="s">
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C149" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D149" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="149" spans="1:7">
-      <c r="C149" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D149" s="2" t="s">
+      <c r="E149" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F149" s="20"/>
+    </row>
+    <row r="150" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E149" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F149" s="20"/>
-    </row>
-    <row r="150" spans="1:7" ht="45">
-      <c r="A150" s="5" t="s">
+      <c r="B150" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B150" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="C150" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E150" s="19"/>
       <c r="F150" s="23"/>
       <c r="G150" s="5"/>
     </row>
-    <row r="151" spans="1:7" ht="150">
+    <row r="151" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="C151" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E151" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F151" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C152" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E152" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F152" s="20"/>
+    </row>
+    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="G151" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7">
-      <c r="C152" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E152" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F152" s="20"/>
-    </row>
-    <row r="153" spans="1:7" ht="30">
-      <c r="A153" s="5" t="s">
+      <c r="B153" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="C153" s="5"/>
       <c r="D153" s="6"/>
@@ -4056,36 +4079,36 @@
       <c r="F153" s="23"/>
       <c r="G153" s="5"/>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C154" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E154" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F154" s="20"/>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C155" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E155" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F155" s="20"/>
     </row>
-    <row r="156" spans="1:7" ht="45">
+    <row r="156" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B156" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="6"/>
@@ -4093,24 +4116,24 @@
       <c r="F156" s="23"/>
       <c r="G156" s="5"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C157" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E157" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F157" s="20"/>
     </row>
-    <row r="158" spans="1:7" ht="45">
+    <row r="158" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B158" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="C158" s="5"/>
       <c r="D158" s="6"/>
@@ -4118,24 +4141,24 @@
       <c r="F158" s="23"/>
       <c r="G158" s="5"/>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E159" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F159" s="20"/>
     </row>
-    <row r="160" spans="1:7" ht="45">
+    <row r="160" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B160" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="C160" s="5"/>
       <c r="D160" s="6"/>
@@ -4143,24 +4166,24 @@
       <c r="F160" s="23"/>
       <c r="G160" s="5"/>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C161" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E161" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F161" s="20"/>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B162" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="B162" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="C162" s="5"/>
       <c r="D162" s="6"/>
@@ -4168,49 +4191,49 @@
       <c r="F162" s="23"/>
       <c r="G162" s="5"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C163" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D163" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E163" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F163" s="20"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C164" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E163" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F163" s="20"/>
-    </row>
-    <row r="164" spans="1:7">
-      <c r="C164" s="1" t="s">
+      <c r="D164" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D164" s="2" t="s">
+      <c r="E164" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F164" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G164" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E164" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F164" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G164" s="3" t="s">
+    </row>
+    <row r="165" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" s="5" customFormat="1">
-      <c r="A165" s="5" t="s">
+      <c r="B165" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B165" s="5" t="s">
+    </row>
+    <row r="166" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C166" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D166" s="2" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" ht="30">
-      <c r="C166" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D166" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="E166" s="11" t="s">
         <v>29</v>
@@ -4218,29 +4241,29 @@
       <c r="F166" s="25"/>
       <c r="G166" s="3"/>
     </row>
-    <row r="167" spans="1:7" ht="50.25" customHeight="1">
+    <row r="167" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C167" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E167" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F167" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B168" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>233</v>
       </c>
       <c r="C168" s="5"/>
       <c r="D168" s="6"/>
@@ -4248,41 +4271,41 @@
       <c r="F168" s="23"/>
       <c r="G168" s="5"/>
     </row>
-    <row r="169" spans="1:7" ht="30">
+    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C169" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D169" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E169" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F169" s="20"/>
+    </row>
+    <row r="170" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C170" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D170" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E169" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F169" s="20"/>
-    </row>
-    <row r="170" spans="1:7" ht="45">
-      <c r="C170" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D170" s="2" t="s">
+      <c r="E170" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F170" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="E170" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F170" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G170" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7">
-      <c r="A171" s="5" t="s">
+      <c r="B171" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="B171" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="C171" s="5"/>
       <c r="D171" s="6"/>
@@ -4290,41 +4313,41 @@
       <c r="F171" s="23"/>
       <c r="G171" s="5"/>
     </row>
-    <row r="172" spans="1:7" ht="30">
+    <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C172" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E172" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F172" s="20"/>
     </row>
-    <row r="173" spans="1:7" ht="33.75" customHeight="1">
+    <row r="173" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C173" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E173" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F173" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B174" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="B174" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="C174" s="5"/>
       <c r="D174" s="6"/>
@@ -4332,80 +4355,80 @@
       <c r="F174" s="23"/>
       <c r="G174" s="5"/>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C175" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D175" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="E175" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F175" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C176" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E175" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F175" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G175" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7">
-      <c r="C176" s="1" t="s">
+      <c r="D176" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="D176" s="13" t="s">
+      <c r="E176" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F176" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C177" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E176" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F176" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G176" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7">
-      <c r="C177" s="1" t="s">
+      <c r="D177" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="D177" s="13" t="s">
+      <c r="E177" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F177" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C178" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E177" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F177" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G177" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7">
-      <c r="C178" s="1" t="s">
+      <c r="D178" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="D178" s="13" t="s">
+      <c r="E178" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F178" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="E178" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F178" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G178" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7">
-      <c r="A179" s="5" t="s">
+      <c r="B179" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="B179" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="C179" s="5"/>
       <c r="D179" s="6"/>
@@ -4413,42 +4436,42 @@
       <c r="F179" s="23"/>
       <c r="G179" s="5"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C180" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D180" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E180" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F180" s="20"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C181" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E180" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F180" s="20"/>
-    </row>
-    <row r="181" spans="1:7">
-      <c r="C181" s="1" t="s">
+      <c r="D181" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D181" s="2" t="s">
+      <c r="E181" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F181" s="20"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E182" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F182" s="20"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E181" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F181" s="20"/>
-    </row>
-    <row r="182" spans="1:7">
-      <c r="E182" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F182" s="20"/>
-    </row>
-    <row r="183" spans="1:7">
-      <c r="A183" s="5" t="s">
+      <c r="B183" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="B183" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="C183" s="5"/>
       <c r="D183" s="6"/>
@@ -4456,41 +4479,41 @@
       <c r="F183" s="23"/>
       <c r="G183" s="5"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C184" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D184" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E184" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F184" s="20"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C185" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E184" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F184" s="20"/>
-    </row>
-    <row r="185" spans="1:7">
-      <c r="C185" s="1" t="s">
+      <c r="D185" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D185" s="2" t="s">
+      <c r="E185" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F185" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G185" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="E185" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F185" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G185" s="3" t="s">
+    </row>
+    <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" ht="30">
-      <c r="A186" s="5" t="s">
+      <c r="B186" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="B186" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="C186" s="5"/>
       <c r="D186" s="6"/>
@@ -4498,41 +4521,41 @@
       <c r="F186" s="23"/>
       <c r="G186" s="5"/>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C187" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E187" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F187" s="20"/>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C188" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E188" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F188" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" ht="60">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B189" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="C189" s="5"/>
       <c r="D189" s="6"/>
@@ -4540,49 +4563,49 @@
       <c r="F189" s="23"/>
       <c r="G189" s="5"/>
     </row>
-    <row r="190" spans="1:7" ht="30">
+    <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C190" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E190" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F190" s="20"/>
     </row>
-    <row r="191" spans="1:7" ht="45">
+    <row r="191" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C191" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E191" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F191" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" s="5" customFormat="1" ht="60">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B192" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B192" s="6" t="s">
+    </row>
+    <row r="193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C193" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D193" s="2" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" ht="30">
-      <c r="C193" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D193" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="E193" s="11" t="s">
         <v>29</v>
@@ -4590,29 +4613,29 @@
       <c r="F193" s="25"/>
       <c r="G193" s="3"/>
     </row>
-    <row r="194" spans="1:7" ht="45.75" customHeight="1">
+    <row r="194" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C194" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E194" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F194" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" ht="30">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B195" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="B195" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="C195" s="5"/>
       <c r="D195" s="6"/>
@@ -4620,36 +4643,36 @@
       <c r="F195" s="23"/>
       <c r="G195" s="5"/>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C196" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E196" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F196" s="20"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C197" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D197" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E197" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F197" s="20"/>
     </row>
-    <row r="198" spans="1:7" ht="30">
+    <row r="198" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B198" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="C198" s="5"/>
       <c r="D198" s="6"/>
@@ -4657,40 +4680,40 @@
       <c r="F198" s="23"/>
       <c r="G198" s="5"/>
     </row>
-    <row r="199" spans="1:7" ht="30">
+    <row r="199" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C199" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E199" s="11" t="b">
         <v>0</v>
       </c>
       <c r="F199" s="20" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" ht="30">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C200" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D200" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E200" s="11" t="b">
         <v>0</v>
       </c>
       <c r="F200" s="20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" ht="30">
-      <c r="A201" s="5" t="s">
+      <c r="B201" s="6" t="s">
         <v>278</v>
-      </c>
-      <c r="B201" s="6" t="s">
-        <v>279</v>
       </c>
       <c r="C201" s="5"/>
       <c r="D201" s="6"/>
@@ -4698,36 +4721,36 @@
       <c r="F201" s="23"/>
       <c r="G201" s="5"/>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C202" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E202" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F202" s="20"/>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C203" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D203" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E203" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F203" s="20"/>
     </row>
-    <row r="204" spans="1:7" ht="30">
+    <row r="204" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B204" s="6" t="s">
         <v>280</v>
-      </c>
-      <c r="B204" s="6" t="s">
-        <v>281</v>
       </c>
       <c r="C204" s="5"/>
       <c r="D204" s="6"/>
@@ -4735,36 +4758,36 @@
       <c r="F204" s="23"/>
       <c r="G204" s="5"/>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C205" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E205" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F205" s="20"/>
     </row>
-    <row r="206" spans="1:7" ht="45">
+    <row r="206" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C206" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D206" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="D206" s="2" t="s">
+      <c r="E206" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F206" s="20"/>
+    </row>
+    <row r="207" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="E206" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F206" s="20"/>
-    </row>
-    <row r="207" spans="1:7" ht="30">
-      <c r="A207" s="5" t="s">
+      <c r="B207" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B207" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="C207" s="5"/>
       <c r="D207" s="16"/>
@@ -4772,24 +4795,24 @@
       <c r="F207" s="23"/>
       <c r="G207" s="17"/>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C208" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E208" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F208" s="20"/>
     </row>
-    <row r="209" spans="3:6">
+    <row r="209" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C209" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D209" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D209" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E209" s="11" t="s">
         <v>29</v>
@@ -5007,61 +5030,61 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G22" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G23" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G21" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G27" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G28:G33" r:id="rId18" display="https://github.com/NREL/openstudio-standards/tree/nrcan/data/weather" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G18" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G4" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G5" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G6" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G7" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G35" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G36" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G37" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G39" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G40:G42" r:id="rId28" display="https://github.com/NREL/openstudio-standards/blob/nrcan/lib/openstudio-standards/standards/necb/NECB2011/demand_controlled_ventilation.md" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G48" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G51" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G77" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G84" r:id="rId32" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G90" r:id="rId33" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="G99" r:id="rId34" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="G105" r:id="rId35" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="G110" r:id="rId36" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="G116" r:id="rId37" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="G121" r:id="rId38" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="G126" r:id="rId39" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="G131" r:id="rId40" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="G136" r:id="rId41" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="G140" r:id="rId42" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="G144" r:id="rId43" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="G164" r:id="rId44" xr:uid="{DAEE4E42-6022-4DDA-A017-AB6CD8C9C890}"/>
-    <hyperlink ref="G170" r:id="rId45" xr:uid="{929F7977-2001-4D3D-839F-5E24317C9333}"/>
-    <hyperlink ref="G173" r:id="rId46" xr:uid="{77D7C4AF-DAA3-42C6-B21E-C5EBE1A6DEA3}"/>
-    <hyperlink ref="G175" r:id="rId47" xr:uid="{B0A0CB60-0CA6-4922-8E1D-5D7B89B014DB}"/>
-    <hyperlink ref="G176" r:id="rId48" xr:uid="{9863D9A4-13DC-4DFE-98B7-DBA7D0F0A582}"/>
-    <hyperlink ref="G177" r:id="rId49" xr:uid="{394155DC-F807-4A32-BCC3-BF1D4F3F0640}"/>
-    <hyperlink ref="G178" r:id="rId50" xr:uid="{6E41286C-D904-4F59-8B10-1344355E8B20}"/>
-    <hyperlink ref="G167" r:id="rId51" xr:uid="{8829EDE6-C64A-4B1D-AD54-18AC4AC3D108}"/>
-    <hyperlink ref="G185" r:id="rId52" xr:uid="{3586365E-6C49-4AF1-A2FA-270FACD4A5F5}"/>
-    <hyperlink ref="G188" r:id="rId53" xr:uid="{04149A8A-83F8-42AB-A059-071227DCFAC7}"/>
-    <hyperlink ref="G191" r:id="rId54" xr:uid="{C1215442-E522-4307-9EAA-4AE7AFC3F978}"/>
-    <hyperlink ref="G194" r:id="rId55" xr:uid="{4B8889AF-13FE-4495-BB41-A62FAFC95838}"/>
+    <hyperlink ref="G9" r:id="rId1"/>
+    <hyperlink ref="G22" r:id="rId2"/>
+    <hyperlink ref="G24" r:id="rId3"/>
+    <hyperlink ref="G15" r:id="rId4"/>
+    <hyperlink ref="G13" r:id="rId5"/>
+    <hyperlink ref="G23" r:id="rId6"/>
+    <hyperlink ref="G12" r:id="rId7"/>
+    <hyperlink ref="G21" r:id="rId8"/>
+    <hyperlink ref="G25" r:id="rId9"/>
+    <hyperlink ref="G10" r:id="rId10"/>
+    <hyperlink ref="G11" r:id="rId11"/>
+    <hyperlink ref="G14" r:id="rId12"/>
+    <hyperlink ref="G16" r:id="rId13"/>
+    <hyperlink ref="G17" r:id="rId14"/>
+    <hyperlink ref="G19" r:id="rId15"/>
+    <hyperlink ref="G20" r:id="rId16"/>
+    <hyperlink ref="G27" r:id="rId17"/>
+    <hyperlink ref="G28:G33" r:id="rId18" display="https://github.com/NREL/openstudio-standards/tree/nrcan/data/weather"/>
+    <hyperlink ref="G18" r:id="rId19"/>
+    <hyperlink ref="G4" r:id="rId20"/>
+    <hyperlink ref="G5" r:id="rId21"/>
+    <hyperlink ref="G6" r:id="rId22"/>
+    <hyperlink ref="G7" r:id="rId23"/>
+    <hyperlink ref="G35" r:id="rId24"/>
+    <hyperlink ref="G36" r:id="rId25"/>
+    <hyperlink ref="G37" r:id="rId26"/>
+    <hyperlink ref="G39" r:id="rId27"/>
+    <hyperlink ref="G40:G42" r:id="rId28" display="https://github.com/NREL/openstudio-standards/blob/nrcan/lib/openstudio-standards/standards/necb/NECB2011/demand_controlled_ventilation.md"/>
+    <hyperlink ref="G48" r:id="rId29"/>
+    <hyperlink ref="G51" r:id="rId30"/>
+    <hyperlink ref="G77" r:id="rId31"/>
+    <hyperlink ref="G84" r:id="rId32" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G90" r:id="rId33" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G99" r:id="rId34" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G105" r:id="rId35" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G110" r:id="rId36" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G116" r:id="rId37" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G121" r:id="rId38" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G126" r:id="rId39" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G131" r:id="rId40" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G136" r:id="rId41" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G140" r:id="rId42" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G144" r:id="rId43" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
+    <hyperlink ref="G164" r:id="rId44"/>
+    <hyperlink ref="G170" r:id="rId45"/>
+    <hyperlink ref="G173" r:id="rId46"/>
+    <hyperlink ref="G175" r:id="rId47"/>
+    <hyperlink ref="G176" r:id="rId48"/>
+    <hyperlink ref="G177" r:id="rId49"/>
+    <hyperlink ref="G178" r:id="rId50"/>
+    <hyperlink ref="G167" r:id="rId51"/>
+    <hyperlink ref="G185" r:id="rId52"/>
+    <hyperlink ref="G188" r:id="rId53"/>
+    <hyperlink ref="G191" r:id="rId54"/>
+    <hyperlink ref="G194" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId56"/>

</xml_diff>

<commit_message>
added a new column called requires debugging to BTAPOptions.xlsx to identify the ECMs need further investigation
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plopez\PycharmProjects\btap_batch\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgilani\Dropbox\NRCan\BTAP\ECM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="14730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ReadME" sheetId="2" r:id="rId1"/>
     <sheet name="BTAPOptions" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BTAPOptions!$A$1:$H$209</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="291">
   <si>
     <t>Variable</t>
   </si>
@@ -898,6 +901,18 @@
   </si>
   <si>
     <t xml:space="preserve">Set the geographic location and climate database to use for the simulation. The available Canadian locations are available in the hyperlink. BTAP supports only the CAN_* files but the american files may work as well. </t>
+  </si>
+  <si>
+    <t>requires debugging</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Not verified</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1128,67 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="63">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1980,26 +2055,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G209"/>
+  <dimension ref="A1:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="44.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2021,8 +2097,11 @@
       <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="H1" s="15" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2034,8 +2113,11 @@
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2049,7 +2131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2063,7 +2145,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2077,7 +2159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2094,7 +2176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>22</v>
@@ -2112,7 +2194,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -2124,8 +2206,11 @@
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
       <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
@@ -2140,7 +2225,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2155,7 +2240,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
@@ -2170,7 +2255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
@@ -2185,7 +2270,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2200,7 +2285,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
@@ -2215,7 +2300,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2230,7 +2315,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
@@ -2245,7 +2330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
@@ -2260,7 +2345,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
@@ -2275,7 +2360,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>48</v>
       </c>
@@ -2290,7 +2375,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>50</v>
       </c>
@@ -2305,7 +2390,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>52</v>
       </c>
@@ -2320,7 +2405,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>54</v>
       </c>
@@ -2335,7 +2420,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>56</v>
       </c>
@@ -2350,7 +2435,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>58</v>
       </c>
@@ -2365,7 +2450,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>60</v>
       </c>
@@ -2380,7 +2465,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="7" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
@@ -2392,8 +2477,11 @@
       <c r="E26" s="5"/>
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>63</v>
       </c>
@@ -2408,7 +2496,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
@@ -2423,7 +2511,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>67</v>
       </c>
@@ -2438,7 +2526,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>68</v>
       </c>
@@ -2453,7 +2541,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>69</v>
       </c>
@@ -2468,7 +2556,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>70</v>
       </c>
@@ -2483,7 +2571,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>71</v>
       </c>
@@ -2498,7 +2586,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>72</v>
       </c>
@@ -2510,8 +2598,11 @@
       <c r="E34" s="12"/>
       <c r="F34" s="21"/>
       <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H34" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>74</v>
       </c>
@@ -2528,7 +2619,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>78</v>
       </c>
@@ -2545,7 +2636,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>80</v>
       </c>
@@ -2562,7 +2653,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>82</v>
       </c>
@@ -2574,8 +2665,11 @@
       <c r="E38" s="5"/>
       <c r="F38" s="6"/>
       <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
         <v>84</v>
       </c>
@@ -2589,7 +2683,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>87</v>
       </c>
@@ -2603,7 +2697,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>89</v>
       </c>
@@ -2617,7 +2711,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>91</v>
       </c>
@@ -2631,7 +2725,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>93</v>
       </c>
@@ -2643,8 +2737,11 @@
       <c r="E43" s="17"/>
       <c r="F43" s="16"/>
       <c r="G43" s="17"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>84</v>
       </c>
@@ -2656,7 +2753,7 @@
       </c>
       <c r="F44" s="20"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>97</v>
       </c>
@@ -2668,7 +2765,7 @@
       </c>
       <c r="F45" s="20"/>
     </row>
-    <row r="46" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>99</v>
       </c>
@@ -2680,8 +2777,11 @@
       <c r="E46" s="5"/>
       <c r="F46" s="6"/>
       <c r="G46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>84</v>
       </c>
@@ -2695,7 +2795,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>103</v>
       </c>
@@ -2710,7 +2810,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>106</v>
       </c>
@@ -2722,8 +2822,11 @@
       <c r="E49" s="5"/>
       <c r="F49" s="6"/>
       <c r="G49" s="5"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>84</v>
       </c>
@@ -2735,7 +2838,7 @@
       </c>
       <c r="F50" s="20"/>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>109</v>
       </c>
@@ -2752,7 +2855,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
@@ -2764,8 +2867,11 @@
       <c r="E52" s="5"/>
       <c r="F52" s="6"/>
       <c r="G52" s="5"/>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H52" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>84</v>
       </c>
@@ -2779,7 +2885,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="C54" s="29" t="s">
         <v>117</v>
       </c>
@@ -2793,7 +2899,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="C55" s="28" t="s">
         <v>120</v>
       </c>
@@ -2807,7 +2913,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="C56" s="31" t="s">
         <v>123</v>
       </c>
@@ -2821,7 +2927,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="C57" s="28" t="s">
         <v>126</v>
       </c>
@@ -2835,7 +2941,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>129</v>
       </c>
@@ -2847,8 +2953,11 @@
       <c r="E58" s="5"/>
       <c r="F58" s="6"/>
       <c r="G58" s="5"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
         <v>84</v>
       </c>
@@ -2860,7 +2969,7 @@
       </c>
       <c r="F59" s="20"/>
     </row>
-    <row r="60" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="C60" s="7" t="s">
         <v>132</v>
       </c>
@@ -2874,7 +2983,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="C61" s="7" t="s">
         <v>135</v>
       </c>
@@ -2888,7 +2997,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>138</v>
       </c>
@@ -2900,8 +3009,11 @@
       <c r="E62" s="5"/>
       <c r="F62" s="6"/>
       <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H62" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
         <v>84</v>
       </c>
@@ -2912,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="C64" s="1" t="s">
         <v>141</v>
       </c>
@@ -2924,7 +3036,7 @@
       </c>
       <c r="F64" s="20"/>
     </row>
-    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
         <v>143</v>
       </c>
@@ -2938,7 +3050,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>146</v>
       </c>
@@ -2950,7 +3062,7 @@
       </c>
       <c r="F66" s="20"/>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
         <v>148</v>
       </c>
@@ -2962,7 +3074,7 @@
       </c>
       <c r="F67" s="20"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
         <v>150</v>
       </c>
@@ -2974,7 +3086,7 @@
       </c>
       <c r="F68" s="20"/>
     </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>152</v>
       </c>
@@ -2986,8 +3098,11 @@
       <c r="E69" s="5"/>
       <c r="F69" s="6"/>
       <c r="G69" s="5"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>84</v>
       </c>
@@ -3001,7 +3116,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
         <v>156</v>
       </c>
@@ -3015,7 +3130,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
         <v>159</v>
       </c>
@@ -3029,7 +3144,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>162</v>
       </c>
@@ -3041,8 +3156,11 @@
       <c r="E73" s="5"/>
       <c r="F73" s="6"/>
       <c r="G73" s="5"/>
-    </row>
-    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H73" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="C74" s="1" t="s">
         <v>84</v>
       </c>
@@ -3056,7 +3174,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
         <v>166</v>
       </c>
@@ -3070,7 +3188,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>169</v>
       </c>
@@ -3082,8 +3200,11 @@
       <c r="E76" s="5"/>
       <c r="F76" s="6"/>
       <c r="G76" s="5"/>
-    </row>
-    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H76" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C77" s="10" t="s">
         <v>84</v>
       </c>
@@ -3100,7 +3221,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>0.314</v>
       </c>
@@ -3112,7 +3233,7 @@
       </c>
       <c r="F78" s="20"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>0.27800000000000002</v>
       </c>
@@ -3124,7 +3245,7 @@
       </c>
       <c r="F79" s="20"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>0.247</v>
       </c>
@@ -3136,7 +3257,7 @@
       </c>
       <c r="F80" s="20"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>0.21</v>
       </c>
@@ -3148,7 +3269,7 @@
       </c>
       <c r="F81" s="20"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>0.183</v>
       </c>
@@ -3160,7 +3281,7 @@
       </c>
       <c r="F82" s="20"/>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>175</v>
       </c>
@@ -3172,8 +3293,11 @@
       <c r="E83" s="5"/>
       <c r="F83" s="6"/>
       <c r="G83" s="5"/>
-    </row>
-    <row r="84" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H83" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C84" s="10" t="s">
         <v>84</v>
       </c>
@@ -3190,7 +3314,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>0.22700000000000001</v>
       </c>
@@ -3202,7 +3326,7 @@
       </c>
       <c r="F85" s="20"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>0.183</v>
       </c>
@@ -3214,7 +3338,7 @@
       </c>
       <c r="F86" s="20"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>0.16200000000000001</v>
       </c>
@@ -3226,7 +3350,7 @@
       </c>
       <c r="F87" s="20"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>0.14199999999999999</v>
       </c>
@@ -3238,7 +3362,7 @@
       </c>
       <c r="F88" s="20"/>
     </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>178</v>
       </c>
@@ -3250,8 +3374,11 @@
       <c r="E89" s="5"/>
       <c r="F89" s="6"/>
       <c r="G89" s="5"/>
-    </row>
-    <row r="90" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H89" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C90" s="9" t="s">
         <v>84</v>
       </c>
@@ -3268,7 +3395,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>0.22700000000000001</v>
       </c>
@@ -3280,7 +3407,7 @@
       </c>
       <c r="F91" s="20"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <v>0.193</v>
       </c>
@@ -3292,7 +3419,7 @@
       </c>
       <c r="F92" s="20"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <v>0.183</v>
       </c>
@@ -3304,7 +3431,7 @@
       </c>
       <c r="F93" s="20"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <v>0.16200000000000001</v>
       </c>
@@ -3316,7 +3443,7 @@
       </c>
       <c r="F94" s="20"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <v>0.14199999999999999</v>
       </c>
@@ -3328,7 +3455,7 @@
       </c>
       <c r="F95" s="20"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <v>0.13800000000000001</v>
       </c>
@@ -3340,7 +3467,7 @@
       </c>
       <c r="F96" s="20"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C97" s="1">
         <v>0.121</v>
       </c>
@@ -3352,7 +3479,7 @@
       </c>
       <c r="F97" s="20"/>
     </row>
-    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>180</v>
       </c>
@@ -3364,8 +3491,11 @@
       <c r="E98" s="5"/>
       <c r="F98" s="6"/>
       <c r="G98" s="5"/>
-    </row>
-    <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H98" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
         <v>84</v>
       </c>
@@ -3382,7 +3512,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
         <v>0.56799999999999995</v>
       </c>
@@ -3394,7 +3524,7 @@
       </c>
       <c r="F100" s="20"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
         <v>0.379</v>
       </c>
@@ -3406,7 +3536,7 @@
       </c>
       <c r="F101" s="20"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C102" s="1">
         <v>0.28399999999999997</v>
       </c>
@@ -3418,7 +3548,7 @@
       </c>
       <c r="F102" s="20"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C103" s="1">
         <v>0.21</v>
       </c>
@@ -3430,7 +3560,7 @@
       </c>
       <c r="F103" s="20"/>
     </row>
-    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>182</v>
       </c>
@@ -3442,8 +3572,11 @@
       <c r="E104" s="5"/>
       <c r="F104" s="6"/>
       <c r="G104" s="5"/>
-    </row>
-    <row r="105" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H104" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C105" s="1" t="s">
         <v>84</v>
       </c>
@@ -3460,7 +3593,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C106" s="1">
         <v>0.75800000000000001</v>
       </c>
@@ -3472,7 +3605,7 @@
       </c>
       <c r="F106" s="20"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C107" s="1">
         <v>0.379</v>
       </c>
@@ -3484,13 +3617,13 @@
       </c>
       <c r="F107" s="20"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E108" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F108" s="20"/>
     </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>184</v>
       </c>
@@ -3502,8 +3635,11 @@
       <c r="E109" s="5"/>
       <c r="F109" s="6"/>
       <c r="G109" s="5"/>
-    </row>
-    <row r="110" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H109" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C110" s="9" t="s">
         <v>186</v>
       </c>
@@ -3520,7 +3656,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C111" s="1">
         <v>0.56799999999999995</v>
       </c>
@@ -3532,7 +3668,7 @@
       </c>
       <c r="F111" s="20"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C112" s="4">
         <v>0.379</v>
       </c>
@@ -3544,7 +3680,7 @@
       </c>
       <c r="F112" s="20"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C113" s="1">
         <v>0.28399999999999997</v>
       </c>
@@ -3556,7 +3692,7 @@
       </c>
       <c r="F113" s="20"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C114" s="1">
         <v>0.21</v>
       </c>
@@ -3568,7 +3704,7 @@
       </c>
       <c r="F114" s="20"/>
     </row>
-    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>187</v>
       </c>
@@ -3580,8 +3716,11 @@
       <c r="E115" s="5"/>
       <c r="F115" s="6"/>
       <c r="G115" s="5"/>
-    </row>
-    <row r="116" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H115" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C116" s="1" t="s">
         <v>84</v>
       </c>
@@ -3598,7 +3737,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C117" s="1">
         <v>2.4</v>
       </c>
@@ -3610,7 +3749,7 @@
       </c>
       <c r="F117" s="20"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C118" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -3622,7 +3761,7 @@
       </c>
       <c r="F118" s="20"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C119" s="1">
         <v>1.6</v>
       </c>
@@ -3634,7 +3773,7 @@
       </c>
       <c r="F119" s="20"/>
     </row>
-    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>189</v>
       </c>
@@ -3645,8 +3784,11 @@
       <c r="D120" s="16"/>
       <c r="E120" s="18"/>
       <c r="F120" s="22"/>
-    </row>
-    <row r="121" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H120" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C121" s="1" t="s">
         <v>84</v>
       </c>
@@ -3663,7 +3805,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C122" s="1">
         <v>2.4</v>
       </c>
@@ -3675,7 +3817,7 @@
       </c>
       <c r="F122" s="20"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C123" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -3687,7 +3829,7 @@
       </c>
       <c r="F123" s="20"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C124" s="1">
         <v>1.6</v>
       </c>
@@ -3699,7 +3841,7 @@
       </c>
       <c r="F124" s="20"/>
     </row>
-    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>191</v>
       </c>
@@ -3711,8 +3853,11 @@
       <c r="E125" s="5"/>
       <c r="F125" s="6"/>
       <c r="G125" s="5"/>
-    </row>
-    <row r="126" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H125" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C126" s="1" t="s">
         <v>84</v>
       </c>
@@ -3729,7 +3874,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C127" s="1">
         <v>2.4</v>
       </c>
@@ -3741,7 +3886,7 @@
       </c>
       <c r="F127" s="20"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C128" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -3753,7 +3898,7 @@
       </c>
       <c r="F128" s="20"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C129" s="1">
         <v>1.6</v>
       </c>
@@ -3765,7 +3910,7 @@
       </c>
       <c r="F129" s="20"/>
     </row>
-    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>193</v>
       </c>
@@ -3777,8 +3922,11 @@
       <c r="E130" s="18"/>
       <c r="F130" s="22"/>
       <c r="G130" s="17"/>
-    </row>
-    <row r="131" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H130" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C131" s="1" t="s">
         <v>84</v>
       </c>
@@ -3795,7 +3943,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C132" s="1">
         <v>2.4</v>
       </c>
@@ -3807,7 +3955,7 @@
       </c>
       <c r="F132" s="20"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C133" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -3819,7 +3967,7 @@
       </c>
       <c r="F133" s="20"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C134" s="1">
         <v>1.6</v>
       </c>
@@ -3831,7 +3979,7 @@
       </c>
       <c r="F134" s="20"/>
     </row>
-    <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>195</v>
       </c>
@@ -3843,8 +3991,11 @@
       <c r="E135" s="18"/>
       <c r="F135" s="22"/>
       <c r="G135" s="5"/>
-    </row>
-    <row r="136" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H135" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C136" s="1" t="s">
         <v>84</v>
       </c>
@@ -3861,7 +4012,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C137" s="1">
         <v>0.05</v>
       </c>
@@ -3870,7 +4021,7 @@
       </c>
       <c r="F137" s="20"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C138" s="1">
         <v>0.9</v>
       </c>
@@ -3882,7 +4033,7 @@
       </c>
       <c r="F138" s="20"/>
     </row>
-    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>197</v>
       </c>
@@ -3894,8 +4045,11 @@
       <c r="E139" s="19"/>
       <c r="F139" s="23"/>
       <c r="G139" s="5"/>
-    </row>
-    <row r="140" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H139" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C140" s="1" t="s">
         <v>84</v>
       </c>
@@ -3912,7 +4066,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C141" s="1">
         <v>0.05</v>
       </c>
@@ -3924,7 +4078,7 @@
       </c>
       <c r="F141" s="20"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C142" s="1">
         <v>0.9</v>
       </c>
@@ -3936,7 +4090,7 @@
       </c>
       <c r="F142" s="20"/>
     </row>
-    <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>199</v>
       </c>
@@ -3948,8 +4102,11 @@
       <c r="E143" s="19"/>
       <c r="F143" s="23"/>
       <c r="G143" s="5"/>
-    </row>
-    <row r="144" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H143" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C144" s="1" t="s">
         <v>84</v>
       </c>
@@ -3963,7 +4120,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C145" s="1">
         <v>0.05</v>
       </c>
@@ -3972,7 +4129,7 @@
       </c>
       <c r="F145" s="20"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C146" s="1">
         <v>0.9</v>
       </c>
@@ -3981,7 +4138,7 @@
       </c>
       <c r="F146" s="20"/>
     </row>
-    <row r="147" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>201</v>
       </c>
@@ -3993,8 +4150,11 @@
       <c r="E147" s="19"/>
       <c r="F147" s="23"/>
       <c r="G147" s="5"/>
-    </row>
-    <row r="148" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="H147" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="C148" s="1" t="s">
         <v>84</v>
       </c>
@@ -4011,7 +4171,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C149" s="1" t="s">
         <v>97</v>
       </c>
@@ -4023,7 +4183,7 @@
       </c>
       <c r="F149" s="20"/>
     </row>
-    <row r="150" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>207</v>
       </c>
@@ -4036,8 +4196,11 @@
       <c r="E150" s="19"/>
       <c r="F150" s="23"/>
       <c r="G150" s="5"/>
-    </row>
-    <row r="151" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="H150" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="C151" s="1" t="s">
         <v>84</v>
       </c>
@@ -4054,7 +4217,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C152" s="1" t="s">
         <v>97</v>
       </c>
@@ -4066,7 +4229,7 @@
       </c>
       <c r="F152" s="20"/>
     </row>
-    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>210</v>
       </c>
@@ -4078,8 +4241,11 @@
       <c r="E153" s="19"/>
       <c r="F153" s="23"/>
       <c r="G153" s="5"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H153" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C154" s="1" t="s">
         <v>84</v>
       </c>
@@ -4091,7 +4257,7 @@
       </c>
       <c r="F154" s="20"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C155" s="1" t="s">
         <v>97</v>
       </c>
@@ -4103,7 +4269,7 @@
       </c>
       <c r="F155" s="20"/>
     </row>
-    <row r="156" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>214</v>
       </c>
@@ -4115,8 +4281,11 @@
       <c r="E156" s="19"/>
       <c r="F156" s="23"/>
       <c r="G156" s="5"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H156" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C157" s="1" t="s">
         <v>97</v>
       </c>
@@ -4128,7 +4297,7 @@
       </c>
       <c r="F157" s="20"/>
     </row>
-    <row r="158" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>217</v>
       </c>
@@ -4140,8 +4309,11 @@
       <c r="E158" s="19"/>
       <c r="F158" s="23"/>
       <c r="G158" s="5"/>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H158" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
         <v>97</v>
       </c>
@@ -4153,7 +4325,7 @@
       </c>
       <c r="F159" s="20"/>
     </row>
-    <row r="160" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>219</v>
       </c>
@@ -4165,8 +4337,11 @@
       <c r="E160" s="19"/>
       <c r="F160" s="23"/>
       <c r="G160" s="5"/>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H160" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C161" s="1" t="s">
         <v>97</v>
       </c>
@@ -4178,7 +4353,7 @@
       </c>
       <c r="F161" s="20"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>221</v>
       </c>
@@ -4190,8 +4365,11 @@
       <c r="E162" s="19"/>
       <c r="F162" s="23"/>
       <c r="G162" s="5"/>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H162" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C163" s="1" t="s">
         <v>84</v>
       </c>
@@ -4203,7 +4381,7 @@
       </c>
       <c r="F163" s="20"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C164" s="1" t="s">
         <v>224</v>
       </c>
@@ -4220,15 +4398,18 @@
         <v>226</v>
       </c>
     </row>
-    <row r="165" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>227</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H165" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="C166" s="1" t="s">
         <v>84</v>
       </c>
@@ -4241,7 +4422,7 @@
       <c r="F166" s="25"/>
       <c r="G166" s="3"/>
     </row>
-    <row r="167" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C167" s="1" t="s">
         <v>97</v>
       </c>
@@ -4258,7 +4439,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>231</v>
       </c>
@@ -4270,8 +4451,11 @@
       <c r="E168" s="19"/>
       <c r="F168" s="23"/>
       <c r="G168" s="5"/>
-    </row>
-    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H168" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C169" s="1" t="s">
         <v>84</v>
       </c>
@@ -4283,7 +4467,7 @@
       </c>
       <c r="F169" s="20"/>
     </row>
-    <row r="170" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="C170" s="1" t="s">
         <v>97</v>
       </c>
@@ -4300,7 +4484,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>235</v>
       </c>
@@ -4312,8 +4496,11 @@
       <c r="E171" s="19"/>
       <c r="F171" s="23"/>
       <c r="G171" s="5"/>
-    </row>
-    <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H171" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C172" s="1" t="s">
         <v>84</v>
       </c>
@@ -4325,7 +4512,7 @@
       </c>
       <c r="F172" s="20"/>
     </row>
-    <row r="173" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C173" s="1" t="s">
         <v>97</v>
       </c>
@@ -4342,7 +4529,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>239</v>
       </c>
@@ -4354,8 +4541,11 @@
       <c r="E174" s="19"/>
       <c r="F174" s="23"/>
       <c r="G174" s="5"/>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H174" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C175" s="1" t="s">
         <v>84</v>
       </c>
@@ -4372,7 +4562,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C176" s="1" t="s">
         <v>242</v>
       </c>
@@ -4389,7 +4579,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C177" s="1" t="s">
         <v>244</v>
       </c>
@@ -4406,7 +4596,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C178" s="1" t="s">
         <v>246</v>
       </c>
@@ -4423,7 +4613,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>248</v>
       </c>
@@ -4435,8 +4625,11 @@
       <c r="E179" s="19"/>
       <c r="F179" s="23"/>
       <c r="G179" s="5"/>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H179" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C180" s="1" t="s">
         <v>84</v>
       </c>
@@ -4448,7 +4641,7 @@
       </c>
       <c r="F180" s="20"/>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C181" s="1" t="s">
         <v>251</v>
       </c>
@@ -4460,13 +4653,13 @@
       </c>
       <c r="F181" s="20"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E182" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F182" s="20"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>253</v>
       </c>
@@ -4478,8 +4671,11 @@
       <c r="E183" s="19"/>
       <c r="F183" s="23"/>
       <c r="G183" s="5"/>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H183" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C184" s="1" t="s">
         <v>84</v>
       </c>
@@ -4491,7 +4687,7 @@
       </c>
       <c r="F184" s="20"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C185" s="1" t="s">
         <v>256</v>
       </c>
@@ -4508,7 +4704,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>259</v>
       </c>
@@ -4520,8 +4716,11 @@
       <c r="E186" s="19"/>
       <c r="F186" s="23"/>
       <c r="G186" s="5"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H186" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C187" s="1" t="s">
         <v>84</v>
       </c>
@@ -4533,7 +4732,7 @@
       </c>
       <c r="F187" s="20"/>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C188" s="1" t="s">
         <v>97</v>
       </c>
@@ -4550,7 +4749,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>263</v>
       </c>
@@ -4562,8 +4761,11 @@
       <c r="E189" s="19"/>
       <c r="F189" s="23"/>
       <c r="G189" s="5"/>
-    </row>
-    <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H189" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="C190" s="1" t="s">
         <v>84</v>
       </c>
@@ -4575,7 +4777,7 @@
       </c>
       <c r="F190" s="20"/>
     </row>
-    <row r="191" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="C191" s="1" t="s">
         <v>97</v>
       </c>
@@ -4592,15 +4794,18 @@
         <v>258</v>
       </c>
     </row>
-    <row r="192" spans="1:7" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" s="5" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>267</v>
       </c>
       <c r="B192" s="6" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H192" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="C193" s="1" t="s">
         <v>84</v>
       </c>
@@ -4613,7 +4818,7 @@
       <c r="F193" s="25"/>
       <c r="G193" s="3"/>
     </row>
-    <row r="194" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C194" s="1" t="s">
         <v>97</v>
       </c>
@@ -4630,7 +4835,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>271</v>
       </c>
@@ -4642,8 +4847,11 @@
       <c r="E195" s="19"/>
       <c r="F195" s="23"/>
       <c r="G195" s="5"/>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H195" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C196" s="1" t="s">
         <v>84</v>
       </c>
@@ -4655,7 +4863,7 @@
       </c>
       <c r="F196" s="20"/>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C197" s="1" t="s">
         <v>97</v>
       </c>
@@ -4667,7 +4875,7 @@
       </c>
       <c r="F197" s="20"/>
     </row>
-    <row r="198" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>273</v>
       </c>
@@ -4679,8 +4887,11 @@
       <c r="E198" s="19"/>
       <c r="F198" s="23"/>
       <c r="G198" s="5"/>
-    </row>
-    <row r="199" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H198" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C199" s="1" t="s">
         <v>84</v>
       </c>
@@ -4694,7 +4905,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C200" s="1" t="s">
         <v>97</v>
       </c>
@@ -4708,7 +4919,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>277</v>
       </c>
@@ -4720,8 +4931,11 @@
       <c r="E201" s="19"/>
       <c r="F201" s="23"/>
       <c r="G201" s="5"/>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H201" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C202" s="1" t="s">
         <v>84</v>
       </c>
@@ -4733,7 +4947,7 @@
       </c>
       <c r="F202" s="20"/>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C203" s="1" t="s">
         <v>97</v>
       </c>
@@ -4745,7 +4959,7 @@
       </c>
       <c r="F203" s="20"/>
     </row>
-    <row r="204" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>279</v>
       </c>
@@ -4757,8 +4971,11 @@
       <c r="E204" s="19"/>
       <c r="F204" s="23"/>
       <c r="G204" s="5"/>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H204" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C205" s="1" t="s">
         <v>84</v>
       </c>
@@ -4770,7 +4987,7 @@
       </c>
       <c r="F205" s="20"/>
     </row>
-    <row r="206" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="C206" s="1" t="s">
         <v>281</v>
       </c>
@@ -4782,7 +4999,7 @@
       </c>
       <c r="F206" s="20"/>
     </row>
-    <row r="207" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>283</v>
       </c>
@@ -4794,8 +5011,11 @@
       <c r="E207" s="19"/>
       <c r="F207" s="23"/>
       <c r="G207" s="17"/>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H207" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C208" s="1" t="s">
         <v>84</v>
       </c>
@@ -4807,7 +5027,7 @@
       </c>
       <c r="F208" s="20"/>
     </row>
-    <row r="209" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C209" s="1" t="s">
         <v>97</v>
       </c>
@@ -4820,29 +5040,52 @@
       <c r="F209" s="20"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H209"/>
   <conditionalFormatting sqref="E3:E7 E148:E149 E151:E152 E154:E155 E157 E159 E161 E163:E164 E169:E170 E175:E178 E180:E182 E184:E185 E196:E197 E199:E200 E202:E203 E205:E206 E208:E209 E187:E188 E190:E191 E193:E194 E166:E167 E172:E173">
-    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E126:E129 E131:E134 E136:E138 E140:E142 E144:E146">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="7" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="8" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:E37">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39:E42 E44:E45">
+    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:E48">
     <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4853,7 +5096,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39:E42 E44:E45">
+  <conditionalFormatting sqref="E50:E51">
     <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4864,7 +5107,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47:E48">
+  <conditionalFormatting sqref="E53:E57">
     <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4875,7 +5118,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50:E51">
+  <conditionalFormatting sqref="E59:E61">
     <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4886,7 +5129,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53:E57">
+  <conditionalFormatting sqref="E63:E68">
     <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4897,7 +5140,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E59:E61">
+  <conditionalFormatting sqref="E70:E72">
     <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4908,7 +5151,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E63:E68">
+  <conditionalFormatting sqref="E74:E75">
     <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4919,7 +5162,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E70:E72">
+  <conditionalFormatting sqref="E77:E82">
     <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4930,7 +5173,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74:E75">
+  <conditionalFormatting sqref="E84:E88">
     <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4941,7 +5184,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77:E82">
+  <conditionalFormatting sqref="E91:E97">
     <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4952,7 +5195,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84:E88">
+  <conditionalFormatting sqref="E90">
     <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4963,7 +5206,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E97">
+  <conditionalFormatting sqref="E99:E103">
     <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4974,7 +5217,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E90">
+  <conditionalFormatting sqref="E105:E108">
     <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4985,7 +5228,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E99:E103">
+  <conditionalFormatting sqref="E110:E114">
     <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -4996,7 +5239,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E105:E108">
+  <conditionalFormatting sqref="E116:E119 E121:E124">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5004,28 +5247,6 @@
       <formula>FALSE</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E110:E114">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E116:E119 E121:E124">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added description for the baseline_system_zones_map_option arg into BTAPOptions.xlsx
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgilani\Dropbox\NRCan\BTAP\ECM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgilani\btap_batch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="297">
   <si>
     <t>Variable</t>
   </si>
@@ -913,6 +913,24 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>:baseline_system_zones_map_option</t>
+  </si>
+  <si>
+    <t>Will choose between in-suite and central DOAS</t>
+  </si>
+  <si>
+    <t>one_sys_per_bldg</t>
+  </si>
+  <si>
+    <t>one_sys_per_dwelling_unit</t>
+  </si>
+  <si>
+    <t>Will use central DOAS</t>
+  </si>
+  <si>
+    <t>Will use in-suite DOAS</t>
   </si>
 </sst>
 </file>
@@ -2055,11 +2073,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H209"/>
+  <dimension ref="A1:H213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C211" sqref="C211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5027,7 +5045,7 @@
       </c>
       <c r="F208" s="20"/>
     </row>
-    <row r="209" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C209" s="1" t="s">
         <v>97</v>
       </c>
@@ -5038,215 +5056,293 @@
         <v>29</v>
       </c>
       <c r="F209" s="20"/>
+    </row>
+    <row r="210" spans="1:8" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A210" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C210" s="6"/>
+      <c r="D210" s="6"/>
+      <c r="E210" s="6"/>
+      <c r="F210" s="6"/>
+      <c r="G210" s="6"/>
+      <c r="H210" s="6"/>
+    </row>
+    <row r="211" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C211" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E211" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H211" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C212" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E212" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H212" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C213" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E213" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H213" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H209"/>
   <conditionalFormatting sqref="E3:E7 E148:E149 E151:E152 E154:E155 E157 E159 E161 E163:E164 E169:E170 E175:E178 E180:E182 E184:E185 E196:E197 E199:E200 E202:E203 E205:E206 E208:E209 E187:E188 E190:E191 E193:E194 E166:E167 E172:E173">
-    <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="68" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="69" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E126:E129 E131:E134 E136:E138 E140:E142 E144:E146">
-    <cfRule type="cellIs" dxfId="59" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="13" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="14" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:E37">
-    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="66" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:E42 E44:E45">
-    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="61" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="62" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="63" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:E48">
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="58" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="59" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50:E51">
-    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E57">
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E61">
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="50" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="51" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:E68">
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:E72">
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="44" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E75">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="41" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77:E82">
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="38" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84:E88">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91:E97">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99:E103">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105:E108">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E110:E114">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E116:E119 E121:E124">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E213">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E211:E212">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed NPV calculation method from btap_batch.py; Added NPV to BTAPOptions.xlsx; Updated all .yml files
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgilani\btap_batch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A52AF4-832C-4896-BE7D-5E9574E2E6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6045" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadME" sheetId="2" r:id="rId1"/>
@@ -23,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="310">
   <si>
     <t>Variable</t>
   </si>
@@ -931,12 +923,51 @@
   </si>
   <si>
     <t>Will use in-suite DOAS</t>
+  </si>
+  <si>
+    <t>:npv_start_year</t>
+  </si>
+  <si>
+    <t>Will set start year for the calculation of net present value</t>
+  </si>
+  <si>
+    <t>Integer/Number</t>
+  </si>
+  <si>
+    <t>Default start year has been set as 2022.</t>
+  </si>
+  <si>
+    <t>:npv_end_year</t>
+  </si>
+  <si>
+    <t>Default end year has been set as 2041.</t>
+  </si>
+  <si>
+    <t>Start year must be larger than start year of Canada Energy Regulator's (CER) energy prices data (See neb_end_use_prices.csv in openstudio-standards).</t>
+  </si>
+  <si>
+    <t>End year must be smaller than end year of Canada Energy Regulator's (CER) energy prices data (See neb_end_use_prices.csv in openstudio-standards).</t>
+  </si>
+  <si>
+    <t>:npv_discount_rate</t>
+  </si>
+  <si>
+    <t>Will set end year for the calculation of net present value</t>
+  </si>
+  <si>
+    <t>Will set discount rate for the calculation of net present value</t>
+  </si>
+  <si>
+    <t>Discount rate must be between 0.0 and 1.0.</t>
+  </si>
+  <si>
+    <t>Default discount rate has been set as 0.03 (i.e. 3%).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2052,7 +2083,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2072,19 +2103,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H213"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C211" sqref="C211"/>
+      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D222" sqref="D222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="44.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.7109375" style="2" customWidth="1"/>
@@ -5113,8 +5144,126 @@
         <v>289</v>
       </c>
     </row>
+    <row r="214" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C214" s="6"/>
+      <c r="D214" s="6"/>
+      <c r="E214" s="6"/>
+      <c r="F214" s="6"/>
+      <c r="G214" s="6"/>
+      <c r="H214" s="6"/>
+    </row>
+    <row r="215" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C215" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+      <c r="C216" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C217" s="6"/>
+      <c r="D217" s="6"/>
+      <c r="E217" s="6"/>
+      <c r="F217" s="6"/>
+      <c r="G217" s="6"/>
+      <c r="H217" s="6"/>
+    </row>
+    <row r="218" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C218" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+      <c r="C219" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C220" s="6"/>
+      <c r="D220" s="6"/>
+      <c r="E220" s="6"/>
+      <c r="F220" s="6"/>
+      <c r="G220" s="6"/>
+      <c r="H220" s="6"/>
+    </row>
+    <row r="221" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="C221" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C222" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="6"/>
+      <c r="B223" s="6"/>
+      <c r="C223" s="6"/>
+      <c r="D223" s="6"/>
+      <c r="E223" s="6"/>
+      <c r="F223" s="6"/>
+      <c r="G223" s="6"/>
+      <c r="H223" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H209"/>
+  <autoFilter ref="A1:H209" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="E3:E7 E148:E149 E151:E152 E154:E155 E157 E159 E161 E163:E164 E169:E170 E175:E178 E180:E182 E184:E185 E196:E197 E199:E200 E202:E203 E205:E206 E208:E209 E187:E188 E190:E191 E193:E194 E166:E167 E172:E173">
     <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"UNKNOWN"</formula>
@@ -5347,61 +5496,61 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1"/>
-    <hyperlink ref="G22" r:id="rId2"/>
-    <hyperlink ref="G24" r:id="rId3"/>
-    <hyperlink ref="G15" r:id="rId4"/>
-    <hyperlink ref="G13" r:id="rId5"/>
-    <hyperlink ref="G23" r:id="rId6"/>
-    <hyperlink ref="G12" r:id="rId7"/>
-    <hyperlink ref="G21" r:id="rId8"/>
-    <hyperlink ref="G25" r:id="rId9"/>
-    <hyperlink ref="G10" r:id="rId10"/>
-    <hyperlink ref="G11" r:id="rId11"/>
-    <hyperlink ref="G14" r:id="rId12"/>
-    <hyperlink ref="G16" r:id="rId13"/>
-    <hyperlink ref="G17" r:id="rId14"/>
-    <hyperlink ref="G19" r:id="rId15"/>
-    <hyperlink ref="G20" r:id="rId16"/>
-    <hyperlink ref="G27" r:id="rId17"/>
-    <hyperlink ref="G28:G33" r:id="rId18" display="https://github.com/NREL/openstudio-standards/tree/nrcan/data/weather"/>
-    <hyperlink ref="G18" r:id="rId19"/>
-    <hyperlink ref="G4" r:id="rId20"/>
-    <hyperlink ref="G5" r:id="rId21"/>
-    <hyperlink ref="G6" r:id="rId22"/>
-    <hyperlink ref="G7" r:id="rId23"/>
-    <hyperlink ref="G35" r:id="rId24"/>
-    <hyperlink ref="G36" r:id="rId25"/>
-    <hyperlink ref="G37" r:id="rId26"/>
-    <hyperlink ref="G39" r:id="rId27"/>
-    <hyperlink ref="G40:G42" r:id="rId28" display="https://github.com/NREL/openstudio-standards/blob/nrcan/lib/openstudio-standards/standards/necb/NECB2011/demand_controlled_ventilation.md"/>
-    <hyperlink ref="G48" r:id="rId29"/>
-    <hyperlink ref="G51" r:id="rId30"/>
-    <hyperlink ref="G77" r:id="rId31"/>
-    <hyperlink ref="G84" r:id="rId32" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G90" r:id="rId33" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G99" r:id="rId34" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G105" r:id="rId35" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G110" r:id="rId36" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G116" r:id="rId37" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G121" r:id="rId38" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G126" r:id="rId39" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G131" r:id="rId40" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G136" r:id="rId41" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G140" r:id="rId42" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G144" r:id="rId43" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm"/>
-    <hyperlink ref="G164" r:id="rId44"/>
-    <hyperlink ref="G170" r:id="rId45"/>
-    <hyperlink ref="G173" r:id="rId46"/>
-    <hyperlink ref="G175" r:id="rId47"/>
-    <hyperlink ref="G176" r:id="rId48"/>
-    <hyperlink ref="G177" r:id="rId49"/>
-    <hyperlink ref="G178" r:id="rId50"/>
-    <hyperlink ref="G167" r:id="rId51"/>
-    <hyperlink ref="G185" r:id="rId52"/>
-    <hyperlink ref="G188" r:id="rId53"/>
-    <hyperlink ref="G191" r:id="rId54"/>
-    <hyperlink ref="G194" r:id="rId55"/>
+    <hyperlink ref="G9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G22" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G24" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G15" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G13" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="G23" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="G12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="G21" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="G25" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="G11" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="G19" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="G20" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="G27" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="G28:G33" r:id="rId18" display="https://github.com/NREL/openstudio-standards/tree/nrcan/data/weather" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="G18" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="G4" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="G5" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="G6" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="G7" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="G35" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="G36" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="G37" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="G39" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="G40:G42" r:id="rId28" display="https://github.com/NREL/openstudio-standards/blob/nrcan/lib/openstudio-standards/standards/necb/NECB2011/demand_controlled_ventilation.md" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="G48" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G51" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G77" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G84" r:id="rId32" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G90" r:id="rId33" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G99" r:id="rId34" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G105" r:id="rId35" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G110" r:id="rId36" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G116" r:id="rId37" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="G121" r:id="rId38" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="G126" r:id="rId39" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="G131" r:id="rId40" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="G136" r:id="rId41" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="G140" r:id="rId42" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="G144" r:id="rId43" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="G164" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="G170" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="G173" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="G175" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="G176" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="G177" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="G178" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="G167" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="G185" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="G188" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="G191" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="G194" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId56"/>

</xml_diff>

<commit_message>
add entry for ecm HS14
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\btap_batch\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khaddad\btap_batch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9816AB-1CC5-434B-B80E-1DFBFD48E64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550534D0-D05F-4BB2-9EDA-A3512525D3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadME" sheetId="2" r:id="rId1"/>
     <sheet name="BTAPOptions" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BTAPOptions!$A$1:$H$214</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BTAPOptions!$A$1:$H$215</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="319">
   <si>
     <t>Variable</t>
   </si>
@@ -980,6 +980,15 @@
   </si>
   <si>
     <t>Adds daylight sensors for light control in each space regardless of  NECB's requirements</t>
+  </si>
+  <si>
+    <t>HS14_CGSHP_FanCoils</t>
+  </si>
+  <si>
+    <t>Use a dedicated-outdoor air system with four-pipe fan coils in the zones. The heating and cooling coils of the air system and the zones are served by a central ground source heat pump and chiller plant.</t>
+  </si>
+  <si>
+    <t>The central-ground source heat pump (size = 40% of peak heating load) and boiler (size = 60% of peak heating load) are used to meet the heating demand. The cooling demand is met using a water-cooled chiller (size = 40% of peak cooling load) and a air-cooled chiller (size = 60% of peak cooling load). The heat pump and water-cooled chiller are connected to a ground-loop heat exchanger.</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1187,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2099,9 +2108,9 @@
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>282</v>
       </c>
@@ -2113,27 +2122,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H228"/>
+  <dimension ref="A1:H229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2159,7 +2168,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2175,7 +2184,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2189,7 +2198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2203,7 +2212,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>307</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
@@ -2248,7 +2257,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>22</v>
@@ -2266,7 +2275,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -2282,7 +2291,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2297,7 +2306,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
@@ -2312,7 +2321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
@@ -2327,7 +2336,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
@@ -2342,7 +2351,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
@@ -2372,7 +2381,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
@@ -2387,7 +2396,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
@@ -2402,7 +2411,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
@@ -2417,7 +2426,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
@@ -2432,7 +2441,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>48</v>
       </c>
@@ -2447,7 +2456,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>50</v>
       </c>
@@ -2462,7 +2471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>52</v>
       </c>
@@ -2477,7 +2486,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
@@ -2492,7 +2501,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>56</v>
       </c>
@@ -2507,7 +2516,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
@@ -2522,7 +2531,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
@@ -2537,7 +2546,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
@@ -2553,7 +2562,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>63</v>
       </c>
@@ -2568,7 +2577,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>66</v>
       </c>
@@ -2583,7 +2592,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>67</v>
       </c>
@@ -2598,7 +2607,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>68</v>
       </c>
@@ -2613,7 +2622,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>69</v>
       </c>
@@ -2628,7 +2637,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>70</v>
       </c>
@@ -2643,7 +2652,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>71</v>
       </c>
@@ -2658,7 +2667,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>72</v>
       </c>
@@ -2674,7 +2683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>74</v>
       </c>
@@ -2691,7 +2700,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>78</v>
       </c>
@@ -2708,7 +2717,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>310</v>
       </c>
@@ -2717,7 +2726,7 @@
       </c>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>311</v>
       </c>
@@ -2726,7 +2735,7 @@
       </c>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>312</v>
       </c>
@@ -2735,7 +2744,7 @@
       </c>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>313</v>
       </c>
@@ -2744,7 +2753,7 @@
       </c>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>80</v>
       </c>
@@ -2761,7 +2770,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>82</v>
       </c>
@@ -2777,7 +2786,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
         <v>84</v>
       </c>
@@ -2791,7 +2800,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>87</v>
       </c>
@@ -2805,7 +2814,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>89</v>
       </c>
@@ -2819,7 +2828,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>91</v>
       </c>
@@ -2833,7 +2842,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>93</v>
       </c>
@@ -2849,7 +2858,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>84</v>
       </c>
@@ -2861,7 +2870,7 @@
       </c>
       <c r="F49" s="17"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>96</v>
       </c>
@@ -2873,7 +2882,7 @@
       </c>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>98</v>
       </c>
@@ -2889,7 +2898,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
         <v>84</v>
       </c>
@@ -2903,7 +2912,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>102</v>
       </c>
@@ -2918,7 +2927,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>105</v>
       </c>
@@ -2934,11 +2943,11 @@
         <v>286</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="2" t="s">
         <v>314</v>
       </c>
       <c r="E55" s="8" t="b">
@@ -2946,11 +2955,11 @@
       </c>
       <c r="F55" s="17"/>
     </row>
-    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D56" s="28" t="s">
+      <c r="D56" s="2" t="s">
         <v>315</v>
       </c>
       <c r="E56" s="8" t="b">
@@ -2963,7 +2972,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>110</v>
       </c>
@@ -2979,7 +2988,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
         <v>84</v>
       </c>
@@ -2993,7 +3002,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C59" s="25" t="s">
         <v>114</v>
       </c>
@@ -3007,7 +3016,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="C60" s="24" t="s">
         <v>117</v>
       </c>
@@ -3021,7 +3030,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C61" s="27" t="s">
         <v>120</v>
       </c>
@@ -3035,7 +3044,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C62" s="24" t="s">
         <v>123</v>
       </c>
@@ -3049,301 +3058,303 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
+    <row r="63" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C63" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="E63" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B64" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="1" t="s">
+      <c r="C64" s="5"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C64" s="1" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E64" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="17"/>
-    </row>
-    <row r="65" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C65" s="1" t="s">
+      <c r="E65" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="17"/>
+    </row>
+    <row r="66" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E65" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="17" t="s">
+      <c r="E66" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C66" s="1" t="s">
+    <row r="67" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E66" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="17" t="s">
+      <c r="E67" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="6" t="s">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B68" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="6" t="s">
+      <c r="C68" s="5"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C68" s="1" t="s">
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E68" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C69" s="1" t="s">
+      <c r="E69" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C70" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E69" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="17"/>
-    </row>
-    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C70" s="1" t="s">
+      <c r="E70" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="17"/>
+    </row>
+    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="17" t="s">
+      <c r="E71" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="17" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C71" s="1" t="s">
+    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E71" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="17"/>
-    </row>
-    <row r="72" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C72" s="1" t="s">
+      <c r="E72" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="17"/>
+    </row>
+    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C73" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E72" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="17"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C73" s="1" t="s">
+      <c r="E73" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="17"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E73" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="17"/>
-    </row>
-    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
+      <c r="E74" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="17"/>
+    </row>
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B75" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="6" t="s">
+      <c r="C75" s="5"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C75" s="1" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E75" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="17" t="s">
+      <c r="E76" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="17" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C76" s="1" t="s">
+    <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C77" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E76" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="17" t="s">
+      <c r="E77" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C77" s="1" t="s">
+    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C78" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E77" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="17" t="s">
+      <c r="E78" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="17" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A78" s="5" t="s">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B79" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="6" t="s">
+      <c r="C79" s="5"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C79" s="1" t="s">
+    <row r="80" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C80" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E79" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="17" t="s">
+      <c r="E80" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="17" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C80" s="1" t="s">
+    <row r="81" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="C81" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E80" s="8" t="b">
+      <c r="E81" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F80" s="17" t="s">
+      <c r="F81" s="17" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A81" s="5" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B82" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="6" t="s">
+      <c r="C82" s="5"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C82" s="7" t="s">
+    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C83" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E82" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="17" t="s">
+      <c r="E83" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G83" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C83" s="1">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C84" s="1">
         <v>0.314</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E83" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="17"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C84" s="1">
-        <v>0.27800000000000002</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>171</v>
@@ -3353,9 +3364,9 @@
       </c>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
-        <v>0.247</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>171</v>
@@ -3365,9 +3376,9 @@
       </c>
       <c r="F85" s="17"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
-        <v>0.21</v>
+        <v>0.247</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>171</v>
@@ -3377,9 +3388,9 @@
       </c>
       <c r="F86" s="17"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
-        <v>0.183</v>
+        <v>0.21</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>171</v>
@@ -3389,54 +3400,54 @@
       </c>
       <c r="F87" s="17"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C88" s="1">
+        <v>0.183</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E88" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="17"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B89" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="6"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="6" t="s">
+      <c r="C89" s="5"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C89" s="7" t="s">
+    <row r="90" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C90" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E89" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="17" t="s">
+      <c r="E90" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G89" s="21" t="s">
+      <c r="G90" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C90" s="1">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C91" s="1">
         <v>0.22700000000000001</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E90" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="17"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C91" s="1">
-        <v>0.183</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>171</v>
@@ -3446,9 +3457,9 @@
       </c>
       <c r="F91" s="17"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
-        <v>0.16200000000000001</v>
+        <v>0.183</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>171</v>
@@ -3458,9 +3469,9 @@
       </c>
       <c r="F92" s="17"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
-        <v>0.14199999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>171</v>
@@ -3470,54 +3481,54 @@
       </c>
       <c r="F93" s="17"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="5" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C94" s="1">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E94" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="17"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B95" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C94" s="5"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="6"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="6" t="s">
+      <c r="C95" s="5"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C95" s="7" t="s">
+    <row r="96" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C96" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E95" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="17" t="s">
+      <c r="E96" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G95" s="21" t="s">
+      <c r="G96" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C96" s="1">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C97" s="1">
         <v>0.22700000000000001</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E96" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="17"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C97" s="1">
-        <v>0.193</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>171</v>
@@ -3527,9 +3538,9 @@
       </c>
       <c r="F97" s="17"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C98" s="1">
-        <v>0.183</v>
+        <v>0.193</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>171</v>
@@ -3539,9 +3550,9 @@
       </c>
       <c r="F98" s="17"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C99" s="1">
-        <v>0.16200000000000001</v>
+        <v>0.183</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>171</v>
@@ -3551,9 +3562,9 @@
       </c>
       <c r="F99" s="17"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
-        <v>0.14199999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>171</v>
@@ -3563,9 +3574,9 @@
       </c>
       <c r="F100" s="17"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
-        <v>0.13800000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>171</v>
@@ -3575,9 +3586,9 @@
       </c>
       <c r="F101" s="17"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C102" s="1">
-        <v>0.121</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>171</v>
@@ -3587,54 +3598,54 @@
       </c>
       <c r="F102" s="17"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="5" t="s">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C103" s="1">
+        <v>0.121</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E103" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="17"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="B104" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C103" s="5"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="6" t="s">
+      <c r="C104" s="5"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C104" s="1" t="s">
+    <row r="105" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C105" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E104" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="17" t="s">
+      <c r="E105" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G104" s="21" t="s">
+      <c r="G105" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C105" s="1">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C106" s="1">
         <v>0.56799999999999995</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E105" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" s="17"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C106" s="1">
-        <v>0.379</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>171</v>
@@ -3644,9 +3655,9 @@
       </c>
       <c r="F106" s="17"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C107" s="1">
-        <v>0.28399999999999997</v>
+        <v>0.379</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>171</v>
@@ -3656,9 +3667,9 @@
       </c>
       <c r="F107" s="17"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C108" s="1">
-        <v>0.21</v>
+        <v>0.28399999999999997</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>171</v>
@@ -3668,54 +3679,54 @@
       </c>
       <c r="F108" s="17"/>
     </row>
-    <row r="109" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C109" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E109" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="17"/>
+    </row>
+    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B109" s="6" t="s">
+      <c r="B110" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C109" s="5"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="6"/>
-      <c r="G109" s="5"/>
-      <c r="H109" s="6" t="s">
+      <c r="C110" s="5"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C110" s="1" t="s">
+    <row r="111" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C111" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E110" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="17" t="s">
+      <c r="E111" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G110" s="21" t="s">
+      <c r="G111" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C111" s="1">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C112" s="1">
         <v>0.75800000000000001</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E111" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" s="17"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C112" s="1">
-        <v>0.379</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>171</v>
@@ -3725,60 +3736,60 @@
       </c>
       <c r="F112" s="17"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C113" s="1">
+        <v>0.379</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="E113" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F113" s="17"/>
     </row>
-    <row r="114" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A114" s="5" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E114" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" s="17"/>
+    </row>
+    <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B114" s="6" t="s">
+      <c r="B115" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C114" s="5"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="6"/>
-      <c r="G114" s="5"/>
-      <c r="H114" s="6" t="s">
+      <c r="C115" s="5"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C115" s="7" t="s">
+    <row r="116" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C116" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D116" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E115" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" s="17" t="s">
+      <c r="E116" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G115" s="21" t="s">
+      <c r="G116" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C116" s="1">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C117" s="1">
         <v>0.56799999999999995</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E116" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" s="17"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C117" s="4">
-        <v>0.379</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>171</v>
@@ -3788,9 +3799,9 @@
       </c>
       <c r="F117" s="17"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C118" s="1">
-        <v>0.28399999999999997</v>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C118" s="4">
+        <v>0.379</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>171</v>
@@ -3800,9 +3811,9 @@
       </c>
       <c r="F118" s="17"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C119" s="1">
-        <v>0.21</v>
+        <v>0.28399999999999997</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>171</v>
@@ -3812,54 +3823,54 @@
       </c>
       <c r="F119" s="17"/>
     </row>
-    <row r="120" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A120" s="5" t="s">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C120" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E120" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F120" s="17"/>
+    </row>
+    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B120" s="6" t="s">
+      <c r="B121" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C120" s="5"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="6"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="6" t="s">
+      <c r="C121" s="5"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C121" s="1" t="s">
+    <row r="122" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C122" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D122" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E121" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F121" s="17" t="s">
+      <c r="E122" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G121" s="21" t="s">
+      <c r="G122" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C122" s="1">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C123" s="1">
         <v>2.4</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E122" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F122" s="17"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C123" s="1">
-        <v>2.2000000000000002</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>171</v>
@@ -3869,9 +3880,9 @@
       </c>
       <c r="F123" s="17"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C124" s="1">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>171</v>
@@ -3881,53 +3892,53 @@
       </c>
       <c r="F124" s="17"/>
     </row>
-    <row r="125" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A125" s="5" t="s">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C125" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E125" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F125" s="17"/>
+    </row>
+    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B125" s="6" t="s">
+      <c r="B126" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C125" s="5"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="19"/>
-      <c r="H125" s="6" t="s">
+      <c r="C126" s="5"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="15"/>
+      <c r="F126" s="19"/>
+      <c r="H126" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C126" s="1" t="s">
+    <row r="127" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C127" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D127" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E126" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F126" s="17" t="s">
+      <c r="E127" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F127" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G126" s="21" t="s">
+      <c r="G127" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C127" s="1">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C128" s="1">
         <v>2.4</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E127" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F127" s="17"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C128" s="1">
-        <v>2.2000000000000002</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>171</v>
@@ -3937,9 +3948,9 @@
       </c>
       <c r="F128" s="17"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C129" s="1">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>171</v>
@@ -3949,54 +3960,54 @@
       </c>
       <c r="F129" s="17"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="5" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C130" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E130" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F130" s="17"/>
+    </row>
+    <row r="131" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B130" s="6" t="s">
+      <c r="B131" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C130" s="5"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="5"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="5"/>
-      <c r="H130" s="6" t="s">
+      <c r="C131" s="5"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="5"/>
+      <c r="H131" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C131" s="1" t="s">
+    <row r="132" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C132" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="D132" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E131" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F131" s="17" t="s">
+      <c r="E132" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F132" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G131" s="21" t="s">
+      <c r="G132" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C132" s="1">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C133" s="1">
         <v>2.4</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E132" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F132" s="17"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C133" s="1">
-        <v>2.2000000000000002</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>171</v>
@@ -4006,9 +4017,9 @@
       </c>
       <c r="F133" s="17"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C134" s="1">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>171</v>
@@ -4018,54 +4029,54 @@
       </c>
       <c r="F134" s="17"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A135" s="5" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C135" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E135" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F135" s="17"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B135" s="6" t="s">
+      <c r="B136" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C135" s="5"/>
-      <c r="D135" s="13"/>
-      <c r="E135" s="15"/>
-      <c r="F135" s="19"/>
-      <c r="G135" s="14"/>
-      <c r="H135" s="6" t="s">
+      <c r="C136" s="5"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="15"/>
+      <c r="F136" s="19"/>
+      <c r="G136" s="14"/>
+      <c r="H136" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C136" s="1" t="s">
+    <row r="137" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C137" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D136" s="2" t="s">
+      <c r="D137" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E136" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F136" s="17" t="s">
+      <c r="E137" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F137" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G136" s="21" t="s">
+      <c r="G137" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C137" s="1">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C138" s="1">
         <v>2.4</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E137" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F137" s="17"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C138" s="1">
-        <v>2.2000000000000002</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>171</v>
@@ -4075,9 +4086,9 @@
       </c>
       <c r="F138" s="17"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C139" s="1">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>171</v>
@@ -4087,108 +4098,108 @@
       </c>
       <c r="F139" s="17"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A140" s="5" t="s">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C140" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E140" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F140" s="17"/>
+    </row>
+    <row r="141" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B141" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C140" s="5"/>
-      <c r="D140" s="6"/>
-      <c r="E140" s="15"/>
-      <c r="F140" s="19"/>
-      <c r="G140" s="5"/>
-      <c r="H140" s="6" t="s">
+      <c r="C141" s="5"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="15"/>
+      <c r="F141" s="19"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C141" s="1" t="s">
+    <row r="142" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C142" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D141" s="2" t="s">
+      <c r="D142" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E141" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F141" s="17" t="s">
+      <c r="E142" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F142" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G141" s="21" t="s">
+      <c r="G142" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C142" s="1">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C143" s="1">
         <v>0.05</v>
       </c>
-      <c r="E142" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F142" s="17"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C143" s="1">
+      <c r="E143" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F143" s="17"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C144" s="1">
         <v>0.9</v>
       </c>
-      <c r="D143" s="2" t="s">
+      <c r="D144" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E143" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F143" s="17"/>
-    </row>
-    <row r="144" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A144" s="5" t="s">
+      <c r="E144" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F144" s="17"/>
+    </row>
+    <row r="145" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B144" s="6" t="s">
+      <c r="B145" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C144" s="5"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="16"/>
-      <c r="F144" s="20"/>
-      <c r="G144" s="5"/>
-      <c r="H144" s="6" t="s">
+      <c r="C145" s="5"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="16"/>
+      <c r="F145" s="20"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C145" s="1" t="s">
+    <row r="146" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C146" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D145" s="2" t="s">
+      <c r="D146" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E145" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F145" s="17" t="s">
+      <c r="E146" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F146" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G145" s="21" t="s">
+      <c r="G146" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C146" s="1">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C147" s="1">
         <v>0.05</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E146" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F146" s="17"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C147" s="1">
-        <v>0.9</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>171</v>
@@ -4198,484 +4209,479 @@
       </c>
       <c r="F147" s="17"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A148" s="5" t="s">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C148" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E148" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F148" s="17"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B148" s="6" t="s">
+      <c r="B149" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C148" s="5"/>
-      <c r="D148" s="6"/>
-      <c r="E148" s="16"/>
-      <c r="F148" s="20"/>
-      <c r="G148" s="5"/>
-      <c r="H148" s="6" t="s">
+      <c r="C149" s="5"/>
+      <c r="D149" s="6"/>
+      <c r="E149" s="16"/>
+      <c r="F149" s="20"/>
+      <c r="G149" s="5"/>
+      <c r="H149" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C149" s="1" t="s">
+    <row r="150" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C150" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E149" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F149" s="17" t="s">
+      <c r="E150" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F150" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G149" s="21" t="s">
+      <c r="G150" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C150" s="1">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C151" s="1">
         <v>0.05</v>
       </c>
-      <c r="E150" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F150" s="17"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C151" s="1">
+      <c r="E151" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F151" s="17"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C152" s="1">
         <v>0.9</v>
       </c>
-      <c r="E151" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F151" s="17"/>
-    </row>
-    <row r="152" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A152" s="5" t="s">
+      <c r="E152" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F152" s="17"/>
+    </row>
+    <row r="153" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B152" s="6" t="s">
+      <c r="B153" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C152" s="5"/>
-      <c r="D152" s="6"/>
-      <c r="E152" s="16"/>
-      <c r="F152" s="20"/>
-      <c r="G152" s="5"/>
-      <c r="H152" s="6" t="s">
+      <c r="C153" s="5"/>
+      <c r="D153" s="6"/>
+      <c r="E153" s="16"/>
+      <c r="F153" s="20"/>
+      <c r="G153" s="5"/>
+      <c r="H153" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C153" s="1" t="s">
+    <row r="154" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="C154" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D153" s="2" t="s">
+      <c r="D154" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E153" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F153" s="17" t="s">
+      <c r="E154" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F154" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="G153" s="1" t="s">
+      <c r="G154" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C154" s="1" t="s">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C155" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D154" s="2" t="s">
+      <c r="D155" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E154" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F154" s="17"/>
-    </row>
-    <row r="155" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A155" s="5" t="s">
+      <c r="E155" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F155" s="17"/>
+    </row>
+    <row r="156" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B155" s="6" t="s">
+      <c r="B156" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C155" s="5" t="s">
+      <c r="C156" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E155" s="16"/>
-      <c r="F155" s="20"/>
-      <c r="G155" s="5"/>
-      <c r="H155" s="6" t="s">
+      <c r="E156" s="16"/>
+      <c r="F156" s="20"/>
+      <c r="G156" s="5"/>
+      <c r="H156" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C156" s="1" t="s">
+    <row r="157" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="C157" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D156" s="2" t="s">
+      <c r="D157" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E156" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F156" s="17" t="s">
+      <c r="E157" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F157" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G156" s="1" t="s">
+      <c r="G157" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C157" s="1" t="s">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C158" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D157" s="2" t="s">
+      <c r="D158" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E157" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F157" s="17"/>
-    </row>
-    <row r="158" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A158" s="5" t="s">
+      <c r="E158" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F158" s="17"/>
+    </row>
+    <row r="159" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B158" s="6" t="s">
+      <c r="B159" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C158" s="5"/>
-      <c r="D158" s="6"/>
-      <c r="E158" s="16"/>
-      <c r="F158" s="20"/>
-      <c r="G158" s="5"/>
-      <c r="H158" s="6" t="s">
+      <c r="C159" s="5"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="16"/>
+      <c r="F159" s="20"/>
+      <c r="G159" s="5"/>
+      <c r="H159" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C159" s="1" t="s">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C160" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D159" s="2" t="s">
+      <c r="D160" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="E159" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F159" s="17"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C160" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="E160" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F160" s="17"/>
     </row>
-    <row r="161" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A161" s="5" t="s">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C161" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E161" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F161" s="17"/>
+    </row>
+    <row r="162" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B161" s="6" t="s">
+      <c r="B162" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C161" s="5"/>
-      <c r="D161" s="6"/>
-      <c r="E161" s="16"/>
-      <c r="F161" s="20"/>
-      <c r="G161" s="5"/>
-      <c r="H161" s="6" t="s">
+      <c r="C162" s="5"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="16"/>
+      <c r="F162" s="20"/>
+      <c r="G162" s="5"/>
+      <c r="H162" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C162" s="1" t="s">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C163" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D162" s="2" t="s">
+      <c r="D163" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E162" s="8" t="s">
+      <c r="E163" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F162" s="17"/>
-    </row>
-    <row r="163" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A163" s="5" t="s">
+      <c r="F163" s="17"/>
+    </row>
+    <row r="164" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B163" s="6" t="s">
+      <c r="B164" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C163" s="5"/>
-      <c r="D163" s="6"/>
-      <c r="E163" s="16"/>
-      <c r="F163" s="20"/>
-      <c r="G163" s="5"/>
-      <c r="H163" s="6" t="s">
+      <c r="C164" s="5"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="16"/>
+      <c r="F164" s="20"/>
+      <c r="G164" s="5"/>
+      <c r="H164" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C164" s="1" t="s">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C165" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D164" s="2" t="s">
+      <c r="D165" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E164" s="8" t="s">
+      <c r="E165" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F164" s="17"/>
-    </row>
-    <row r="165" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A165" s="5" t="s">
+      <c r="F165" s="17"/>
+    </row>
+    <row r="166" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B165" s="6" t="s">
+      <c r="B166" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C165" s="5"/>
-      <c r="D165" s="6"/>
-      <c r="E165" s="16"/>
-      <c r="F165" s="20"/>
-      <c r="G165" s="5"/>
-      <c r="H165" s="6" t="s">
+      <c r="C166" s="5"/>
+      <c r="D166" s="6"/>
+      <c r="E166" s="16"/>
+      <c r="F166" s="20"/>
+      <c r="G166" s="5"/>
+      <c r="H166" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C166" s="1" t="s">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C167" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D166" s="2" t="s">
+      <c r="D167" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E166" s="8" t="s">
+      <c r="E167" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F166" s="17"/>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A167" s="5" t="s">
+      <c r="F167" s="17"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B167" s="6" t="s">
+      <c r="B168" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C167" s="5"/>
-      <c r="D167" s="6"/>
-      <c r="E167" s="16"/>
-      <c r="F167" s="20"/>
-      <c r="G167" s="5"/>
-      <c r="H167" s="6" t="s">
+      <c r="C168" s="5"/>
+      <c r="D168" s="6"/>
+      <c r="E168" s="16"/>
+      <c r="F168" s="20"/>
+      <c r="G168" s="5"/>
+      <c r="H168" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C168" s="1" t="s">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C169" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D168" s="2" t="s">
+      <c r="D169" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E168" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F168" s="17"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C169" s="1" t="s">
+      <c r="E169" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F169" s="17"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C170" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D169" s="2" t="s">
+      <c r="D170" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E169" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F169" s="22" t="s">
+      <c r="E170" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F170" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G169" s="3" t="s">
+      <c r="G170" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="5" t="s">
+    <row r="171" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="B170" s="5" t="s">
+      <c r="B171" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="H170" s="6" t="s">
+      <c r="H171" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C171" s="1" t="s">
+    <row r="172" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C172" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D171" s="2" t="s">
+      <c r="D172" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="E171" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F171" s="22"/>
-      <c r="G171" s="3"/>
-    </row>
-    <row r="172" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C172" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D172" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F172" s="22" t="s">
+      <c r="F172" s="22"/>
+      <c r="G172" s="3"/>
+    </row>
+    <row r="173" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C173" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E173" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F173" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G172" s="3" t="s">
+      <c r="G173" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A173" s="5" t="s">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B173" s="6" t="s">
+      <c r="B174" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C173" s="5"/>
-      <c r="D173" s="6"/>
-      <c r="E173" s="16"/>
-      <c r="F173" s="20"/>
-      <c r="G173" s="5"/>
-      <c r="H173" s="6" t="s">
+      <c r="C174" s="5"/>
+      <c r="D174" s="6"/>
+      <c r="E174" s="16"/>
+      <c r="F174" s="20"/>
+      <c r="G174" s="5"/>
+      <c r="H174" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C174" s="1" t="s">
+    <row r="175" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C175" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D174" s="2" t="s">
+      <c r="D175" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E174" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F174" s="17"/>
-    </row>
-    <row r="175" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C175" s="1" t="s">
+      <c r="E175" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F175" s="17"/>
+    </row>
+    <row r="176" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C176" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D175" s="2" t="s">
+      <c r="D176" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E175" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F175" s="22" t="s">
+      <c r="E176" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F176" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G175" s="3" t="s">
+      <c r="G176" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A176" s="5" t="s">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B176" s="6" t="s">
+      <c r="B177" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C176" s="5"/>
-      <c r="D176" s="6"/>
-      <c r="E176" s="16"/>
-      <c r="F176" s="20"/>
-      <c r="G176" s="5"/>
-      <c r="H176" s="6" t="s">
+      <c r="C177" s="5"/>
+      <c r="D177" s="6"/>
+      <c r="E177" s="16"/>
+      <c r="F177" s="20"/>
+      <c r="G177" s="5"/>
+      <c r="H177" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C177" s="1" t="s">
+    <row r="178" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C178" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D177" s="2" t="s">
+      <c r="D178" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="E177" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F177" s="17"/>
-    </row>
-    <row r="178" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C178" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D178" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="E178" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F178" s="22" t="s">
+      <c r="F178" s="17"/>
+    </row>
+    <row r="179" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C179" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E179" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F179" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G178" s="3" t="s">
+      <c r="G179" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A179" s="5" t="s">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B179" s="6" t="s">
+      <c r="B180" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C179" s="5"/>
-      <c r="D179" s="6"/>
-      <c r="E179" s="16"/>
-      <c r="F179" s="20"/>
-      <c r="G179" s="5"/>
-      <c r="H179" s="6" t="s">
+      <c r="C180" s="5"/>
+      <c r="D180" s="6"/>
+      <c r="E180" s="16"/>
+      <c r="F180" s="20"/>
+      <c r="G180" s="5"/>
+      <c r="H180" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C180" s="1" t="s">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C181" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D180" s="10" t="s">
+      <c r="D181" s="10" t="s">
         <v>238</v>
-      </c>
-      <c r="E180" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F180" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G180" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C181" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D181" s="10" t="s">
-        <v>240</v>
       </c>
       <c r="E181" s="8" t="b">
         <v>1</v>
@@ -4687,12 +4693,12 @@
         <v>223</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C182" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E182" s="8" t="b">
         <v>1</v>
@@ -4704,12 +4710,12 @@
         <v>223</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C183" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E183" s="8" t="b">
         <v>1</v>
@@ -4721,463 +4727,466 @@
         <v>223</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A184" s="5" t="s">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C184" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D184" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="E184" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F184" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B184" s="6" t="s">
+      <c r="B185" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C184" s="5"/>
-      <c r="D184" s="6"/>
-      <c r="E184" s="16"/>
-      <c r="F184" s="20"/>
-      <c r="G184" s="5"/>
-      <c r="H184" s="6" t="s">
+      <c r="C185" s="5"/>
+      <c r="D185" s="6"/>
+      <c r="E185" s="16"/>
+      <c r="F185" s="20"/>
+      <c r="G185" s="5"/>
+      <c r="H185" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C185" s="1" t="s">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C186" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D185" s="2" t="s">
+      <c r="D186" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E185" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F185" s="17"/>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C186" s="1" t="s">
+      <c r="E186" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F186" s="17"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C187" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D186" s="2" t="s">
+      <c r="D187" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E186" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F186" s="17"/>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E187" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F187" s="17"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A188" s="5" t="s">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E188" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F188" s="17"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B188" s="6" t="s">
+      <c r="B189" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C188" s="5"/>
-      <c r="D188" s="6"/>
-      <c r="E188" s="16"/>
-      <c r="F188" s="20"/>
-      <c r="G188" s="5"/>
-      <c r="H188" s="6" t="s">
+      <c r="C189" s="5"/>
+      <c r="D189" s="6"/>
+      <c r="E189" s="16"/>
+      <c r="F189" s="20"/>
+      <c r="G189" s="5"/>
+      <c r="H189" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C189" s="1" t="s">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C190" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D189" s="2" t="s">
+      <c r="D190" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E189" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F189" s="17"/>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C190" s="1" t="s">
+      <c r="E190" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F190" s="17"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C191" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D190" s="2" t="s">
+      <c r="D191" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E190" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F190" s="22" t="s">
+      <c r="E191" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F191" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G190" s="3" t="s">
+      <c r="G191" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A191" s="5" t="s">
+    <row r="192" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A192" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B191" s="6" t="s">
+      <c r="B192" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C191" s="5"/>
-      <c r="D191" s="6"/>
-      <c r="E191" s="16"/>
-      <c r="F191" s="20"/>
-      <c r="G191" s="5"/>
-      <c r="H191" s="6" t="s">
+      <c r="C192" s="5"/>
+      <c r="D192" s="6"/>
+      <c r="E192" s="16"/>
+      <c r="F192" s="20"/>
+      <c r="G192" s="5"/>
+      <c r="H192" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C192" s="1" t="s">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C193" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D192" s="2" t="s">
+      <c r="D193" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="E192" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F192" s="17"/>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C193" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D193" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F193" s="22" t="s">
+      <c r="F193" s="17"/>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C194" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E194" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F194" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G193" s="3" t="s">
+      <c r="G194" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A194" s="5" t="s">
+    <row r="195" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B194" s="6" t="s">
+      <c r="B195" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="C194" s="5"/>
-      <c r="D194" s="6"/>
-      <c r="E194" s="16"/>
-      <c r="F194" s="20"/>
-      <c r="G194" s="5"/>
-      <c r="H194" s="6" t="s">
+      <c r="C195" s="5"/>
+      <c r="D195" s="6"/>
+      <c r="E195" s="16"/>
+      <c r="F195" s="20"/>
+      <c r="G195" s="5"/>
+      <c r="H195" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C195" s="1" t="s">
+    <row r="196" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C196" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D195" s="2" t="s">
+      <c r="D196" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="E195" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F195" s="17"/>
-    </row>
-    <row r="196" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C196" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D196" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F196" s="22" t="s">
+      <c r="F196" s="17"/>
+    </row>
+    <row r="197" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C197" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F197" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G196" s="3" t="s">
+      <c r="G197" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="197" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A197" s="5" t="s">
+    <row r="198" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B197" s="6" t="s">
+      <c r="B198" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="H197" s="6" t="s">
+      <c r="H198" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C198" s="1" t="s">
+    <row r="199" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C199" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D198" s="2" t="s">
+      <c r="D199" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="E198" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F198" s="22"/>
-      <c r="G198" s="3"/>
-    </row>
-    <row r="199" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C199" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F199" s="22" t="s">
+      <c r="F199" s="22"/>
+      <c r="G199" s="3"/>
+    </row>
+    <row r="200" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C200" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E200" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F200" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G199" s="3" t="s">
+      <c r="G200" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A200" s="5" t="s">
+    <row r="201" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B200" s="6" t="s">
+      <c r="B201" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C200" s="5"/>
-      <c r="D200" s="6"/>
-      <c r="E200" s="16"/>
-      <c r="F200" s="20"/>
-      <c r="G200" s="5"/>
-      <c r="H200" s="6" t="s">
+      <c r="C201" s="5"/>
+      <c r="D201" s="6"/>
+      <c r="E201" s="16"/>
+      <c r="F201" s="20"/>
+      <c r="G201" s="5"/>
+      <c r="H201" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C201" s="1" t="s">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C202" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D201" s="2" t="s">
+      <c r="D202" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E201" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F201" s="17"/>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C202" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E202" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F202" s="17"/>
     </row>
-    <row r="203" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A203" s="5" t="s">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C203" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E203" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F203" s="17"/>
+    </row>
+    <row r="204" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B203" s="6" t="s">
+      <c r="B204" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C203" s="5"/>
-      <c r="D203" s="6"/>
-      <c r="E203" s="16"/>
-      <c r="F203" s="20"/>
-      <c r="G203" s="5"/>
-      <c r="H203" s="6" t="s">
+      <c r="C204" s="5"/>
+      <c r="D204" s="6"/>
+      <c r="E204" s="16"/>
+      <c r="F204" s="20"/>
+      <c r="G204" s="5"/>
+      <c r="H204" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C204" s="1" t="s">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C205" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D204" s="2" t="s">
+      <c r="D205" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E204" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F204" s="17" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C205" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E205" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F205" s="17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C206" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E206" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F206" s="17" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A206" s="5" t="s">
+    <row r="207" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B206" s="6" t="s">
+      <c r="B207" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="C206" s="5"/>
-      <c r="D206" s="6"/>
-      <c r="E206" s="16"/>
-      <c r="F206" s="20"/>
-      <c r="G206" s="5"/>
-      <c r="H206" s="6" t="s">
+      <c r="C207" s="5"/>
+      <c r="D207" s="6"/>
+      <c r="E207" s="16"/>
+      <c r="F207" s="20"/>
+      <c r="G207" s="5"/>
+      <c r="H207" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C207" s="1" t="s">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C208" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D207" s="2" t="s">
+      <c r="D208" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E207" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F207" s="17"/>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C208" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D208" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E208" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F208" s="17"/>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A209" s="5" t="s">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C209" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E209" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F209" s="17"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="B209" s="6" t="s">
+      <c r="B210" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C209" s="5"/>
-      <c r="D209" s="6"/>
-      <c r="E209" s="16"/>
-      <c r="F209" s="20"/>
-      <c r="G209" s="5"/>
-      <c r="H209" s="6" t="s">
+      <c r="C210" s="5"/>
+      <c r="D210" s="6"/>
+      <c r="E210" s="16"/>
+      <c r="F210" s="20"/>
+      <c r="G210" s="5"/>
+      <c r="H210" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C210" s="1" t="s">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C211" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D210" s="2" t="s">
+      <c r="D211" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E210" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F210" s="17"/>
-    </row>
-    <row r="211" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C211" s="1" t="s">
+      <c r="E211" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F211" s="17"/>
+    </row>
+    <row r="212" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C212" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D211" s="2" t="s">
+      <c r="D212" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E211" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F211" s="17"/>
-    </row>
-    <row r="212" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A212" s="5" t="s">
+      <c r="E212" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F212" s="17"/>
+    </row>
+    <row r="213" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A213" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B212" s="6" t="s">
+      <c r="B213" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="C212" s="5"/>
-      <c r="D212" s="13"/>
-      <c r="E212" s="16"/>
-      <c r="F212" s="20"/>
-      <c r="G212" s="14"/>
-      <c r="H212" s="6" t="s">
+      <c r="C213" s="5"/>
+      <c r="D213" s="13"/>
+      <c r="E213" s="16"/>
+      <c r="F213" s="20"/>
+      <c r="G213" s="14"/>
+      <c r="H213" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C213" s="1" t="s">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C214" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D213" s="2" t="s">
+      <c r="D214" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E213" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F213" s="17"/>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C214" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D214" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E214" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F214" s="17"/>
     </row>
-    <row r="215" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="6" t="s">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C215" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E215" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F215" s="17"/>
+    </row>
+    <row r="216" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A216" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B215" s="6" t="s">
+      <c r="B216" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="C215" s="6"/>
-      <c r="D215" s="6"/>
-      <c r="E215" s="6"/>
-      <c r="F215" s="6"/>
-      <c r="G215" s="6"/>
-      <c r="H215" s="6"/>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C216" s="2" t="s">
+      <c r="C216" s="6"/>
+      <c r="D216" s="6"/>
+      <c r="E216" s="6"/>
+      <c r="F216" s="6"/>
+      <c r="G216" s="6"/>
+      <c r="H216" s="6"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C217" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E216" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H216" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C217" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>292</v>
@@ -5189,141 +5198,155 @@
         <v>286</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C218" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E218" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H218" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="219" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="6" t="s">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C219" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E219" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H219" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B219" s="6" t="s">
+      <c r="B220" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C219" s="6"/>
-      <c r="D219" s="6"/>
-      <c r="E219" s="6"/>
-      <c r="F219" s="6"/>
-      <c r="G219" s="6"/>
-      <c r="H219" s="6"/>
-    </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C220" s="2" t="s">
+      <c r="C220" s="6"/>
+      <c r="D220" s="6"/>
+      <c r="E220" s="6"/>
+      <c r="F220" s="6"/>
+      <c r="G220" s="6"/>
+      <c r="H220" s="6"/>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C221" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D220" s="2" t="s">
+      <c r="D221" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="221" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C221" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="222" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="6" t="s">
+    <row r="222" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C222" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B222" s="6" t="s">
+      <c r="B223" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="C222" s="6"/>
-      <c r="D222" s="6"/>
-      <c r="E222" s="6"/>
-      <c r="F222" s="6"/>
-      <c r="G222" s="6"/>
-      <c r="H222" s="6"/>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C223" s="2" t="s">
+      <c r="C223" s="6"/>
+      <c r="D223" s="6"/>
+      <c r="E223" s="6"/>
+      <c r="F223" s="6"/>
+      <c r="G223" s="6"/>
+      <c r="H223" s="6"/>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C224" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D223" s="2" t="s">
+      <c r="D224" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="224" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C224" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D224" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="E224" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="225" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="6" t="s">
+    <row r="225" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C225" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B225" s="6" t="s">
+      <c r="B226" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="C225" s="6"/>
-      <c r="D225" s="6"/>
-      <c r="E225" s="6"/>
-      <c r="F225" s="6"/>
-      <c r="G225" s="6"/>
-      <c r="H225" s="6"/>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C226" s="2" t="s">
+      <c r="C226" s="6"/>
+      <c r="D226" s="6"/>
+      <c r="E226" s="6"/>
+      <c r="F226" s="6"/>
+      <c r="G226" s="6"/>
+      <c r="H226" s="6"/>
+    </row>
+    <row r="227" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C227" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D226" s="2" t="s">
+      <c r="D227" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C227" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D227" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="E227" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="228" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="6"/>
-      <c r="B228" s="6"/>
-      <c r="C228" s="6"/>
-      <c r="D228" s="6"/>
-      <c r="E228" s="6"/>
-      <c r="F228" s="6"/>
-      <c r="G228" s="6"/>
-      <c r="H228" s="6"/>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C228" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="6"/>
+      <c r="B229" s="6"/>
+      <c r="C229" s="6"/>
+      <c r="D229" s="6"/>
+      <c r="E229" s="6"/>
+      <c r="F229" s="6"/>
+      <c r="G229" s="6"/>
+      <c r="H229" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H214" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <conditionalFormatting sqref="E3:E8 E153:E154 E156:E157 E159:E160 E162 E164 E166 E168:E169 E174:E175 E180:E183 E185:E187 E189:E190 E201:E202 E204:E205 E207:E208 E210:E211 E213:E214 E192:E193 E195:E196 E198:E199 E171:E172 E177:E178">
+  <autoFilter ref="A1:H215" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <conditionalFormatting sqref="E3:E8 E154:E155 E157:E158 E160:E161 E163 E165 E167 E169:E170 E175:E176 E181:E184 E186:E188 E190:E191 E202:E203 E205:E206 E208:E209 E211:E212 E214:E215 E193:E194 E196:E197 E199:E200 E172:E173 E178:E179">
     <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5334,7 +5357,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E131:E134 E136:E139 E141:E143 E145:E147 E149:E151">
+  <conditionalFormatting sqref="E132:E135 E137:E140 E142:E144 E146:E148 E150:E152">
     <cfRule type="cellIs" dxfId="59" priority="13" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5389,7 +5412,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E62">
+  <conditionalFormatting sqref="E58:E63">
     <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5400,7 +5423,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64:E66">
+  <conditionalFormatting sqref="E65:E67">
     <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5411,7 +5434,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68:E73">
+  <conditionalFormatting sqref="E69:E74">
     <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5422,7 +5445,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75:E77">
+  <conditionalFormatting sqref="E76:E78">
     <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5433,7 +5456,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E79:E80">
+  <conditionalFormatting sqref="E80:E81">
     <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5444,7 +5467,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82:E87">
+  <conditionalFormatting sqref="E83:E88">
     <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5455,7 +5478,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E89:E93">
+  <conditionalFormatting sqref="E90:E94">
     <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5466,7 +5489,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96:E102">
+  <conditionalFormatting sqref="E97:E103">
     <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5477,7 +5500,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95">
+  <conditionalFormatting sqref="E96">
     <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5488,7 +5511,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E104:E108">
+  <conditionalFormatting sqref="E105:E109">
     <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5499,7 +5522,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E110:E113">
+  <conditionalFormatting sqref="E111:E114">
     <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5510,7 +5533,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E115:E119">
+  <conditionalFormatting sqref="E116:E120">
     <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5521,7 +5544,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E121:E124 E126:E129">
+  <conditionalFormatting sqref="E122:E125 E127:E130">
     <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5532,7 +5555,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E218">
+  <conditionalFormatting sqref="E219">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5543,7 +5566,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E216:E217">
+  <conditionalFormatting sqref="E217:E218">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5585,31 +5608,31 @@
     <hyperlink ref="G45:G47" r:id="rId28" display="https://github.com/NREL/openstudio-standards/blob/nrcan/lib/openstudio-standards/standards/necb/NECB2011/demand_controlled_ventilation.md" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
     <hyperlink ref="G53" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
     <hyperlink ref="G56" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G82" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G89" r:id="rId32" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G95" r:id="rId33" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G104" r:id="rId34" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G110" r:id="rId35" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G115" r:id="rId36" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="G121" r:id="rId37" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="G126" r:id="rId38" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="G131" r:id="rId39" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="G136" r:id="rId40" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="G141" r:id="rId41" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="G145" r:id="rId42" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="G149" r:id="rId43" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="G169" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="G175" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="G178" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="G180" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="G181" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="G182" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="G183" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="G172" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="G190" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="G193" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="G196" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="G199" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="G83" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G90" r:id="rId32" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G96" r:id="rId33" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G105" r:id="rId34" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G111" r:id="rId35" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G116" r:id="rId36" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G122" r:id="rId37" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="G127" r:id="rId38" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="G132" r:id="rId39" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="G137" r:id="rId40" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="G142" r:id="rId41" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="G146" r:id="rId42" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="G150" r:id="rId43" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="G170" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="G176" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="G179" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="G181" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="G182" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="G183" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="G184" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="G173" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="G191" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="G194" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="G197" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="G200" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
     <hyperlink ref="G6" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Including none option for daylighting controls in BTAPOptions.xlsx and in input.yml example files.
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khaddad\btap_batch\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckirney\projects\btap_batch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550534D0-D05F-4BB2-9EDA-A3512525D3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DE7628-FDA2-4F6A-946A-4C37C7608B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="15" windowWidth="26055" windowHeight="15015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadME" sheetId="2" r:id="rId1"/>
     <sheet name="BTAPOptions" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BTAPOptions!$A$1:$H$215</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BTAPOptions!$A$1:$H$216</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="321">
   <si>
     <t>Variable</t>
   </si>
@@ -989,6 +989,12 @@
   </si>
   <si>
     <t>The central-ground source heat pump (size = 40% of peak heating load) and boiler (size = 60% of peak heating load) are used to meet the heating demand. The cooling demand is met using a water-cooled chiller (size = 40% of peak cooling load) and a air-cooled chiller (size = 60% of peak cooling load). The heat pump and water-cooled chiller are connected to a ground-loop heat exchanger.</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Do no add daylighting sensors.</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1193,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2122,11 +2128,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H229"/>
+  <dimension ref="A1:H230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,401 +2978,402 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E57" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="17"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="6" t="s">
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="1" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E58" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="17" t="s">
+      <c r="E59" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="C59" s="25" t="s">
+    <row r="60" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C60" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="D59" s="26" t="s">
+      <c r="D60" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="E59" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="17" t="s">
+      <c r="E60" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="C60" s="24" t="s">
+    <row r="61" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="C61" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D60" s="23" t="s">
+      <c r="D61" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="17" t="s">
+      <c r="E61" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="17" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="C61" s="27" t="s">
+    <row r="62" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C62" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D61" s="26" t="s">
+      <c r="D62" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="E61" s="8" t="b">
+      <c r="E62" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C63" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E63" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C64" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="E64" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F61" s="17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C62" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="D62" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="E62" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="C63" s="24" t="s">
-        <v>316</v>
-      </c>
-      <c r="D63" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="E63" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="17" t="s">
+      <c r="F64" s="17" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B65" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="1" t="s">
+      <c r="C65" s="5"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C65" s="1" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E65" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="17"/>
-    </row>
-    <row r="66" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C66" s="1" t="s">
+      <c r="E66" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="17"/>
+    </row>
+    <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E66" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="17" t="s">
+      <c r="E67" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="C67" s="1" t="s">
+    <row r="68" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E67" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="17" t="s">
+      <c r="E68" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B69" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="6" t="s">
+      <c r="C69" s="5"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="6" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C69" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E69" s="8" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E70" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E70" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="17"/>
-    </row>
-    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C71" s="1" t="s">
+      <c r="E71" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="17"/>
+    </row>
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E71" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="17" t="s">
+      <c r="E72" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="17" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C72" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E72" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="17"/>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E73" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="17"/>
+    </row>
+    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E73" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="17"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C74" s="1" t="s">
+      <c r="E74" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="17"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E74" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="17"/>
-    </row>
-    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+      <c r="E75" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="17"/>
+    </row>
+    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B76" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="6" t="s">
+      <c r="C76" s="5"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C76" s="1" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C77" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E76" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="17" t="s">
+      <c r="E77" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="17" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C77" s="1" t="s">
+    <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C78" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E77" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="17" t="s">
+      <c r="E78" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C78" s="1" t="s">
+    <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C79" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E78" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="17" t="s">
+      <c r="E79" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" s="17" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B80" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="6" t="s">
+      <c r="C80" s="5"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="C80" s="1" t="s">
+    <row r="81" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C81" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E80" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="17" t="s">
+      <c r="E81" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="17" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="C81" s="1" t="s">
+    <row r="82" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E81" s="8" t="b">
+      <c r="E82" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F81" s="17" t="s">
+      <c r="F82" s="17" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B83" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="6" t="s">
+      <c r="C83" s="5"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C83" s="7" t="s">
+    <row r="84" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C84" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E83" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="17" t="s">
+      <c r="E84" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G83" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C84" s="1">
-        <v>0.314</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E84" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="17"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
-        <v>0.27800000000000002</v>
+        <v>0.314</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>171</v>
@@ -3378,7 +3385,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
-        <v>0.247</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>171</v>
@@ -3390,7 +3397,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
-        <v>0.21</v>
+        <v>0.247</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>171</v>
@@ -3402,7 +3409,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
-        <v>0.183</v>
+        <v>0.21</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>171</v>
@@ -3413,53 +3420,53 @@
       <c r="F88" s="17"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+      <c r="C89" s="1">
+        <v>0.183</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E89" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="17"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B90" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="6"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="6" t="s">
+      <c r="C90" s="5"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C90" s="7" t="s">
+    <row r="91" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C91" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D91" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E90" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="17" t="s">
+      <c r="E91" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G90" s="21" t="s">
+      <c r="G91" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C91" s="1">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E91" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="17"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
-        <v>0.183</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>171</v>
@@ -3471,7 +3478,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
-        <v>0.16200000000000001</v>
+        <v>0.183</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>171</v>
@@ -3483,7 +3490,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
-        <v>0.14199999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>171</v>
@@ -3494,53 +3501,53 @@
       <c r="F94" s="17"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+      <c r="C95" s="1">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E95" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="17"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B96" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C95" s="5"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="6"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="6" t="s">
+      <c r="C96" s="5"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C96" s="7" t="s">
+    <row r="97" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C97" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E96" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="17" t="s">
+      <c r="E97" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G96" s="21" t="s">
+      <c r="G97" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C97" s="1">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E97" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="17"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C98" s="1">
-        <v>0.193</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>171</v>
@@ -3552,7 +3559,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C99" s="1">
-        <v>0.183</v>
+        <v>0.193</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>171</v>
@@ -3564,7 +3571,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
-        <v>0.16200000000000001</v>
+        <v>0.183</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>171</v>
@@ -3576,7 +3583,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
-        <v>0.14199999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>171</v>
@@ -3588,7 +3595,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C102" s="1">
-        <v>0.13800000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>171</v>
@@ -3600,7 +3607,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C103" s="1">
-        <v>0.121</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>171</v>
@@ -3611,53 +3618,53 @@
       <c r="F103" s="17"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+      <c r="C104" s="1">
+        <v>0.121</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E104" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="17"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B105" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="6" t="s">
+      <c r="C105" s="5"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C105" s="1" t="s">
+    <row r="106" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C106" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E105" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" s="17" t="s">
+      <c r="E106" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G105" s="21" t="s">
+      <c r="G106" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C106" s="1">
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E106" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F106" s="17"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C107" s="1">
-        <v>0.379</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>171</v>
@@ -3669,7 +3676,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C108" s="1">
-        <v>0.28399999999999997</v>
+        <v>0.379</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>171</v>
@@ -3681,7 +3688,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C109" s="1">
-        <v>0.21</v>
+        <v>0.28399999999999997</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>171</v>
@@ -3691,54 +3698,54 @@
       </c>
       <c r="F109" s="17"/>
     </row>
-    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C110" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E110" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" s="17"/>
+    </row>
+    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B110" s="6" t="s">
+      <c r="B111" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C110" s="5"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="6"/>
-      <c r="G110" s="5"/>
-      <c r="H110" s="6" t="s">
+      <c r="C111" s="5"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C111" s="1" t="s">
+    <row r="112" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C112" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E111" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" s="17" t="s">
+      <c r="E112" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G111" s="21" t="s">
+      <c r="G112" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C112" s="1">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E112" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F112" s="17"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C113" s="1">
-        <v>0.379</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>171</v>
@@ -3749,59 +3756,59 @@
       <c r="F113" s="17"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C114" s="1">
+        <v>0.379</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="E114" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F114" s="17"/>
     </row>
-    <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E115" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" s="17"/>
+    </row>
+    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B115" s="6" t="s">
+      <c r="B116" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C115" s="5"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="6"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="6" t="s">
+      <c r="C116" s="5"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C116" s="7" t="s">
+    <row r="117" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C117" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D117" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E116" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" s="17" t="s">
+      <c r="E117" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G116" s="21" t="s">
+      <c r="G117" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C117" s="1">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C118" s="1">
         <v>0.56799999999999995</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E117" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F117" s="17"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C118" s="4">
-        <v>0.379</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>171</v>
@@ -3812,8 +3819,8 @@
       <c r="F118" s="17"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C119" s="1">
-        <v>0.28399999999999997</v>
+      <c r="C119" s="4">
+        <v>0.379</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>171</v>
@@ -3825,7 +3832,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C120" s="1">
-        <v>0.21</v>
+        <v>0.28399999999999997</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>171</v>
@@ -3835,54 +3842,54 @@
       </c>
       <c r="F120" s="17"/>
     </row>
-    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C121" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E121" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="17"/>
+    </row>
+    <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B121" s="6" t="s">
+      <c r="B122" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C121" s="5"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="5"/>
-      <c r="H121" s="6" t="s">
+      <c r="C122" s="5"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="5"/>
+      <c r="H122" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C122" s="1" t="s">
+    <row r="123" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C123" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D123" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E122" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F122" s="17" t="s">
+      <c r="E123" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F123" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G122" s="21" t="s">
+      <c r="G123" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C123" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E123" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F123" s="17"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C124" s="1">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>171</v>
@@ -3894,7 +3901,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C125" s="1">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>171</v>
@@ -3904,53 +3911,53 @@
       </c>
       <c r="F125" s="17"/>
     </row>
-    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C126" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E126" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F126" s="17"/>
+    </row>
+    <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="B127" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C126" s="5"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="15"/>
-      <c r="F126" s="19"/>
-      <c r="H126" s="6" t="s">
+      <c r="C127" s="5"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="15"/>
+      <c r="F127" s="19"/>
+      <c r="H127" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C127" s="1" t="s">
+    <row r="128" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C128" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D128" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E127" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F127" s="17" t="s">
+      <c r="E128" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F128" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G127" s="21" t="s">
+      <c r="G128" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C128" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E128" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F128" s="17"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C129" s="1">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>171</v>
@@ -3962,7 +3969,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C130" s="1">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>171</v>
@@ -3972,54 +3979,54 @@
       </c>
       <c r="F130" s="17"/>
     </row>
-    <row r="131" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C131" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E131" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F131" s="17"/>
+    </row>
+    <row r="132" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B131" s="6" t="s">
+      <c r="B132" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C131" s="5"/>
-      <c r="D131" s="6"/>
-      <c r="E131" s="5"/>
-      <c r="F131" s="6"/>
-      <c r="G131" s="5"/>
-      <c r="H131" s="6" t="s">
+      <c r="C132" s="5"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C132" s="1" t="s">
+    <row r="133" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C133" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D132" s="2" t="s">
+      <c r="D133" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E132" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F132" s="17" t="s">
+      <c r="E133" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F133" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G132" s="21" t="s">
+      <c r="G133" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C133" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E133" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F133" s="17"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C134" s="1">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>171</v>
@@ -4031,7 +4038,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C135" s="1">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>171</v>
@@ -4042,53 +4049,53 @@
       <c r="F135" s="17"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" s="5" t="s">
+      <c r="C136" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E136" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F136" s="17"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="B137" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C136" s="5"/>
-      <c r="D136" s="13"/>
-      <c r="E136" s="15"/>
-      <c r="F136" s="19"/>
-      <c r="G136" s="14"/>
-      <c r="H136" s="6" t="s">
+      <c r="C137" s="5"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="15"/>
+      <c r="F137" s="19"/>
+      <c r="G137" s="14"/>
+      <c r="H137" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C137" s="1" t="s">
+    <row r="138" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C138" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D137" s="2" t="s">
+      <c r="D138" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E137" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F137" s="17" t="s">
+      <c r="E138" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F138" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G137" s="21" t="s">
+      <c r="G138" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C138" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E138" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F138" s="17"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C139" s="1">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>171</v>
@@ -4100,7 +4107,7 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C140" s="1">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>171</v>
@@ -4110,108 +4117,108 @@
       </c>
       <c r="F140" s="17"/>
     </row>
-    <row r="141" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C141" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E141" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F141" s="17"/>
+    </row>
+    <row r="142" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B141" s="6" t="s">
+      <c r="B142" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C141" s="5"/>
-      <c r="D141" s="6"/>
-      <c r="E141" s="15"/>
-      <c r="F141" s="19"/>
-      <c r="G141" s="5"/>
-      <c r="H141" s="6" t="s">
+      <c r="C142" s="5"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="15"/>
+      <c r="F142" s="19"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C142" s="1" t="s">
+    <row r="143" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C143" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D142" s="2" t="s">
+      <c r="D143" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E142" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F142" s="17" t="s">
+      <c r="E143" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F143" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G142" s="21" t="s">
+      <c r="G143" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C143" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="E143" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F143" s="17"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C144" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E144" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F144" s="17"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C145" s="1">
         <v>0.9</v>
       </c>
-      <c r="D144" s="2" t="s">
+      <c r="D145" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E144" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F144" s="17"/>
-    </row>
-    <row r="145" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
+      <c r="E145" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F145" s="17"/>
+    </row>
+    <row r="146" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B145" s="6" t="s">
+      <c r="B146" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C145" s="5"/>
-      <c r="D145" s="6"/>
-      <c r="E145" s="16"/>
-      <c r="F145" s="20"/>
-      <c r="G145" s="5"/>
-      <c r="H145" s="6" t="s">
+      <c r="C146" s="5"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="16"/>
+      <c r="F146" s="20"/>
+      <c r="G146" s="5"/>
+      <c r="H146" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C146" s="1" t="s">
+    <row r="147" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C147" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D146" s="2" t="s">
+      <c r="D147" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E146" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F146" s="17" t="s">
+      <c r="E147" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F147" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G146" s="21" t="s">
+      <c r="G147" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C147" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E147" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F147" s="17"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C148" s="1">
-        <v>0.9</v>
+        <v>0.05</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>171</v>
@@ -4222,483 +4229,478 @@
       <c r="F148" s="17"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
+      <c r="C149" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E149" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F149" s="17"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B149" s="6" t="s">
+      <c r="B150" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C149" s="5"/>
-      <c r="D149" s="6"/>
-      <c r="E149" s="16"/>
-      <c r="F149" s="20"/>
-      <c r="G149" s="5"/>
-      <c r="H149" s="6" t="s">
+      <c r="C150" s="5"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="16"/>
+      <c r="F150" s="20"/>
+      <c r="G150" s="5"/>
+      <c r="H150" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C150" s="1" t="s">
+    <row r="151" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C151" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E150" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F150" s="17" t="s">
+      <c r="E151" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F151" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G150" s="21" t="s">
+      <c r="G151" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C151" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="E151" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F151" s="17"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C152" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E152" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F152" s="17"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C153" s="1">
         <v>0.9</v>
       </c>
-      <c r="E152" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F152" s="17"/>
-    </row>
-    <row r="153" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="5" t="s">
+      <c r="E153" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F153" s="17"/>
+    </row>
+    <row r="154" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B153" s="6" t="s">
+      <c r="B154" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C153" s="5"/>
-      <c r="D153" s="6"/>
-      <c r="E153" s="16"/>
-      <c r="F153" s="20"/>
-      <c r="G153" s="5"/>
-      <c r="H153" s="6" t="s">
+      <c r="C154" s="5"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="16"/>
+      <c r="F154" s="20"/>
+      <c r="G154" s="5"/>
+      <c r="H154" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="C154" s="1" t="s">
+    <row r="155" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="C155" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D154" s="2" t="s">
+      <c r="D155" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E154" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F154" s="17" t="s">
+      <c r="E155" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F155" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="G154" s="1" t="s">
+      <c r="G155" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C155" s="1" t="s">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C156" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D155" s="2" t="s">
+      <c r="D156" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E155" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F155" s="17"/>
-    </row>
-    <row r="156" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
+      <c r="E156" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F156" s="17"/>
+    </row>
+    <row r="157" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B156" s="6" t="s">
+      <c r="B157" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C156" s="5" t="s">
+      <c r="C157" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E156" s="16"/>
-      <c r="F156" s="20"/>
-      <c r="G156" s="5"/>
-      <c r="H156" s="6" t="s">
+      <c r="E157" s="16"/>
+      <c r="F157" s="20"/>
+      <c r="G157" s="5"/>
+      <c r="H157" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="C157" s="1" t="s">
+    <row r="158" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="C158" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D157" s="2" t="s">
+      <c r="D158" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E157" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F157" s="17" t="s">
+      <c r="E158" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F158" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G157" s="1" t="s">
+      <c r="G158" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C158" s="1" t="s">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C159" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D158" s="2" t="s">
+      <c r="D159" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E158" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F158" s="17"/>
-    </row>
-    <row r="159" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
+      <c r="E159" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F159" s="17"/>
+    </row>
+    <row r="160" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B159" s="6" t="s">
+      <c r="B160" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C159" s="5"/>
-      <c r="D159" s="6"/>
-      <c r="E159" s="16"/>
-      <c r="F159" s="20"/>
-      <c r="G159" s="5"/>
-      <c r="H159" s="6" t="s">
+      <c r="C160" s="5"/>
+      <c r="D160" s="6"/>
+      <c r="E160" s="16"/>
+      <c r="F160" s="20"/>
+      <c r="G160" s="5"/>
+      <c r="H160" s="6" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C160" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E160" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F160" s="17"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C161" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F161" s="17"/>
     </row>
-    <row r="162" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C162" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E162" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F162" s="17"/>
+    </row>
+    <row r="163" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A163" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B162" s="6" t="s">
+      <c r="B163" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C162" s="5"/>
-      <c r="D162" s="6"/>
-      <c r="E162" s="16"/>
-      <c r="F162" s="20"/>
-      <c r="G162" s="5"/>
-      <c r="H162" s="6" t="s">
+      <c r="C163" s="5"/>
+      <c r="D163" s="6"/>
+      <c r="E163" s="16"/>
+      <c r="F163" s="20"/>
+      <c r="G163" s="5"/>
+      <c r="H163" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C163" s="1" t="s">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C164" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D163" s="2" t="s">
+      <c r="D164" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E163" s="8" t="s">
+      <c r="E164" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F163" s="17"/>
-    </row>
-    <row r="164" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
+      <c r="F164" s="17"/>
+    </row>
+    <row r="165" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B164" s="6" t="s">
+      <c r="B165" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C164" s="5"/>
-      <c r="D164" s="6"/>
-      <c r="E164" s="16"/>
-      <c r="F164" s="20"/>
-      <c r="G164" s="5"/>
-      <c r="H164" s="6" t="s">
+      <c r="C165" s="5"/>
+      <c r="D165" s="6"/>
+      <c r="E165" s="16"/>
+      <c r="F165" s="20"/>
+      <c r="G165" s="5"/>
+      <c r="H165" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C165" s="1" t="s">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C166" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D165" s="2" t="s">
+      <c r="D166" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E165" s="8" t="s">
+      <c r="E166" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F165" s="17"/>
-    </row>
-    <row r="166" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
+      <c r="F166" s="17"/>
+    </row>
+    <row r="167" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B166" s="6" t="s">
+      <c r="B167" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C166" s="5"/>
-      <c r="D166" s="6"/>
-      <c r="E166" s="16"/>
-      <c r="F166" s="20"/>
-      <c r="G166" s="5"/>
-      <c r="H166" s="6" t="s">
+      <c r="C167" s="5"/>
+      <c r="D167" s="6"/>
+      <c r="E167" s="16"/>
+      <c r="F167" s="20"/>
+      <c r="G167" s="5"/>
+      <c r="H167" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C167" s="1" t="s">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C168" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D167" s="2" t="s">
+      <c r="D168" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E167" s="8" t="s">
+      <c r="E168" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F167" s="17"/>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A168" s="5" t="s">
+      <c r="F168" s="17"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B168" s="6" t="s">
+      <c r="B169" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C168" s="5"/>
-      <c r="D168" s="6"/>
-      <c r="E168" s="16"/>
-      <c r="F168" s="20"/>
-      <c r="G168" s="5"/>
-      <c r="H168" s="6" t="s">
+      <c r="C169" s="5"/>
+      <c r="D169" s="6"/>
+      <c r="E169" s="16"/>
+      <c r="F169" s="20"/>
+      <c r="G169" s="5"/>
+      <c r="H169" s="6" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C169" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E169" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F169" s="17"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C170" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E170" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F170" s="17"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C171" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D170" s="2" t="s">
+      <c r="D171" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E170" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F170" s="22" t="s">
+      <c r="E171" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F171" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G170" s="3" t="s">
+      <c r="G171" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
+    <row r="172" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="B171" s="5" t="s">
+      <c r="B172" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="H171" s="6" t="s">
+      <c r="H172" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C172" s="1" t="s">
+    <row r="173" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C173" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D172" s="2" t="s">
+      <c r="D173" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="E172" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F172" s="22"/>
-      <c r="G172" s="3"/>
-    </row>
-    <row r="173" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C173" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D173" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="E173" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F173" s="22" t="s">
+      <c r="F173" s="22"/>
+      <c r="G173" s="3"/>
+    </row>
+    <row r="174" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C174" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E174" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F174" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G173" s="3" t="s">
+      <c r="G174" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" s="5" t="s">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B174" s="6" t="s">
+      <c r="B175" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C174" s="5"/>
-      <c r="D174" s="6"/>
-      <c r="E174" s="16"/>
-      <c r="F174" s="20"/>
-      <c r="G174" s="5"/>
-      <c r="H174" s="6" t="s">
+      <c r="C175" s="5"/>
+      <c r="D175" s="6"/>
+      <c r="E175" s="16"/>
+      <c r="F175" s="20"/>
+      <c r="G175" s="5"/>
+      <c r="H175" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C175" s="1" t="s">
+    <row r="176" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C176" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D175" s="2" t="s">
+      <c r="D176" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E175" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F175" s="17"/>
-    </row>
-    <row r="176" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C176" s="1" t="s">
+      <c r="E176" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F176" s="17"/>
+    </row>
+    <row r="177" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C177" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D176" s="2" t="s">
+      <c r="D177" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E176" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F176" s="22" t="s">
+      <c r="E177" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F177" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G176" s="3" t="s">
+      <c r="G177" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B177" s="6" t="s">
+      <c r="B178" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C177" s="5"/>
-      <c r="D177" s="6"/>
-      <c r="E177" s="16"/>
-      <c r="F177" s="20"/>
-      <c r="G177" s="5"/>
-      <c r="H177" s="6" t="s">
+      <c r="C178" s="5"/>
+      <c r="D178" s="6"/>
+      <c r="E178" s="16"/>
+      <c r="F178" s="20"/>
+      <c r="G178" s="5"/>
+      <c r="H178" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C178" s="1" t="s">
+    <row r="179" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C179" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D178" s="2" t="s">
+      <c r="D179" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="E178" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F178" s="17"/>
-    </row>
-    <row r="179" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C179" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="E179" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F179" s="22" t="s">
+      <c r="F179" s="17"/>
+    </row>
+    <row r="180" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C180" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E180" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F180" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G179" s="3" t="s">
+      <c r="G180" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A180" s="5" t="s">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B180" s="6" t="s">
+      <c r="B181" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C180" s="5"/>
-      <c r="D180" s="6"/>
-      <c r="E180" s="16"/>
-      <c r="F180" s="20"/>
-      <c r="G180" s="5"/>
-      <c r="H180" s="6" t="s">
+      <c r="C181" s="5"/>
+      <c r="D181" s="6"/>
+      <c r="E181" s="16"/>
+      <c r="F181" s="20"/>
+      <c r="G181" s="5"/>
+      <c r="H181" s="6" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C181" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D181" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="E181" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F181" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G181" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C182" s="1" t="s">
-        <v>239</v>
+        <v>84</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E182" s="8" t="b">
         <v>1</v>
@@ -4712,10 +4714,10 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C183" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E183" s="8" t="b">
         <v>1</v>
@@ -4729,10 +4731,10 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C184" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E184" s="8" t="b">
         <v>1</v>
@@ -4745,345 +4747,350 @@
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A185" s="5" t="s">
+      <c r="C185" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D185" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="E185" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F185" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B185" s="6" t="s">
+      <c r="B186" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C185" s="5"/>
-      <c r="D185" s="6"/>
-      <c r="E185" s="16"/>
-      <c r="F185" s="20"/>
-      <c r="G185" s="5"/>
-      <c r="H185" s="6" t="s">
+      <c r="C186" s="5"/>
+      <c r="D186" s="6"/>
+      <c r="E186" s="16"/>
+      <c r="F186" s="20"/>
+      <c r="G186" s="5"/>
+      <c r="H186" s="6" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C186" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E186" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F186" s="17"/>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C187" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E187" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F187" s="17"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C188" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D187" s="2" t="s">
+      <c r="D188" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E187" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F187" s="17"/>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E188" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F188" s="17"/>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A189" s="5" t="s">
+      <c r="E189" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F189" s="17"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B189" s="6" t="s">
+      <c r="B190" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C189" s="5"/>
-      <c r="D189" s="6"/>
-      <c r="E189" s="16"/>
-      <c r="F189" s="20"/>
-      <c r="G189" s="5"/>
-      <c r="H189" s="6" t="s">
+      <c r="C190" s="5"/>
+      <c r="D190" s="6"/>
+      <c r="E190" s="16"/>
+      <c r="F190" s="20"/>
+      <c r="G190" s="5"/>
+      <c r="H190" s="6" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C190" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D190" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E190" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F190" s="17"/>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C191" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E191" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F191" s="17"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C192" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D191" s="2" t="s">
+      <c r="D192" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E191" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F191" s="22" t="s">
+      <c r="E192" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F192" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G191" s="3" t="s">
+      <c r="G192" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A192" s="5" t="s">
+    <row r="193" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B192" s="6" t="s">
+      <c r="B193" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C192" s="5"/>
-      <c r="D192" s="6"/>
-      <c r="E192" s="16"/>
-      <c r="F192" s="20"/>
-      <c r="G192" s="5"/>
-      <c r="H192" s="6" t="s">
+      <c r="C193" s="5"/>
+      <c r="D193" s="6"/>
+      <c r="E193" s="16"/>
+      <c r="F193" s="20"/>
+      <c r="G193" s="5"/>
+      <c r="H193" s="6" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C193" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D193" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E193" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F193" s="17"/>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C194" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F194" s="22" t="s">
+      <c r="F194" s="17"/>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C195" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E195" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F195" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G194" s="3" t="s">
+      <c r="G195" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A195" s="5" t="s">
+    <row r="196" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B195" s="6" t="s">
+      <c r="B196" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="C195" s="5"/>
-      <c r="D195" s="6"/>
-      <c r="E195" s="16"/>
-      <c r="F195" s="20"/>
-      <c r="G195" s="5"/>
-      <c r="H195" s="6" t="s">
+      <c r="C196" s="5"/>
+      <c r="D196" s="6"/>
+      <c r="E196" s="16"/>
+      <c r="F196" s="20"/>
+      <c r="G196" s="5"/>
+      <c r="H196" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C196" s="1" t="s">
+    <row r="197" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C197" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D196" s="2" t="s">
+      <c r="D197" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="E196" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F196" s="17"/>
-    </row>
-    <row r="197" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C197" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F197" s="22" t="s">
+      <c r="F197" s="17"/>
+    </row>
+    <row r="198" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C198" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E198" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F198" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G197" s="3" t="s">
+      <c r="G198" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="198" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A198" s="5" t="s">
+    <row r="199" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B198" s="6" t="s">
+      <c r="B199" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="H198" s="6" t="s">
+      <c r="H199" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C199" s="1" t="s">
+    <row r="200" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C200" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D199" s="2" t="s">
+      <c r="D200" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="E199" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F199" s="22"/>
-      <c r="G199" s="3"/>
-    </row>
-    <row r="200" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C200" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F200" s="22" t="s">
+      <c r="F200" s="22"/>
+      <c r="G200" s="3"/>
+    </row>
+    <row r="201" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C201" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E201" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F201" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G200" s="3" t="s">
+      <c r="G201" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A201" s="5" t="s">
+    <row r="202" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A202" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B201" s="6" t="s">
+      <c r="B202" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C201" s="5"/>
-      <c r="D201" s="6"/>
-      <c r="E201" s="16"/>
-      <c r="F201" s="20"/>
-      <c r="G201" s="5"/>
-      <c r="H201" s="6" t="s">
+      <c r="C202" s="5"/>
+      <c r="D202" s="6"/>
+      <c r="E202" s="16"/>
+      <c r="F202" s="20"/>
+      <c r="G202" s="5"/>
+      <c r="H202" s="6" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C202" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E202" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F202" s="17"/>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C203" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F203" s="17"/>
     </row>
-    <row r="204" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A204" s="5" t="s">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C204" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E204" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F204" s="17"/>
+    </row>
+    <row r="205" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A205" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B204" s="6" t="s">
+      <c r="B205" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C204" s="5"/>
-      <c r="D204" s="6"/>
-      <c r="E204" s="16"/>
-      <c r="F204" s="20"/>
-      <c r="G204" s="5"/>
-      <c r="H204" s="6" t="s">
+      <c r="C205" s="5"/>
+      <c r="D205" s="6"/>
+      <c r="E205" s="16"/>
+      <c r="F205" s="20"/>
+      <c r="G205" s="5"/>
+      <c r="H205" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C205" s="1" t="s">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C206" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D205" s="2" t="s">
+      <c r="D206" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E205" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F205" s="17" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C206" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E206" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F206" s="17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C207" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E207" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F207" s="17" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A207" s="5" t="s">
+    <row r="208" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A208" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B207" s="6" t="s">
+      <c r="B208" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="C207" s="5"/>
-      <c r="D207" s="6"/>
-      <c r="E207" s="16"/>
-      <c r="F207" s="20"/>
-      <c r="G207" s="5"/>
-      <c r="H207" s="6" t="s">
+      <c r="C208" s="5"/>
+      <c r="D208" s="6"/>
+      <c r="E208" s="16"/>
+      <c r="F208" s="20"/>
+      <c r="G208" s="5"/>
+      <c r="H208" s="6" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C208" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D208" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E208" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F208" s="17"/>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C209" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E209" s="8" t="s">
         <v>29</v>
@@ -5091,116 +5098,114 @@
       <c r="F209" s="17"/>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A210" s="5" t="s">
+      <c r="C210" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E210" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F210" s="17"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="B210" s="6" t="s">
+      <c r="B211" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C210" s="5"/>
-      <c r="D210" s="6"/>
-      <c r="E210" s="16"/>
-      <c r="F210" s="20"/>
-      <c r="G210" s="5"/>
-      <c r="H210" s="6" t="s">
+      <c r="C211" s="5"/>
+      <c r="D211" s="6"/>
+      <c r="E211" s="16"/>
+      <c r="F211" s="20"/>
+      <c r="G211" s="5"/>
+      <c r="H211" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C211" s="1" t="s">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C212" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D211" s="2" t="s">
+      <c r="D212" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E211" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F211" s="17"/>
-    </row>
-    <row r="212" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C212" s="1" t="s">
+      <c r="E212" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F212" s="17"/>
+    </row>
+    <row r="213" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C213" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D212" s="2" t="s">
+      <c r="D213" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E212" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F212" s="17"/>
-    </row>
-    <row r="213" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A213" s="5" t="s">
+      <c r="E213" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F213" s="17"/>
+    </row>
+    <row r="214" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A214" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B213" s="6" t="s">
+      <c r="B214" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="C213" s="5"/>
-      <c r="D213" s="13"/>
-      <c r="E213" s="16"/>
-      <c r="F213" s="20"/>
-      <c r="G213" s="14"/>
-      <c r="H213" s="6" t="s">
+      <c r="C214" s="5"/>
+      <c r="D214" s="13"/>
+      <c r="E214" s="16"/>
+      <c r="F214" s="20"/>
+      <c r="G214" s="14"/>
+      <c r="H214" s="6" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C214" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D214" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E214" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F214" s="17"/>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C215" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E215" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F215" s="17"/>
     </row>
-    <row r="216" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A216" s="6" t="s">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C216" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E216" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F216" s="17"/>
+    </row>
+    <row r="217" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A217" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B216" s="6" t="s">
+      <c r="B217" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="C216" s="6"/>
-      <c r="D216" s="6"/>
-      <c r="E216" s="6"/>
-      <c r="F216" s="6"/>
-      <c r="G216" s="6"/>
-      <c r="H216" s="6"/>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C217" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D217" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E217" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H217" s="1" t="s">
-        <v>286</v>
-      </c>
+      <c r="C217" s="6"/>
+      <c r="D217" s="6"/>
+      <c r="E217" s="6"/>
+      <c r="F217" s="6"/>
+      <c r="G217" s="6"/>
+      <c r="H217" s="6"/>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C218" s="2" t="s">
-        <v>290</v>
+        <v>84</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>292</v>
@@ -5214,139 +5219,153 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C219" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E219" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H219" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="220" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="6" t="s">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C220" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D220" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E220" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H220" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B220" s="6" t="s">
+      <c r="B221" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C220" s="6"/>
-      <c r="D220" s="6"/>
-      <c r="E220" s="6"/>
-      <c r="F220" s="6"/>
-      <c r="G220" s="6"/>
-      <c r="H220" s="6"/>
-    </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C221" s="2" t="s">
+      <c r="C221" s="6"/>
+      <c r="D221" s="6"/>
+      <c r="E221" s="6"/>
+      <c r="F221" s="6"/>
+      <c r="G221" s="6"/>
+      <c r="H221" s="6"/>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C222" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D221" s="2" t="s">
+      <c r="D222" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="222" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="C222" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D222" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="223" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="6" t="s">
+    <row r="223" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C223" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B223" s="6" t="s">
+      <c r="B224" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="C223" s="6"/>
-      <c r="D223" s="6"/>
-      <c r="E223" s="6"/>
-      <c r="F223" s="6"/>
-      <c r="G223" s="6"/>
-      <c r="H223" s="6"/>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C224" s="2" t="s">
+      <c r="C224" s="6"/>
+      <c r="D224" s="6"/>
+      <c r="E224" s="6"/>
+      <c r="F224" s="6"/>
+      <c r="G224" s="6"/>
+      <c r="H224" s="6"/>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C225" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D224" s="2" t="s">
+      <c r="D225" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="225" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="C225" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D225" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="E225" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="6" t="s">
+    <row r="226" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C226" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D226" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B226" s="6" t="s">
+      <c r="B227" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="C226" s="6"/>
-      <c r="D226" s="6"/>
-      <c r="E226" s="6"/>
-      <c r="F226" s="6"/>
-      <c r="G226" s="6"/>
-      <c r="H226" s="6"/>
-    </row>
-    <row r="227" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C227" s="2" t="s">
+      <c r="C227" s="6"/>
+      <c r="D227" s="6"/>
+      <c r="E227" s="6"/>
+      <c r="F227" s="6"/>
+      <c r="G227" s="6"/>
+      <c r="H227" s="6"/>
+    </row>
+    <row r="228" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C228" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D227" s="2" t="s">
+      <c r="D228" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C228" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D228" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="E228" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="229" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="6"/>
-      <c r="B229" s="6"/>
-      <c r="C229" s="6"/>
-      <c r="D229" s="6"/>
-      <c r="E229" s="6"/>
-      <c r="F229" s="6"/>
-      <c r="G229" s="6"/>
-      <c r="H229" s="6"/>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C229" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="6"/>
+      <c r="B230" s="6"/>
+      <c r="C230" s="6"/>
+      <c r="D230" s="6"/>
+      <c r="E230" s="6"/>
+      <c r="F230" s="6"/>
+      <c r="G230" s="6"/>
+      <c r="H230" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H215" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <conditionalFormatting sqref="E3:E8 E154:E155 E157:E158 E160:E161 E163 E165 E167 E169:E170 E175:E176 E181:E184 E186:E188 E190:E191 E202:E203 E205:E206 E208:E209 E211:E212 E214:E215 E193:E194 E196:E197 E199:E200 E172:E173 E178:E179">
+  <autoFilter ref="A1:H216" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <conditionalFormatting sqref="E3:E8 E155:E156 E158:E159 E161:E162 E164 E166 E168 E170:E171 E176:E177 E182:E185 E187:E189 E191:E192 E203:E204 E206:E207 E209:E210 E212:E213 E215:E216 E194:E195 E197:E198 E200:E201 E173:E174 E179:E180">
     <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5357,7 +5376,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E132:E135 E137:E140 E142:E144 E146:E148 E150:E152">
+  <conditionalFormatting sqref="E133:E136 E138:E141 E143:E145 E147:E149 E151:E153">
     <cfRule type="cellIs" dxfId="59" priority="13" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5401,7 +5420,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E55:E56">
+  <conditionalFormatting sqref="E55:E57">
     <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5412,7 +5431,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E63">
+  <conditionalFormatting sqref="E59:E64">
     <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5423,7 +5442,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E65:E67">
+  <conditionalFormatting sqref="E66:E68">
     <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5434,7 +5453,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69:E74">
+  <conditionalFormatting sqref="E70:E75">
     <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5445,7 +5464,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E76:E78">
+  <conditionalFormatting sqref="E77:E79">
     <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5456,7 +5475,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E80:E81">
+  <conditionalFormatting sqref="E81:E82">
     <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5467,7 +5486,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E83:E88">
+  <conditionalFormatting sqref="E84:E89">
     <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5478,7 +5497,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E90:E94">
+  <conditionalFormatting sqref="E91:E95">
     <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5489,7 +5508,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E97:E103">
+  <conditionalFormatting sqref="E98:E104">
     <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5500,7 +5519,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
+  <conditionalFormatting sqref="E97">
     <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5511,7 +5530,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E105:E109">
+  <conditionalFormatting sqref="E106:E110">
     <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5522,7 +5541,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E111:E114">
+  <conditionalFormatting sqref="E112:E115">
     <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5533,7 +5552,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E116:E120">
+  <conditionalFormatting sqref="E117:E121">
     <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5544,7 +5563,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E122:E125 E127:E130">
+  <conditionalFormatting sqref="E123:E126 E128:E131">
     <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5555,7 +5574,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E219">
+  <conditionalFormatting sqref="E220">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5566,7 +5585,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E217:E218">
+  <conditionalFormatting sqref="E218:E219">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
@@ -5608,31 +5627,31 @@
     <hyperlink ref="G45:G47" r:id="rId28" display="https://github.com/NREL/openstudio-standards/blob/nrcan/lib/openstudio-standards/standards/necb/NECB2011/demand_controlled_ventilation.md" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
     <hyperlink ref="G53" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
     <hyperlink ref="G56" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G83" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G90" r:id="rId32" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G96" r:id="rId33" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G105" r:id="rId34" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G111" r:id="rId35" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G116" r:id="rId36" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="G122" r:id="rId37" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="G127" r:id="rId38" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="G132" r:id="rId39" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="G137" r:id="rId40" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="G142" r:id="rId41" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="G146" r:id="rId42" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="G150" r:id="rId43" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="G170" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="G176" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="G179" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="G181" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="G182" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="G183" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="G184" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="G173" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="G191" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="G194" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="G197" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="G200" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="G84" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G91" r:id="rId32" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G97" r:id="rId33" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G106" r:id="rId34" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G112" r:id="rId35" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G117" r:id="rId36" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G123" r:id="rId37" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="G128" r:id="rId38" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="G133" r:id="rId39" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="G138" r:id="rId40" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="G143" r:id="rId41" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="G147" r:id="rId42" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="G151" r:id="rId43" display="https://github.com/canmet-energy/btap_costing/blob/master/common_resources/national_average_cost_information.xlsm" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="G171" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="G177" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="G180" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="G182" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="G183" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="G184" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="G185" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="G174" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="G192" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="G195" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="G198" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="G201" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
     <hyperlink ref="G6" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Setting HS14_CGSHP_FanCoils option costing flag to true in BTAPOptions.xlsx.  Updating input.yml files to include NECB2020 and the basic 7 weather files which will be inculded in openstudio-standards.
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckirney\projects\btap_batch\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\projects\btap_batch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DE7628-FDA2-4F6A-946A-4C37C7608B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3714E888-26FA-4AF8-A970-097C6D32AAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="15" windowWidth="26055" windowHeight="15015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3348" yWindow="1140" windowWidth="34560" windowHeight="18552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadME" sheetId="2" r:id="rId1"/>
@@ -1201,7 +1201,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="57">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1214,6 +1224,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1224,6 +1254,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1234,6 +1274,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1244,6 +1294,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1264,6 +1334,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1274,6 +1354,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1284,6 +1374,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1294,6 +1394,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1304,6 +1414,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1314,6 +1434,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1324,6 +1474,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1334,6 +1504,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1344,6 +1524,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1354,6 +1544,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1364,6 +1564,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1374,6 +1584,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1384,6 +1604,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1404,6 +1634,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1414,6 +1654,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1424,6 +1684,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1434,6 +1704,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1444,6 +1724,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1454,381 +1744,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2114,9 +2054,9 @@
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>282</v>
       </c>
@@ -2131,24 +2071,24 @@
   <dimension ref="A1:H230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2114,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2190,7 +2130,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2204,7 +2144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2218,7 +2158,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2232,7 +2172,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>307</v>
       </c>
@@ -2246,7 +2186,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
@@ -2263,7 +2203,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>22</v>
@@ -2281,7 +2221,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -2297,7 +2237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2312,7 +2252,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
@@ -2327,7 +2267,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
@@ -2342,7 +2282,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
@@ -2357,7 +2297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
@@ -2372,7 +2312,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
@@ -2387,7 +2327,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
@@ -2402,7 +2342,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
@@ -2417,7 +2357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
@@ -2432,7 +2372,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
@@ -2447,7 +2387,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>48</v>
       </c>
@@ -2462,7 +2402,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>50</v>
       </c>
@@ -2477,7 +2417,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>52</v>
       </c>
@@ -2492,7 +2432,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
@@ -2507,7 +2447,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
         <v>56</v>
       </c>
@@ -2522,7 +2462,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
@@ -2537,7 +2477,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
@@ -2552,7 +2492,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
@@ -2568,7 +2508,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
         <v>63</v>
       </c>
@@ -2583,7 +2523,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>66</v>
       </c>
@@ -2598,7 +2538,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
         <v>67</v>
       </c>
@@ -2613,7 +2553,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
         <v>68</v>
       </c>
@@ -2628,7 +2568,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>69</v>
       </c>
@@ -2643,7 +2583,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>70</v>
       </c>
@@ -2658,7 +2598,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>71</v>
       </c>
@@ -2673,7 +2613,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>72</v>
       </c>
@@ -2689,7 +2629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
         <v>74</v>
       </c>
@@ -2706,7 +2646,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
         <v>78</v>
       </c>
@@ -2723,7 +2663,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
         <v>310</v>
       </c>
@@ -2732,7 +2672,7 @@
       </c>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
         <v>311</v>
       </c>
@@ -2741,7 +2681,7 @@
       </c>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
         <v>312</v>
       </c>
@@ -2750,7 +2690,7 @@
       </c>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
         <v>313</v>
       </c>
@@ -2759,7 +2699,7 @@
       </c>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C42" s="1" t="s">
         <v>80</v>
       </c>
@@ -2776,7 +2716,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>82</v>
       </c>
@@ -2792,7 +2732,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C44" s="4" t="s">
         <v>84</v>
       </c>
@@ -2806,7 +2746,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C45" s="1" t="s">
         <v>87</v>
       </c>
@@ -2820,7 +2760,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C46" s="1" t="s">
         <v>89</v>
       </c>
@@ -2834,7 +2774,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C47" s="1" t="s">
         <v>91</v>
       </c>
@@ -2848,7 +2788,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>93</v>
       </c>
@@ -2864,7 +2804,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C49" s="1" t="s">
         <v>84</v>
       </c>
@@ -2876,7 +2816,7 @@
       </c>
       <c r="F49" s="17"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C50" s="1" t="s">
         <v>96</v>
       </c>
@@ -2888,7 +2828,7 @@
       </c>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>98</v>
       </c>
@@ -2904,7 +2844,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C52" s="1" t="s">
         <v>84</v>
       </c>
@@ -2918,7 +2858,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C53" s="1" t="s">
         <v>102</v>
       </c>
@@ -2933,7 +2873,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>105</v>
       </c>
@@ -2949,7 +2889,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C55" s="1" t="s">
         <v>84</v>
       </c>
@@ -2961,7 +2901,7 @@
       </c>
       <c r="F55" s="17"/>
     </row>
-    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C56" s="1" t="s">
         <v>107</v>
       </c>
@@ -2978,7 +2918,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C57" s="1" t="s">
         <v>319</v>
       </c>
@@ -2991,7 +2931,7 @@
       <c r="F57" s="17"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>110</v>
       </c>
@@ -3007,7 +2947,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C59" s="1" t="s">
         <v>84</v>
       </c>
@@ -3021,7 +2961,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C60" s="25" t="s">
         <v>114</v>
       </c>
@@ -3035,7 +2975,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="C61" s="24" t="s">
         <v>117</v>
       </c>
@@ -3049,7 +2989,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C62" s="27" t="s">
         <v>120</v>
       </c>
@@ -3063,7 +3003,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="C63" s="24" t="s">
         <v>123</v>
       </c>
@@ -3077,7 +3017,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="C64" s="24" t="s">
         <v>316</v>
       </c>
@@ -3085,13 +3025,13 @@
         <v>317</v>
       </c>
       <c r="E64" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" s="17" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>126</v>
       </c>
@@ -3107,7 +3047,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C66" s="1" t="s">
         <v>84</v>
       </c>
@@ -3119,7 +3059,7 @@
       </c>
       <c r="F66" s="17"/>
     </row>
-    <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C67" s="1" t="s">
         <v>129</v>
       </c>
@@ -3133,7 +3073,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C68" s="1" t="s">
         <v>132</v>
       </c>
@@ -3147,7 +3087,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>135</v>
       </c>
@@ -3163,7 +3103,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C70" s="1" t="s">
         <v>84</v>
       </c>
@@ -3174,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C71" s="1" t="s">
         <v>138</v>
       </c>
@@ -3186,7 +3126,7 @@
       </c>
       <c r="F71" s="17"/>
     </row>
-    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C72" s="1" t="s">
         <v>140</v>
       </c>
@@ -3200,7 +3140,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C73" s="1" t="s">
         <v>143</v>
       </c>
@@ -3212,7 +3152,7 @@
       </c>
       <c r="F73" s="17"/>
     </row>
-    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C74" s="1" t="s">
         <v>145</v>
       </c>
@@ -3224,7 +3164,7 @@
       </c>
       <c r="F74" s="17"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C75" s="1" t="s">
         <v>147</v>
       </c>
@@ -3236,7 +3176,7 @@
       </c>
       <c r="F75" s="17"/>
     </row>
-    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>149</v>
       </c>
@@ -3252,7 +3192,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C77" s="1" t="s">
         <v>84</v>
       </c>
@@ -3266,7 +3206,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C78" s="1" t="s">
         <v>153</v>
       </c>
@@ -3280,7 +3220,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C79" s="1" t="s">
         <v>156</v>
       </c>
@@ -3294,7 +3234,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>159</v>
       </c>
@@ -3310,7 +3250,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C81" s="1" t="s">
         <v>84</v>
       </c>
@@ -3324,7 +3264,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C82" s="1" t="s">
         <v>163</v>
       </c>
@@ -3338,7 +3278,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>166</v>
       </c>
@@ -3354,7 +3294,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C84" s="7" t="s">
         <v>84</v>
       </c>
@@ -3371,7 +3311,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C85" s="1">
         <v>0.314</v>
       </c>
@@ -3383,7 +3323,7 @@
       </c>
       <c r="F85" s="17"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C86" s="1">
         <v>0.27800000000000002</v>
       </c>
@@ -3395,7 +3335,7 @@
       </c>
       <c r="F86" s="17"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C87" s="1">
         <v>0.247</v>
       </c>
@@ -3407,7 +3347,7 @@
       </c>
       <c r="F87" s="17"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C88" s="1">
         <v>0.21</v>
       </c>
@@ -3419,7 +3359,7 @@
       </c>
       <c r="F88" s="17"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C89" s="1">
         <v>0.183</v>
       </c>
@@ -3431,7 +3371,7 @@
       </c>
       <c r="F89" s="17"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>172</v>
       </c>
@@ -3447,7 +3387,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C91" s="7" t="s">
         <v>84</v>
       </c>
@@ -3464,7 +3404,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C92" s="1">
         <v>0.22700000000000001</v>
       </c>
@@ -3476,7 +3416,7 @@
       </c>
       <c r="F92" s="17"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C93" s="1">
         <v>0.183</v>
       </c>
@@ -3488,7 +3428,7 @@
       </c>
       <c r="F93" s="17"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C94" s="1">
         <v>0.16200000000000001</v>
       </c>
@@ -3500,7 +3440,7 @@
       </c>
       <c r="F94" s="17"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C95" s="1">
         <v>0.14199999999999999</v>
       </c>
@@ -3512,7 +3452,7 @@
       </c>
       <c r="F95" s="17"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>175</v>
       </c>
@@ -3528,7 +3468,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C97" s="7" t="s">
         <v>84</v>
       </c>
@@ -3545,7 +3485,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C98" s="1">
         <v>0.22700000000000001</v>
       </c>
@@ -3557,7 +3497,7 @@
       </c>
       <c r="F98" s="17"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C99" s="1">
         <v>0.193</v>
       </c>
@@ -3569,7 +3509,7 @@
       </c>
       <c r="F99" s="17"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C100" s="1">
         <v>0.183</v>
       </c>
@@ -3581,7 +3521,7 @@
       </c>
       <c r="F100" s="17"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C101" s="1">
         <v>0.16200000000000001</v>
       </c>
@@ -3593,7 +3533,7 @@
       </c>
       <c r="F101" s="17"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C102" s="1">
         <v>0.14199999999999999</v>
       </c>
@@ -3605,7 +3545,7 @@
       </c>
       <c r="F102" s="17"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C103" s="1">
         <v>0.13800000000000001</v>
       </c>
@@ -3617,7 +3557,7 @@
       </c>
       <c r="F103" s="17"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C104" s="1">
         <v>0.121</v>
       </c>
@@ -3629,7 +3569,7 @@
       </c>
       <c r="F104" s="17"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>177</v>
       </c>
@@ -3645,7 +3585,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C106" s="1" t="s">
         <v>84</v>
       </c>
@@ -3662,7 +3602,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C107" s="1">
         <v>0.56799999999999995</v>
       </c>
@@ -3674,7 +3614,7 @@
       </c>
       <c r="F107" s="17"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C108" s="1">
         <v>0.379</v>
       </c>
@@ -3686,7 +3626,7 @@
       </c>
       <c r="F108" s="17"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C109" s="1">
         <v>0.28399999999999997</v>
       </c>
@@ -3698,7 +3638,7 @@
       </c>
       <c r="F109" s="17"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C110" s="1">
         <v>0.21</v>
       </c>
@@ -3710,7 +3650,7 @@
       </c>
       <c r="F110" s="17"/>
     </row>
-    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>179</v>
       </c>
@@ -3726,7 +3666,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C112" s="1" t="s">
         <v>84</v>
       </c>
@@ -3743,7 +3683,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C113" s="1">
         <v>0.75800000000000001</v>
       </c>
@@ -3755,7 +3695,7 @@
       </c>
       <c r="F113" s="17"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C114" s="1">
         <v>0.379</v>
       </c>
@@ -3767,13 +3707,13 @@
       </c>
       <c r="F114" s="17"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E115" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F115" s="17"/>
     </row>
-    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>181</v>
       </c>
@@ -3789,7 +3729,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C117" s="7" t="s">
         <v>183</v>
       </c>
@@ -3806,7 +3746,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C118" s="1">
         <v>0.56799999999999995</v>
       </c>
@@ -3818,7 +3758,7 @@
       </c>
       <c r="F118" s="17"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C119" s="4">
         <v>0.379</v>
       </c>
@@ -3830,7 +3770,7 @@
       </c>
       <c r="F119" s="17"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C120" s="1">
         <v>0.28399999999999997</v>
       </c>
@@ -3842,7 +3782,7 @@
       </c>
       <c r="F120" s="17"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C121" s="1">
         <v>0.21</v>
       </c>
@@ -3854,7 +3794,7 @@
       </c>
       <c r="F121" s="17"/>
     </row>
-    <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>184</v>
       </c>
@@ -3870,7 +3810,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C123" s="1" t="s">
         <v>84</v>
       </c>
@@ -3887,7 +3827,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C124" s="1">
         <v>2.4</v>
       </c>
@@ -3899,7 +3839,7 @@
       </c>
       <c r="F124" s="17"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C125" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -3911,7 +3851,7 @@
       </c>
       <c r="F125" s="17"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C126" s="1">
         <v>1.6</v>
       </c>
@@ -3923,7 +3863,7 @@
       </c>
       <c r="F126" s="17"/>
     </row>
-    <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>186</v>
       </c>
@@ -3938,7 +3878,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C128" s="1" t="s">
         <v>84</v>
       </c>
@@ -3955,7 +3895,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C129" s="1">
         <v>2.4</v>
       </c>
@@ -3967,7 +3907,7 @@
       </c>
       <c r="F129" s="17"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C130" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -3979,7 +3919,7 @@
       </c>
       <c r="F130" s="17"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C131" s="1">
         <v>1.6</v>
       </c>
@@ -3991,7 +3931,7 @@
       </c>
       <c r="F131" s="17"/>
     </row>
-    <row r="132" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>188</v>
       </c>
@@ -4007,7 +3947,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C133" s="1" t="s">
         <v>84</v>
       </c>
@@ -4024,7 +3964,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C134" s="1">
         <v>2.4</v>
       </c>
@@ -4036,7 +3976,7 @@
       </c>
       <c r="F134" s="17"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C135" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -4048,7 +3988,7 @@
       </c>
       <c r="F135" s="17"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C136" s="1">
         <v>1.6</v>
       </c>
@@ -4060,7 +4000,7 @@
       </c>
       <c r="F136" s="17"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>190</v>
       </c>
@@ -4076,7 +4016,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C138" s="1" t="s">
         <v>84</v>
       </c>
@@ -4093,7 +4033,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C139" s="1">
         <v>2.4</v>
       </c>
@@ -4105,7 +4045,7 @@
       </c>
       <c r="F139" s="17"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C140" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -4117,7 +4057,7 @@
       </c>
       <c r="F140" s="17"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C141" s="1">
         <v>1.6</v>
       </c>
@@ -4129,7 +4069,7 @@
       </c>
       <c r="F141" s="17"/>
     </row>
-    <row r="142" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>192</v>
       </c>
@@ -4145,7 +4085,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C143" s="1" t="s">
         <v>84</v>
       </c>
@@ -4162,7 +4102,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C144" s="1">
         <v>0.05</v>
       </c>
@@ -4171,7 +4111,7 @@
       </c>
       <c r="F144" s="17"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C145" s="1">
         <v>0.9</v>
       </c>
@@ -4183,7 +4123,7 @@
       </c>
       <c r="F145" s="17"/>
     </row>
-    <row r="146" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>194</v>
       </c>
@@ -4199,7 +4139,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C147" s="1" t="s">
         <v>84</v>
       </c>
@@ -4216,7 +4156,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C148" s="1">
         <v>0.05</v>
       </c>
@@ -4228,7 +4168,7 @@
       </c>
       <c r="F148" s="17"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C149" s="1">
         <v>0.9</v>
       </c>
@@ -4240,7 +4180,7 @@
       </c>
       <c r="F149" s="17"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>196</v>
       </c>
@@ -4256,7 +4196,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C151" s="1" t="s">
         <v>84</v>
       </c>
@@ -4270,7 +4210,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C152" s="1">
         <v>0.05</v>
       </c>
@@ -4279,7 +4219,7 @@
       </c>
       <c r="F152" s="17"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C153" s="1">
         <v>0.9</v>
       </c>
@@ -4288,7 +4228,7 @@
       </c>
       <c r="F153" s="17"/>
     </row>
-    <row r="154" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>198</v>
       </c>
@@ -4304,7 +4244,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C155" s="1" t="s">
         <v>84</v>
       </c>
@@ -4321,7 +4261,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C156" s="1" t="s">
         <v>96</v>
       </c>
@@ -4333,7 +4273,7 @@
       </c>
       <c r="F156" s="17"/>
     </row>
-    <row r="157" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>204</v>
       </c>
@@ -4350,7 +4290,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="C158" s="1" t="s">
         <v>84</v>
       </c>
@@ -4367,7 +4307,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C159" s="1" t="s">
         <v>96</v>
       </c>
@@ -4379,7 +4319,7 @@
       </c>
       <c r="F159" s="17"/>
     </row>
-    <row r="160" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>207</v>
       </c>
@@ -4395,7 +4335,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C161" s="1" t="s">
         <v>84</v>
       </c>
@@ -4407,7 +4347,7 @@
       </c>
       <c r="F161" s="17"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C162" s="1" t="s">
         <v>96</v>
       </c>
@@ -4419,7 +4359,7 @@
       </c>
       <c r="F162" s="17"/>
     </row>
-    <row r="163" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>211</v>
       </c>
@@ -4435,7 +4375,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C164" s="1" t="s">
         <v>96</v>
       </c>
@@ -4447,7 +4387,7 @@
       </c>
       <c r="F164" s="17"/>
     </row>
-    <row r="165" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>214</v>
       </c>
@@ -4463,7 +4403,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C166" s="1" t="s">
         <v>96</v>
       </c>
@@ -4475,7 +4415,7 @@
       </c>
       <c r="F166" s="17"/>
     </row>
-    <row r="167" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>216</v>
       </c>
@@ -4491,7 +4431,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C168" s="1" t="s">
         <v>96</v>
       </c>
@@ -4503,7 +4443,7 @@
       </c>
       <c r="F168" s="17"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>218</v>
       </c>
@@ -4519,7 +4459,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C170" s="1" t="s">
         <v>84</v>
       </c>
@@ -4531,7 +4471,7 @@
       </c>
       <c r="F170" s="17"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C171" s="1" t="s">
         <v>221</v>
       </c>
@@ -4548,7 +4488,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="172" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>224</v>
       </c>
@@ -4559,7 +4499,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C173" s="1" t="s">
         <v>84</v>
       </c>
@@ -4572,7 +4512,7 @@
       <c r="F173" s="22"/>
       <c r="G173" s="3"/>
     </row>
-    <row r="174" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C174" s="1" t="s">
         <v>96</v>
       </c>
@@ -4589,7 +4529,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>228</v>
       </c>
@@ -4605,7 +4545,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C176" s="1" t="s">
         <v>84</v>
       </c>
@@ -4617,7 +4557,7 @@
       </c>
       <c r="F176" s="17"/>
     </row>
-    <row r="177" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C177" s="1" t="s">
         <v>96</v>
       </c>
@@ -4634,7 +4574,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>232</v>
       </c>
@@ -4650,7 +4590,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C179" s="1" t="s">
         <v>84</v>
       </c>
@@ -4662,7 +4602,7 @@
       </c>
       <c r="F179" s="17"/>
     </row>
-    <row r="180" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C180" s="1" t="s">
         <v>96</v>
       </c>
@@ -4679,7 +4619,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>236</v>
       </c>
@@ -4695,7 +4635,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C182" s="1" t="s">
         <v>84</v>
       </c>
@@ -4712,7 +4652,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C183" s="1" t="s">
         <v>239</v>
       </c>
@@ -4729,7 +4669,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C184" s="1" t="s">
         <v>241</v>
       </c>
@@ -4746,7 +4686,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C185" s="1" t="s">
         <v>243</v>
       </c>
@@ -4763,7 +4703,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>245</v>
       </c>
@@ -4779,7 +4719,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C187" s="1" t="s">
         <v>84</v>
       </c>
@@ -4791,7 +4731,7 @@
       </c>
       <c r="F187" s="17"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C188" s="1" t="s">
         <v>248</v>
       </c>
@@ -4803,13 +4743,13 @@
       </c>
       <c r="F188" s="17"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E189" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F189" s="17"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>250</v>
       </c>
@@ -4825,7 +4765,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C191" s="1" t="s">
         <v>84</v>
       </c>
@@ -4837,7 +4777,7 @@
       </c>
       <c r="F191" s="17"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C192" s="1" t="s">
         <v>253</v>
       </c>
@@ -4854,7 +4794,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>256</v>
       </c>
@@ -4870,7 +4810,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C194" s="1" t="s">
         <v>84</v>
       </c>
@@ -4882,7 +4822,7 @@
       </c>
       <c r="F194" s="17"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C195" s="1" t="s">
         <v>96</v>
       </c>
@@ -4899,7 +4839,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>260</v>
       </c>
@@ -4915,7 +4855,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C197" s="1" t="s">
         <v>84</v>
       </c>
@@ -4927,7 +4867,7 @@
       </c>
       <c r="F197" s="17"/>
     </row>
-    <row r="198" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C198" s="1" t="s">
         <v>96</v>
       </c>
@@ -4944,7 +4884,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="199" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>264</v>
       </c>
@@ -4955,7 +4895,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C200" s="1" t="s">
         <v>84</v>
       </c>
@@ -4968,7 +4908,7 @@
       <c r="F200" s="22"/>
       <c r="G200" s="3"/>
     </row>
-    <row r="201" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C201" s="1" t="s">
         <v>96</v>
       </c>
@@ -4985,7 +4925,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>268</v>
       </c>
@@ -5001,7 +4941,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C203" s="1" t="s">
         <v>84</v>
       </c>
@@ -5013,7 +4953,7 @@
       </c>
       <c r="F203" s="17"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C204" s="1" t="s">
         <v>96</v>
       </c>
@@ -5025,7 +4965,7 @@
       </c>
       <c r="F204" s="17"/>
     </row>
-    <row r="205" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
         <v>270</v>
       </c>
@@ -5041,7 +4981,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C206" s="1" t="s">
         <v>84</v>
       </c>
@@ -5055,7 +4995,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C207" s="1" t="s">
         <v>96</v>
       </c>
@@ -5069,7 +5009,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>274</v>
       </c>
@@ -5085,7 +5025,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C209" s="1" t="s">
         <v>84</v>
       </c>
@@ -5097,7 +5037,7 @@
       </c>
       <c r="F209" s="17"/>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C210" s="1" t="s">
         <v>96</v>
       </c>
@@ -5109,7 +5049,7 @@
       </c>
       <c r="F210" s="17"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>276</v>
       </c>
@@ -5125,7 +5065,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C212" s="1" t="s">
         <v>84</v>
       </c>
@@ -5137,7 +5077,7 @@
       </c>
       <c r="F212" s="17"/>
     </row>
-    <row r="213" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C213" s="1" t="s">
         <v>278</v>
       </c>
@@ -5149,7 +5089,7 @@
       </c>
       <c r="F213" s="17"/>
     </row>
-    <row r="214" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>280</v>
       </c>
@@ -5165,7 +5105,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C215" s="1" t="s">
         <v>84</v>
       </c>
@@ -5177,7 +5117,7 @@
       </c>
       <c r="F215" s="17"/>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C216" s="1" t="s">
         <v>96</v>
       </c>
@@ -5189,7 +5129,7 @@
       </c>
       <c r="F216" s="17"/>
     </row>
-    <row r="217" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6" t="s">
         <v>288</v>
       </c>
@@ -5203,7 +5143,7 @@
       <c r="G217" s="6"/>
       <c r="H217" s="6"/>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C218" s="2" t="s">
         <v>84</v>
       </c>
@@ -5217,7 +5157,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C219" s="2" t="s">
         <v>290</v>
       </c>
@@ -5231,7 +5171,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C220" s="2" t="s">
         <v>291</v>
       </c>
@@ -5245,7 +5185,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="221" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6" t="s">
         <v>294</v>
       </c>
@@ -5259,7 +5199,7 @@
       <c r="G221" s="6"/>
       <c r="H221" s="6"/>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C222" s="2" t="s">
         <v>84</v>
       </c>
@@ -5270,7 +5210,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C223" s="2" t="s">
         <v>296</v>
       </c>
@@ -5281,7 +5221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="224" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6" t="s">
         <v>298</v>
       </c>
@@ -5295,7 +5235,7 @@
       <c r="G224" s="6"/>
       <c r="H224" s="6"/>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C225" s="2" t="s">
         <v>84</v>
       </c>
@@ -5306,7 +5246,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C226" s="2" t="s">
         <v>296</v>
       </c>
@@ -5317,7 +5257,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
         <v>302</v>
       </c>
@@ -5331,7 +5271,7 @@
       <c r="G227" s="6"/>
       <c r="H227" s="6"/>
     </row>
-    <row r="228" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C228" s="2" t="s">
         <v>84</v>
       </c>
@@ -5342,7 +5282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C229" s="2" t="s">
         <v>96</v>
       </c>
@@ -5353,7 +5293,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="230" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
@@ -5365,235 +5305,213 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H216" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <conditionalFormatting sqref="E3:E8 E155:E156 E158:E159 E161:E162 E164 E166 E168 E170:E171 E176:E177 E182:E185 E187:E189 E191:E192 E203:E204 E206:E207 E209:E210 E212:E213 E215:E216 E194:E195 E197:E198 E200:E201 E173:E174 E179:E180">
-    <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
+  <conditionalFormatting sqref="E3:E8 E155:E156 E158:E159 E161:E162 E164 E166 E168 E170:E171 E173:E174 E176:E177 E179:E180 E182:E185 E187:E189 E191:E192 E194:E195 E197:E198 E200:E201 E203:E204 E206:E207 E209:E210 E212:E213 E215:E216">
+    <cfRule type="cellIs" dxfId="56" priority="68" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="67" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="69" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36:E42">
+    <cfRule type="cellIs" dxfId="53" priority="66" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="65" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="64" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44:E47 E49:E50">
+    <cfRule type="cellIs" dxfId="50" priority="63" operator="equal">
       <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="62" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="61" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52:E53">
+    <cfRule type="cellIs" dxfId="47" priority="60" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55:E57">
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="56" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59:E64">
+    <cfRule type="cellIs" dxfId="41" priority="54" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="53" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="52" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66:E68">
+    <cfRule type="cellIs" dxfId="38" priority="51" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="50" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="49" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70:E75">
+    <cfRule type="cellIs" dxfId="35" priority="48" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="47" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="46" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E77:E79">
+    <cfRule type="cellIs" dxfId="32" priority="45" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="44" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="43" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E81:E82">
+    <cfRule type="cellIs" dxfId="29" priority="42" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="41" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="40" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84:E89">
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="38" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="39" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E91:E95">
+    <cfRule type="cellIs" dxfId="23" priority="36" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="35" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="34" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E97:E104">
+    <cfRule type="cellIs" dxfId="20" priority="30" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E106:E110">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="25" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E112:E115">
+    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E117:E121">
+    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E123:E126 E128:E131">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E133:E136 E138:E141 E143:E145 E147:E149 E151:E153">
-    <cfRule type="cellIs" dxfId="59" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="14" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36:E42">
-    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="66" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44:E47 E49:E50">
-    <cfRule type="cellIs" dxfId="53" priority="61" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="62" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="63" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52:E53">
-    <cfRule type="cellIs" dxfId="50" priority="58" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="59" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E55:E57">
-    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59:E64">
-    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66:E68">
-    <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="50" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="51" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E70:E75">
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E77:E79">
-    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="44" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E81:E82">
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="41" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E84:E89">
-    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="38" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E95">
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E98:E104">
-    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E106:E110">
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E112:E115">
-    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E117:E121">
-    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E123:E126 E128:E131">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E220">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
-      <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E218:E219">
+  <conditionalFormatting sqref="E218:E220">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Updating BTAPOptions.xlsx file to reflect change to basic weather locations.
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\projects\btap_batch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3714E888-26FA-4AF8-A970-097C6D32AAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D8E60C-4470-4467-884D-D956BC382893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3348" yWindow="1140" windowWidth="34560" windowHeight="18552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="322">
   <si>
     <t>Variable</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>CAN_ON_Toronto.Pearson.Intl.AP.716240_CWEC2016.epw</t>
-  </si>
-  <si>
-    <t>CAN_YT_Whitehorse.Intl.AP.719640_CWEC2016.epw</t>
   </si>
   <si>
     <t>:primary_heating_fuel</t>
@@ -995,13 +992,19 @@
   </si>
   <si>
     <t>Do no add daylighting sensors.</t>
+  </si>
+  <si>
+    <t>CAN_NT_Yellowknife.AP.719360_CWEC2016.epw</t>
+  </si>
+  <si>
+    <t>Default location for climate zone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1037,6 +1040,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1112,7 +1120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1196,6 +1204,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1294,6 +1303,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1304,6 +1333,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1469,36 +1508,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2058,7 +2067,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -2071,8 +2080,8 @@
   <dimension ref="A1:H230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2111,7 +2120,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2174,16 +2183,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="E6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2194,7 +2203,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>20</v>
@@ -2212,7 +2221,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>20</v>
@@ -2497,7 +2506,7 @@
         <v>62</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -2513,7 +2522,7 @@
         <v>63</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>64</v>
+        <v>321</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>29</v>
@@ -2528,7 +2537,7 @@
         <v>66</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>64</v>
+        <v>321</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>29</v>
@@ -2543,7 +2552,7 @@
         <v>67</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>64</v>
+        <v>321</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>29</v>
@@ -2558,7 +2567,7 @@
         <v>68</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>64</v>
+        <v>321</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>29</v>
@@ -2598,9 +2607,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C34" s="1" t="s">
-        <v>71</v>
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+      <c r="C34" s="29" t="s">
+        <v>320</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>64</v>
@@ -2615,10 +2624,10 @@
     </row>
     <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
@@ -2631,41 +2640,41 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E38" s="1" t="b">
         <v>1</v>
@@ -2674,7 +2683,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E39" s="1" t="b">
         <v>1</v>
@@ -2683,7 +2692,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E40" s="1" t="b">
         <v>1</v>
@@ -2692,7 +2701,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E41" s="1" t="b">
         <v>1</v>
@@ -2701,27 +2710,27 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="E42" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
@@ -2729,71 +2738,71 @@
       <c r="F43" s="6"/>
       <c r="G43" s="5"/>
       <c r="H43" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C44" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="E44" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C45" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="E45" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="E46" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="E47" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="13"/>
@@ -2801,15 +2810,15 @@
       <c r="F48" s="13"/>
       <c r="G48" s="14"/>
       <c r="H48" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C49" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>29</v>
@@ -2818,10 +2827,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>29</v>
@@ -2830,10 +2839,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="6"/>
@@ -2841,44 +2850,44 @@
       <c r="F51" s="6"/>
       <c r="G51" s="5"/>
       <c r="H51" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C52" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E52" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="E52" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C53" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="E53" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>106</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="6"/>
@@ -2886,15 +2895,15 @@
       <c r="F54" s="6"/>
       <c r="G54" s="5"/>
       <c r="H54" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C55" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E55" s="8" t="b">
         <v>1</v>
@@ -2903,27 +2912,27 @@
     </row>
     <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C56" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E56" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E56" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="17" t="s">
+      <c r="G56" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C57" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>320</v>
       </c>
       <c r="E57" s="8" t="b">
         <v>1</v>
@@ -2933,10 +2942,10 @@
     </row>
     <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
@@ -2944,99 +2953,99 @@
       <c r="F58" s="6"/>
       <c r="G58" s="5"/>
       <c r="H58" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C59" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="17" t="s">
         <v>112</v>
-      </c>
-      <c r="E59" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="17" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C60" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D60" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="26" t="s">
+      <c r="E60" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="E60" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="17" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="C61" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D61" s="23" t="s">
+      <c r="E61" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="17" t="s">
         <v>118</v>
-      </c>
-      <c r="E61" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C62" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D62" s="26" t="s">
+      <c r="E62" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="17" t="s">
         <v>121</v>
-      </c>
-      <c r="E62" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="C63" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="23" t="s">
+      <c r="E63" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="17" t="s">
         <v>124</v>
-      </c>
-      <c r="E63" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="17" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="C64" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="D64" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="D64" s="28" t="s">
+      <c r="E64" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="17" t="s">
         <v>317</v>
-      </c>
-      <c r="E64" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
@@ -3044,15 +3053,15 @@
       <c r="F65" s="6"/>
       <c r="G65" s="5"/>
       <c r="H65" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C66" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E66" s="8" t="b">
         <v>1</v>
@@ -3061,38 +3070,38 @@
     </row>
     <row r="67" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="17" t="s">
         <v>130</v>
-      </c>
-      <c r="E67" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="17" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C68" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="E68" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="17" t="s">
         <v>133</v>
-      </c>
-      <c r="E68" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" s="17" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>136</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="6"/>
@@ -3100,15 +3109,15 @@
       <c r="F69" s="6"/>
       <c r="G69" s="5"/>
       <c r="H69" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C70" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E70" s="8" t="b">
         <v>1</v>
@@ -3116,10 +3125,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C71" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="E71" s="8" t="b">
         <v>1</v>
@@ -3128,24 +3137,24 @@
     </row>
     <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C72" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="E72" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="17" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C73" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="E73" s="8" t="b">
         <v>1</v>
@@ -3154,10 +3163,10 @@
     </row>
     <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C74" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="E74" s="8" t="b">
         <v>1</v>
@@ -3166,10 +3175,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C75" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="E75" s="8" t="b">
         <v>1</v>
@@ -3178,10 +3187,10 @@
     </row>
     <row r="76" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
@@ -3189,57 +3198,57 @@
       <c r="F76" s="6"/>
       <c r="G76" s="5"/>
       <c r="H76" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C77" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E77" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="17" t="s">
         <v>151</v>
-      </c>
-      <c r="E77" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C78" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="E78" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="17" t="s">
         <v>154</v>
-      </c>
-      <c r="E78" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C79" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="E79" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="6"/>
@@ -3247,43 +3256,43 @@
       <c r="F80" s="6"/>
       <c r="G80" s="5"/>
       <c r="H80" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C81" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E81" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="E81" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="17" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="E82" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="6"/>
@@ -3291,24 +3300,24 @@
       <c r="F83" s="6"/>
       <c r="G83" s="5"/>
       <c r="H83" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C84" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D84" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E84" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E84" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="17" t="s">
+      <c r="G84" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
@@ -3316,7 +3325,7 @@
         <v>0.314</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E85" s="8" t="b">
         <v>1</v>
@@ -3328,7 +3337,7 @@
         <v>0.27800000000000002</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E86" s="8" t="b">
         <v>1</v>
@@ -3340,7 +3349,7 @@
         <v>0.247</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E87" s="8" t="b">
         <v>1</v>
@@ -3352,7 +3361,7 @@
         <v>0.21</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E88" s="8" t="b">
         <v>1</v>
@@ -3364,7 +3373,7 @@
         <v>0.183</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E89" s="8" t="b">
         <v>1</v>
@@ -3373,10 +3382,10 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="6"/>
@@ -3384,24 +3393,24 @@
       <c r="F90" s="6"/>
       <c r="G90" s="5"/>
       <c r="H90" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C91" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D91" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E91" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E91" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G91" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
@@ -3409,7 +3418,7 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E92" s="8" t="b">
         <v>1</v>
@@ -3421,7 +3430,7 @@
         <v>0.183</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E93" s="8" t="b">
         <v>1</v>
@@ -3433,7 +3442,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E94" s="8" t="b">
         <v>1</v>
@@ -3445,7 +3454,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E95" s="8" t="b">
         <v>1</v>
@@ -3454,10 +3463,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="6"/>
@@ -3465,24 +3474,24 @@
       <c r="F96" s="6"/>
       <c r="G96" s="5"/>
       <c r="H96" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C97" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E97" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E97" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G97" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -3490,7 +3499,7 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E98" s="8" t="b">
         <v>1</v>
@@ -3502,7 +3511,7 @@
         <v>0.193</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E99" s="8" t="b">
         <v>1</v>
@@ -3514,7 +3523,7 @@
         <v>0.183</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E100" s="8" t="b">
         <v>1</v>
@@ -3526,7 +3535,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E101" s="8" t="b">
         <v>1</v>
@@ -3538,7 +3547,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E102" s="8" t="b">
         <v>1</v>
@@ -3550,7 +3559,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E103" s="8" t="b">
         <v>1</v>
@@ -3562,7 +3571,7 @@
         <v>0.121</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E104" s="8" t="b">
         <v>1</v>
@@ -3571,10 +3580,10 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="6"/>
@@ -3582,24 +3591,24 @@
       <c r="F105" s="6"/>
       <c r="G105" s="5"/>
       <c r="H105" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C106" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D106" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E106" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E106" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F106" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G106" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
@@ -3607,7 +3616,7 @@
         <v>0.56799999999999995</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E107" s="8" t="b">
         <v>1</v>
@@ -3619,7 +3628,7 @@
         <v>0.379</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E108" s="8" t="b">
         <v>1</v>
@@ -3631,7 +3640,7 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E109" s="8" t="b">
         <v>1</v>
@@ -3643,7 +3652,7 @@
         <v>0.21</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E110" s="8" t="b">
         <v>1</v>
@@ -3652,10 +3661,10 @@
     </row>
     <row r="111" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B111" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="6"/>
@@ -3663,24 +3672,24 @@
       <c r="F111" s="6"/>
       <c r="G111" s="5"/>
       <c r="H111" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C112" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D112" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E112" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E112" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F112" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G112" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
@@ -3688,7 +3697,7 @@
         <v>0.75800000000000001</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E113" s="8" t="b">
         <v>1</v>
@@ -3700,7 +3709,7 @@
         <v>0.379</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E114" s="8" t="b">
         <v>1</v>
@@ -3715,10 +3724,10 @@
     </row>
     <row r="116" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B116" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="C116" s="5"/>
       <c r="D116" s="6"/>
@@ -3726,24 +3735,24 @@
       <c r="F116" s="6"/>
       <c r="G116" s="5"/>
       <c r="H116" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C117" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D117" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E117" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E117" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F117" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G117" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
@@ -3751,7 +3760,7 @@
         <v>0.56799999999999995</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E118" s="8" t="b">
         <v>1</v>
@@ -3763,7 +3772,7 @@
         <v>0.379</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E119" s="8" t="b">
         <v>1</v>
@@ -3775,7 +3784,7 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E120" s="8" t="b">
         <v>1</v>
@@ -3787,7 +3796,7 @@
         <v>0.21</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E121" s="8" t="b">
         <v>1</v>
@@ -3796,10 +3805,10 @@
     </row>
     <row r="122" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B122" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="C122" s="5"/>
       <c r="D122" s="6"/>
@@ -3807,24 +3816,24 @@
       <c r="F122" s="6"/>
       <c r="G122" s="5"/>
       <c r="H122" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C123" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D123" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E123" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F123" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E123" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F123" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G123" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
@@ -3832,7 +3841,7 @@
         <v>2.4</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E124" s="8" t="b">
         <v>1</v>
@@ -3844,7 +3853,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E125" s="8" t="b">
         <v>1</v>
@@ -3856,7 +3865,7 @@
         <v>1.6</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E126" s="8" t="b">
         <v>1</v>
@@ -3865,34 +3874,34 @@
     </row>
     <row r="127" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B127" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="C127" s="5"/>
       <c r="D127" s="13"/>
       <c r="E127" s="15"/>
       <c r="F127" s="19"/>
       <c r="H127" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C128" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D128" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E128" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F128" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E128" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F128" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G128" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
@@ -3900,7 +3909,7 @@
         <v>2.4</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E129" s="8" t="b">
         <v>1</v>
@@ -3912,7 +3921,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E130" s="8" t="b">
         <v>1</v>
@@ -3924,7 +3933,7 @@
         <v>1.6</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E131" s="8" t="b">
         <v>1</v>
@@ -3933,10 +3942,10 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B132" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="B132" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="C132" s="5"/>
       <c r="D132" s="6"/>
@@ -3944,24 +3953,24 @@
       <c r="F132" s="6"/>
       <c r="G132" s="5"/>
       <c r="H132" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C133" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D133" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E133" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F133" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E133" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F133" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G133" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
@@ -3969,7 +3978,7 @@
         <v>2.4</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E134" s="8" t="b">
         <v>1</v>
@@ -3981,7 +3990,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E135" s="8" t="b">
         <v>1</v>
@@ -3993,7 +4002,7 @@
         <v>1.6</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E136" s="8" t="b">
         <v>1</v>
@@ -4002,10 +4011,10 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B137" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="B137" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="C137" s="5"/>
       <c r="D137" s="13"/>
@@ -4013,24 +4022,24 @@
       <c r="F137" s="19"/>
       <c r="G137" s="14"/>
       <c r="H137" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C138" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D138" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E138" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F138" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E138" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F138" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G138" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
@@ -4038,7 +4047,7 @@
         <v>2.4</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E139" s="8" t="b">
         <v>1</v>
@@ -4050,7 +4059,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E140" s="8" t="b">
         <v>1</v>
@@ -4062,7 +4071,7 @@
         <v>1.6</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E141" s="8" t="b">
         <v>1</v>
@@ -4071,10 +4080,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B142" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="B142" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="C142" s="5"/>
       <c r="D142" s="6"/>
@@ -4082,24 +4091,24 @@
       <c r="F142" s="19"/>
       <c r="G142" s="5"/>
       <c r="H142" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C143" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D143" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E143" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F143" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E143" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F143" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G143" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
@@ -4116,7 +4125,7 @@
         <v>0.9</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E145" s="8" t="b">
         <v>1</v>
@@ -4125,10 +4134,10 @@
     </row>
     <row r="146" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B146" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="B146" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="C146" s="5"/>
       <c r="D146" s="6"/>
@@ -4136,24 +4145,24 @@
       <c r="F146" s="20"/>
       <c r="G146" s="5"/>
       <c r="H146" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C147" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D147" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E147" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F147" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E147" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F147" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="G147" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -4161,7 +4170,7 @@
         <v>0.05</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E148" s="8" t="b">
         <v>1</v>
@@ -4173,7 +4182,7 @@
         <v>0.9</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E149" s="8" t="b">
         <v>1</v>
@@ -4182,10 +4191,10 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B150" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="B150" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="C150" s="5"/>
       <c r="D150" s="6"/>
@@ -4193,21 +4202,21 @@
       <c r="F150" s="20"/>
       <c r="G150" s="5"/>
       <c r="H150" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C151" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E151" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F151" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G151" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
@@ -4230,10 +4239,10 @@
     </row>
     <row r="154" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B154" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="B154" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="C154" s="5"/>
       <c r="D154" s="6"/>
@@ -4241,32 +4250,32 @@
       <c r="F154" s="20"/>
       <c r="G154" s="5"/>
       <c r="H154" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C155" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D155" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E155" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F155" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="E155" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F155" s="17" t="s">
+      <c r="G155" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C156" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E156" s="8" t="b">
         <v>1</v>
@@ -4275,44 +4284,44 @@
     </row>
     <row r="157" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B157" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B157" s="6" t="s">
-        <v>205</v>
-      </c>
       <c r="C157" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E157" s="16"/>
       <c r="F157" s="20"/>
       <c r="G157" s="5"/>
       <c r="H157" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="C158" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E158" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F158" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C159" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E159" s="8" t="b">
         <v>1</v>
@@ -4321,10 +4330,10 @@
     </row>
     <row r="160" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B160" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="C160" s="5"/>
       <c r="D160" s="6"/>
@@ -4332,15 +4341,15 @@
       <c r="F160" s="20"/>
       <c r="G160" s="5"/>
       <c r="H160" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C161" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>29</v>
@@ -4349,10 +4358,10 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C162" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>29</v>
@@ -4361,10 +4370,10 @@
     </row>
     <row r="163" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B163" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="B163" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="C163" s="5"/>
       <c r="D163" s="6"/>
@@ -4372,15 +4381,15 @@
       <c r="F163" s="20"/>
       <c r="G163" s="5"/>
       <c r="H163" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C164" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E164" s="8" t="s">
         <v>29</v>
@@ -4389,10 +4398,10 @@
     </row>
     <row r="165" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B165" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="B165" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="C165" s="5"/>
       <c r="D165" s="6"/>
@@ -4400,15 +4409,15 @@
       <c r="F165" s="20"/>
       <c r="G165" s="5"/>
       <c r="H165" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C166" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>29</v>
@@ -4417,10 +4426,10 @@
     </row>
     <row r="167" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B167" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="B167" s="6" t="s">
-        <v>217</v>
       </c>
       <c r="C167" s="5"/>
       <c r="D167" s="6"/>
@@ -4428,15 +4437,15 @@
       <c r="F167" s="20"/>
       <c r="G167" s="5"/>
       <c r="H167" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C168" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>29</v>
@@ -4445,10 +4454,10 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B169" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="B169" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="C169" s="5"/>
       <c r="D169" s="6"/>
@@ -4456,15 +4465,15 @@
       <c r="F169" s="20"/>
       <c r="G169" s="5"/>
       <c r="H169" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C170" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E170" s="8" t="b">
         <v>1</v>
@@ -4473,38 +4482,38 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C171" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D171" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D171" s="2" t="s">
+      <c r="E171" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F171" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G171" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="E171" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F171" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G171" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="172" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B172" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="B172" s="5" t="s">
-        <v>225</v>
-      </c>
       <c r="H172" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="173" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C173" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E173" s="8" t="s">
         <v>29</v>
@@ -4514,27 +4523,27 @@
     </row>
     <row r="174" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C174" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E174" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F174" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B175" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="B175" s="6" t="s">
-        <v>229</v>
       </c>
       <c r="C175" s="5"/>
       <c r="D175" s="6"/>
@@ -4542,15 +4551,15 @@
       <c r="F175" s="20"/>
       <c r="G175" s="5"/>
       <c r="H175" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="176" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C176" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E176" s="8" t="b">
         <v>1</v>
@@ -4559,27 +4568,27 @@
     </row>
     <row r="177" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C177" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E177" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F177" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B178" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="B178" s="6" t="s">
-        <v>233</v>
       </c>
       <c r="C178" s="5"/>
       <c r="D178" s="6"/>
@@ -4587,15 +4596,15 @@
       <c r="F178" s="20"/>
       <c r="G178" s="5"/>
       <c r="H178" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C179" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E179" s="8" t="s">
         <v>29</v>
@@ -4604,27 +4613,27 @@
     </row>
     <row r="180" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C180" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F180" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B181" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="B181" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="C181" s="5"/>
       <c r="D181" s="6"/>
@@ -4632,83 +4641,83 @@
       <c r="F181" s="20"/>
       <c r="G181" s="5"/>
       <c r="H181" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C182" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E182" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F182" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C183" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D183" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D183" s="10" t="s">
-        <v>240</v>
-      </c>
       <c r="E183" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F183" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C184" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D184" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="D184" s="10" t="s">
-        <v>242</v>
-      </c>
       <c r="E184" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F184" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C185" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D185" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="D185" s="10" t="s">
-        <v>244</v>
-      </c>
       <c r="E185" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F185" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B186" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="B186" s="6" t="s">
-        <v>246</v>
       </c>
       <c r="C186" s="5"/>
       <c r="D186" s="6"/>
@@ -4716,15 +4725,15 @@
       <c r="F186" s="20"/>
       <c r="G186" s="5"/>
       <c r="H186" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C187" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E187" s="8" t="b">
         <v>1</v>
@@ -4733,10 +4742,10 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C188" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D188" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="D188" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="E188" s="8" t="b">
         <v>1</v>
@@ -4751,10 +4760,10 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B190" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="C190" s="5"/>
       <c r="D190" s="6"/>
@@ -4762,15 +4771,15 @@
       <c r="F190" s="20"/>
       <c r="G190" s="5"/>
       <c r="H190" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C191" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E191" s="8" t="b">
         <v>1</v>
@@ -4779,27 +4788,27 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C192" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D192" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D192" s="2" t="s">
+      <c r="E192" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F192" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G192" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="E192" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F192" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G192" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B193" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="B193" s="6" t="s">
-        <v>257</v>
       </c>
       <c r="C193" s="5"/>
       <c r="D193" s="6"/>
@@ -4807,15 +4816,15 @@
       <c r="F193" s="20"/>
       <c r="G193" s="5"/>
       <c r="H193" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C194" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>29</v>
@@ -4824,27 +4833,27 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C195" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F195" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B196" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="B196" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="C196" s="5"/>
       <c r="D196" s="6"/>
@@ -4852,15 +4861,15 @@
       <c r="F196" s="20"/>
       <c r="G196" s="5"/>
       <c r="H196" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="197" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C197" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>29</v>
@@ -4869,38 +4878,38 @@
     </row>
     <row r="198" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C198" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F198" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B199" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B199" s="6" t="s">
-        <v>265</v>
-      </c>
       <c r="H199" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="200" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C200" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>29</v>
@@ -4910,27 +4919,27 @@
     </row>
     <row r="201" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C201" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F201" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="202" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B202" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="B202" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="C202" s="5"/>
       <c r="D202" s="6"/>
@@ -4938,15 +4947,15 @@
       <c r="F202" s="20"/>
       <c r="G202" s="5"/>
       <c r="H202" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C203" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>29</v>
@@ -4955,10 +4964,10 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C204" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D204" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D204" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E204" s="8" t="s">
         <v>29</v>
@@ -4967,10 +4976,10 @@
     </row>
     <row r="205" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B205" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="B205" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="C205" s="5"/>
       <c r="D205" s="6"/>
@@ -4978,43 +4987,43 @@
       <c r="F205" s="20"/>
       <c r="G205" s="5"/>
       <c r="H205" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C206" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E206" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F206" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C207" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D207" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D207" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E207" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F207" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="208" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B208" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="B208" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="C208" s="5"/>
       <c r="D208" s="6"/>
@@ -5022,15 +5031,15 @@
       <c r="F208" s="20"/>
       <c r="G208" s="5"/>
       <c r="H208" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C209" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E209" s="8" t="s">
         <v>29</v>
@@ -5039,10 +5048,10 @@
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C210" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D210" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D210" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E210" s="8" t="s">
         <v>29</v>
@@ -5051,10 +5060,10 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B211" s="6" t="s">
         <v>276</v>
-      </c>
-      <c r="B211" s="6" t="s">
-        <v>277</v>
       </c>
       <c r="C211" s="5"/>
       <c r="D211" s="6"/>
@@ -5062,15 +5071,15 @@
       <c r="F211" s="20"/>
       <c r="G211" s="5"/>
       <c r="H211" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C212" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E212" s="8" t="b">
         <v>1</v>
@@ -5079,10 +5088,10 @@
     </row>
     <row r="213" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C213" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D213" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="D213" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="E213" s="8" t="b">
         <v>1</v>
@@ -5091,10 +5100,10 @@
     </row>
     <row r="214" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B214" s="6" t="s">
         <v>280</v>
-      </c>
-      <c r="B214" s="6" t="s">
-        <v>281</v>
       </c>
       <c r="C214" s="5"/>
       <c r="D214" s="13"/>
@@ -5102,15 +5111,15 @@
       <c r="F214" s="20"/>
       <c r="G214" s="14"/>
       <c r="H214" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C215" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E215" s="8" t="s">
         <v>29</v>
@@ -5119,10 +5128,10 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C216" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D216" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E216" s="8" t="s">
         <v>29</v>
@@ -5131,10 +5140,10 @@
     </row>
     <row r="217" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B217" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="B217" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="C217" s="6"/>
       <c r="D217" s="6"/>
@@ -5145,52 +5154,52 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C218" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E218" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H218" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C219" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E219" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H219" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C220" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E220" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H220" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="221" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B221" s="6" t="s">
         <v>294</v>
-      </c>
-      <c r="B221" s="6" t="s">
-        <v>295</v>
       </c>
       <c r="C221" s="6"/>
       <c r="D221" s="6"/>
@@ -5201,10 +5210,10 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C222" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>29</v>
@@ -5212,10 +5221,10 @@
     </row>
     <row r="223" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C223" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E223" s="1" t="s">
         <v>29</v>
@@ -5223,10 +5232,10 @@
     </row>
     <row r="224" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C224" s="6"/>
       <c r="D224" s="6"/>
@@ -5237,10 +5246,10 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C225" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E225" s="1" t="s">
         <v>29</v>
@@ -5248,10 +5257,10 @@
     </row>
     <row r="226" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C226" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E226" s="1" t="s">
         <v>29</v>
@@ -5259,10 +5268,10 @@
     </row>
     <row r="227" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C227" s="6"/>
       <c r="D227" s="6"/>
@@ -5273,10 +5282,10 @@
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C228" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E228" s="1" t="s">
         <v>29</v>
@@ -5284,10 +5293,10 @@
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C229" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E229" s="1" t="s">
         <v>29</v>
@@ -5405,25 +5414,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81:E82">
-    <cfRule type="cellIs" dxfId="29" priority="42" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="29" priority="40" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="28" priority="41" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="40" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="27" priority="42" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84:E89">
-    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="26" priority="39" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="25" priority="38" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="39" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="24" priority="37" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91:E95">
@@ -5460,25 +5469,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E112:E115">
-    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
       <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
-      <formula>"UNKNOWN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E117:E121">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"UNKNOWN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
-      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E123:E126 E128:E131">

</xml_diff>

<commit_message>
Inculding descriptions of boiler_fuel and boiler_cap_ratio options.
</commit_message>
<xml_diff>
--- a/resources/BTAPOptions.xlsx
+++ b/resources/BTAPOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\projects\btap_batch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D8E60C-4470-4467-884D-D956BC382893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933191F2-1079-4DAD-B33A-F4860282C34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="1140" windowWidth="34560" windowHeight="18552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5436" yWindow="5628" windowWidth="36420" windowHeight="18552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadME" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="339">
   <si>
     <t>Variable</t>
   </si>
@@ -998,13 +998,64 @@
   </si>
   <si>
     <t>Default location for climate zone</t>
+  </si>
+  <si>
+    <t>:boiler_fuel</t>
+  </si>
+  <si>
+    <t>Specify the fuel type of the primary and secondary boilers.</t>
+  </si>
+  <si>
+    <t>NaturalGasElecBackup</t>
+  </si>
+  <si>
+    <t>ElectricityGasBackup</t>
+  </si>
+  <si>
+    <t>Use NECB Default settings and take boiler fuel type from the primary heating fuel option.</t>
+  </si>
+  <si>
+    <t>Will force the creation of natural gas primary and secondary boilers and create baseboard hot-water heaters.  This will happen even if the NCEB default building would not normally inculde a boiler or hot-water baseboards.</t>
+  </si>
+  <si>
+    <t>Will force the creation of a natural gas primary and electric secondary boiler and create baseboard hot-water heaters.  This will happen even if the NCEB default building would not normally inculde a boiler or hot-water baseboards.</t>
+  </si>
+  <si>
+    <t>Will force the creation of electric primary and secondary boilers and create baseboard hot-water heaters.  This will happen even if the NCEB default building would not normally inculde a boiler or hot-water baseboards.</t>
+  </si>
+  <si>
+    <t>Will force the creation of an electric primary and natural gas secondary boiler and create baseboard hot-water heaters.  This will happen even if the NCEB default building would not normally inculde a boiler or hot-water baseboards.</t>
+  </si>
+  <si>
+    <t>Will force the creation of FuelOirNo2 primary and secondary boilers and create baseboard hot-water heaters.  This will happen even if the NCEB default building would not normally inculde a boiler or hot-water baseboards.</t>
+  </si>
+  <si>
+    <t>:boiler_cap_ratio</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>Use the default NECB behaviour.  If the boiler_fuel option was used, and it inculded disimilar primary and secondary boiler fuel types, the primary boiler will be 75% of the required boiler capacity and the secondary boiler will be 25% of the required boiler capacity.</t>
+  </si>
+  <si>
+    <t>Specify the ratio of primary and secondary boiler capacities.  These are based on the total required capacity for the boilers based on the sizing run.  They can sum to be more or less than 100%.</t>
+  </si>
+  <si>
+    <t>Use the default NECB behaviour regarless of boiler fuels.</t>
+  </si>
+  <si>
+    <t>80-20</t>
+  </si>
+  <si>
+    <t>The first number sets the percent of the total required boiler capacity applied to the primary boiler.  The second number does the same for the secondary boiler.  In this case the primary boiler would have a capacity that is 80% of the total required boiler capacity and the secondary bolier's capacity would be 20% of the total required capacity.  Thes numbers can sum to more or less than 100.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1046,8 +1097,15 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1076,6 +1134,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1116,11 +1179,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1205,22 +1269,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="57">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1228,126 +1286,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1368,116 +1306,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1513,11 +1341,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1533,91 +1361,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1643,11 +1391,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1663,11 +1431,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1683,11 +1451,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1703,11 +1491,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1723,11 +1531,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1743,11 +1571,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1763,6 +1591,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1773,11 +1611,241 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2077,11 +2145,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H230"/>
+  <dimension ref="A1:H241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D238" sqref="D238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5303,8 +5371,12 @@
       </c>
     </row>
     <row r="230" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="6"/>
-      <c r="B230" s="6"/>
+      <c r="A230" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>323</v>
+      </c>
       <c r="C230" s="6"/>
       <c r="D230" s="6"/>
       <c r="E230" s="6"/>
@@ -5312,105 +5384,228 @@
       <c r="G230" s="6"/>
       <c r="H230" s="6"/>
     </row>
+    <row r="231" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C231" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D231" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E231" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C232" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D232" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E232" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C233" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E233" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C234" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E234" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C235" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E235" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C236" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E236" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B237" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C237" s="6"/>
+      <c r="D237" s="6"/>
+      <c r="E237" s="6"/>
+      <c r="F237" s="6"/>
+      <c r="G237" s="6"/>
+      <c r="H237" s="6"/>
+    </row>
+    <row r="238" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C238" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E238" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C239" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E239" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C240" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E240" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="6"/>
+      <c r="B241" s="6"/>
+      <c r="C241" s="6"/>
+      <c r="D241" s="6"/>
+      <c r="E241" s="6"/>
+      <c r="F241" s="6"/>
+      <c r="G241" s="6"/>
+      <c r="H241" s="6"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H216" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="E3:E8 E155:E156 E158:E159 E161:E162 E164 E166 E168 E170:E171 E173:E174 E176:E177 E179:E180 E182:E185 E187:E189 E191:E192 E194:E195 E197:E198 E200:E201 E203:E204 E206:E207 E209:E210 E212:E213 E215:E216">
-    <cfRule type="cellIs" dxfId="56" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="67" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="68" operator="equal">
       <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="67" operator="equal">
-      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="54" priority="69" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:E42">
-    <cfRule type="cellIs" dxfId="53" priority="66" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="52" priority="65" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="64" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="51" priority="66" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:E47 E49:E50">
-    <cfRule type="cellIs" dxfId="50" priority="63" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="50" priority="61" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="49" priority="62" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="61" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="48" priority="63" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:E53">
-    <cfRule type="cellIs" dxfId="47" priority="60" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="45" priority="60" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E57">
     <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="57" operator="equal">
       <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="56" operator="equal">
-      <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E64">
-    <cfRule type="cellIs" dxfId="41" priority="54" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="40" priority="53" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="52" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="39" priority="54" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66:E68">
-    <cfRule type="cellIs" dxfId="38" priority="51" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="38" priority="49" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="37" priority="50" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="49" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="36" priority="51" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:E75">
-    <cfRule type="cellIs" dxfId="35" priority="48" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="34" priority="47" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="46" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="33" priority="48" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77:E79">
-    <cfRule type="cellIs" dxfId="32" priority="45" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="32" priority="43" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="31" priority="44" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="43" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="30" priority="45" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81:E82">
@@ -5425,102 +5620,102 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84:E89">
-    <cfRule type="cellIs" dxfId="26" priority="39" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="25" priority="38" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="37" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="24" priority="39" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91:E95">
-    <cfRule type="cellIs" dxfId="23" priority="36" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="22" priority="35" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="34" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97:E104">
-    <cfRule type="cellIs" dxfId="20" priority="30" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106:E110">
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="25" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E112:E115">
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
+      <formula>"UNKNOWN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
       <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
-      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E117:E121">
-    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E123:E126 E128:E131">
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E133:E136 E138:E141 E143:E145 E147:E149 E151:E153">
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
-      <formula>TRUE</formula>
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+      <formula>"UNKNOWN"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
-      <formula>"UNKNOWN"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E218:E220">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"UNKNOWN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>